<commit_message>
Evaluation of Questions & Responses
</commit_message>
<xml_diff>
--- a/evaluation_results.xlsx
+++ b/evaluation_results.xlsx
@@ -463,12 +463,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Based on the research paper, what were the estimated damages to the aquaculture and agriculture sectors due to salt intrusion in the Mekong Delta in 2016?</t>
+          <t>Theo nghiên cứu, đâu là tỉnh chịu ảnh hưởng nặng nề nhất do xâm nhập mặn năm 2016 và mức độ thiệt hại ước tính là bao nhiêu?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>The research paper does not provide specific estimates of the damages to the aquaculture and agriculture sectors due to salt intrusion in the Mekong Delta in 2016. However, it does mention that salinity intrusion severely affected livelihoods and welfare of households in wider areas during that year. The paper also states that higher salinity decreases the productivity and revenue share of rice crop, decreases aquaculture production, and reduces farmer households’ income and consumption.</t>
+          <t>Tỉnh chịu ảnh hưởng nặng nề nhất do xâm nhập mặn năm 2016 là tỉnh Cà Mau, với mức độ thiệt hại ước tính khoảng 16 nghìn tỷ.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,46 +483,46 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and provides a detailed response, even though it does not provide specific estimates. It gives a comprehensive overview of the impact of salt intrusion on the aquaculture and agriculture sectors in the Mekong Delta in 2016, as per the research paper. The only reason it doesn't get a full score is because it doesn't provide the exact figures asked for in the question.</t>
+          <t>The generated answer is relevant and appears to be correct, providing specific information in response to the user's query about the province most affected by salt intrusion in 2016 and the estimated damage.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>According to the paper, how does a salinity level of 3‰ affect rice plants, and what species can be raised in areas with a salinity level of 5 - 10‰ and 10 - 25‰?</t>
+          <t>Các loài nào có thể sống trong môi trường nước có độ mặn từ 5 - 10‰ và từ 10 - 25‰?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on how a salinity level of 3‰ affects rice plants, or what species can be raised in areas with a salinity level of 5 - 10‰ and 10 - 25‰.</t>
+          <t>The context does not provide information on which species can live in water with salinity levels of 5 - 10‰ and 10 - 25‰.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the question about salinity levels and their effects on rice plants and other species. However, it does not provide any specific information or answer the question, hence the score is in the middle range.</t>
+          <t>The generated answer is relevant to the user query, but it does not provide a specific answer to the question. However, without a reference answer, it's hard to judge if the bot could have provided a more specific answer.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Based on the research paper, what were the economic impacts of the 2016 saline intrusion in the Vietnamese Mekong Delta, particularly in the province of Cà Mau?</t>
+          <t>Theo nghiên cứu, xâm nhập mặn đã ảnh hưởng như thế nào đến công tác quản lý nguồn tài nguyên nước trong sản xuất nông nghiệp tại huyện Long Phú, tỉnh Sóc Trăng?</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>The research paper does not provide specific information on the economic impacts of the 2016 saline intrusion in the Vietnamese Mekong Delta, particularly in the province of Cà Mau.</t>
+          <t>Xâm nhập mặn đã gây ra khó khăn trong việc điều tiết nguồn nước, đặc biệt là việc không cung cấp đủ nước ngọt cho canh tác lúa vụ 3 (vụ Xuân - Hè) đầu năm 2016. Khô hạn kéo dài đã làm tăng nhu cầu sử dụng nước cho sản xuất lúa. Tuy nhiên, vấn đề khai thác nước dưới đất được quản lý tốt và không có mâu thuẫn giữa các nông hộ trong việc sử dụng nguồn nước mặt phục vụ cho sản xuất lúa.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -537,22 +537,21 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and seems correct, but without a reference answer or the actual research paper, it's hard to confirm its full accuracy.</t>
+          <t>The generated answer is relevant and provides a detailed explanation of how saltwater intrusion has affected water resource management in agricultural production in Long Phu district, Soc Trang province. It mentions specific impacts such as difficulties in water regulation and increased demand for water due to prolonged drought. However, without a reference answer, it's hard to confirm the full accuracy of the information.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Discuss the challenges faced in water resources management due to saline intrusion in the Vietnamese Mekong Delta as highlighted in the paper. How did these challenges affect rice cultivation in the region?</t>
+          <t>Hãy phân tích và đánh giá ảnh hưởng của xâm nhập mặn năm 2016 đối với kinh tế (nông nghiệp, nuôi trồng thủy sản) ở Việt Nam, cụ thể là tỉnh Cà Mau và một số tỉnh ít ảnh hưởng mặn như Đồng Tháp, Cần Thơ, An Giang.</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Saline intrusion in the Vietnamese Mekong Delta presents several challenges for water resources management. This phenomenon occurs when not enough river discharge is flowing to the low-lying estuaries, causing salt water to flow into the land. The factors affecting saline intrusion include the amplitude and period of tides, local rainfall and runoff, the slope of the river bed, wind velocity and direction, and the depth of the estuary. 
-The intrusion of salt water affects different provinces in varying degrees due to the difference in water volumes at each mouth of the tributaries. This makes it difficult to quantify the damage costs to farmers. During the annual saline intrusion period, from March to May, vegetables and other crops become scarce in the affected areas. Salinity intrusion also restricts the use of canal water for domestic and industrial uses and causes corrosion of metal materials in engines, construction artefacts, and elsewhere.
-The impact of saline intrusion is particularly significant on rice cultivation. The research suggests that salinity shocks have adverse impacts on the production of rice in the Mekong Delta. Evidence of salinization reducing agricultural land, labor supply in agriculture, and farmer households’ income and consumption has been found. 
-To cope with these challenges, farmers have been observed to switch to salt-resistant crop production and diversify their crops to sustain their income and food security against salinization shocks. However, these adjustments within the agricultural sector are not always sufficient, and further research is needed to develop strategies for flood loss prevention and salinity management for the vulnerable agricultural sector.</t>
+          <t>Xâm nhập mặn năm 2016 đã gây ra những ảnh hưởng tiêu cực đáng kể đối với kinh tế, đặc biệt là trong lĩnh vực nông nghiệp và nuôi trồng thủy sản ở Việt Nam. Tổng thiệt hại ước tính đối với kinh tế là khoảng 38.500 tỷ VNĐ và ảnh hưởng đến khoảng 8.111 nghìn người.
+Tỉnh Cà Mau là tỉnh chịu thiệt hại nặng nề nhất do xâm nhập mặn với mức độ thiệt hại khoảng 16 nghìn tỷ. Xâm nhập mặn đã gây ra khó khăn trong việc cung cấp nước ngọt cho canh tác, làm tăng nhu cầu sử dụng nước và gây ra những thách thức cho công tác quản lý nguồn tài nguyên nước.
+Mặt khác, một số tỉnh ít ảnh hưởng mặn như Đồng Tháp, Cần Thơ, An Giang đã không chịu ảnh hưởng nặng nề như Cà Mau. Tuy nhiên, cần lưu ý rằng các số liệu này có thể chưa chính xác do sự thay đổi nhiều về sử dụng đất và giá trị đất so với thực tế.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -567,20 +566,19 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the challenges faced in water resources management due to saline intrusion in the Vietnamese Mekong Delta. It also discusses the impact of these challenges on rice cultivation in the region. The answer is comprehensive and appears to be accurate, although without a reference answer, it's difficult to confirm the absolute correctness of all details.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the impact of saltwater intrusion in 2016 on the economy, specifically agriculture and aquaculture, in Vietnam. It also specifically addresses the impact on Ca Mau province and other less affected provinces like Dong Thap, Can Tho, and An Giang. The only reason it doesn't get a full score is because it mentions that the data might not be accurate due to changes in land use and land value, which introduces a slight uncertainty.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Based on the research conducted in the Sóc Trăng province, how did the salt intrusion affect the farming practices and water resources in the region? Provide specific examples from the text.</t>
+          <t>Theo kết quả thống kê của Phòng Nông nghiệp và Phát triển Nông thôn huyện Long Phú năm 2016, hai xã nào chịu ảnh hưởng nặng nề nhất từ đợt xâm nhập mặn - khô hạn cuối năm 2015 và đầu năm 2016? Hãy nêu diện tích lúa bị thiệt hại của từng xã.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Salt intrusion, particularly under the impact of climate change, has significantly affected farming practices and water resources in the Sóc Trăng province. For instance, it has had a notable impact on rice cultivation areas. The research identified three main rice crops systems - triple rice crop, double rice crop, and rice-shrimp rotation crop - and found that the impact of saline intrusion varied across these systems and districts. In the My Xuyen district, the affected area of rice-shrimp rotation crop increased by 14.7 ha, while in the Tran De and Long Phu districts, the affected areas of double rice crop and triple rice crop decreased by 155.5 ha and 35.5 ha, respectively.
-Furthermore, salinity intrusion, freshwater scarcity, and ebb tide influences were identified as the most significant hazards, and these have been increasing in recent years. To cope with these challenges, the local government and people have developed strategies such as dyke building, farming technical changes, financial support for production recovery from disasters, underground water exploitation, and income diversification. However, these adaptation options have shown some limitations as they did not fully consider the differences in terms of ecological, social, and economic environment. Future adaptation strategies are suggested to take these factors into account.</t>
+          <t>Xin lỗi, nhưng thông tin cung cấp không đề cập đến hai xã cụ thể nào chịu ảnh hưởng nặng nề nhất từ đợt xâm nhập mặn - khô hạn cuối năm 2015 và đầu năm 2016, cũng như diện tích lúa bị thiệt hại của từng xã.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -590,26 +588,24 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides specific examples from the research conducted in the Sóc Trăng province. It explains how salt intrusion has affected farming practices and water resources in the region, and also mentions the strategies developed to cope with these challenges. The only reason it doesn't get a full score is because it doesn't provide specific examples of how the water resources were affected, which was part of the user's query.</t>
+          <t>The generated answer is relevant to the user query and it is correct in the sense that it admits the lack of specific information asked for. However, it does not provide any additional information or attempt to provide a solution, hence it is not a perfect response.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>According to the survey results mentioned in the text, how did the farmers in the researched area manage their water resources and farming schedules? Discuss the benefits and challenges they faced.</t>
+          <t>Theo kết quả phỏng vấn, phần trăm hộ dân nào có thống nhất thời gian lấy nước canh tác với các nông hộ lân cận? Hãy giải thích tác động của việc lấy nước không đồng loạt đối với việc canh tác.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Farmers in the researched area, the Mekong Delta, have had to adapt their farming practices due to water-related challenges such as salinity intrusion, floods, acid sulfate soils, polluted water, and fresh water shortages. One of the strategies they have adopted is shifting to salt-resistant industrial crops, which helps them maintain their income and food security against salinization shocks. This is seen as a within-agricultural adjustment in response to salinity shock.
-However, the farmers face several challenges. The water control infrastructure systems, which are funded by about 10 percent of the state budget and labor contributed by the people, suffer from many shortcomings in terms of both their structure and management. Furthermore, the water resources planning process is largely "top-down", with villagers and farmers playing a very minor role. This means that many grass-roots people have little voice in the planning and natural prevention projection processes.
-Despite these challenges, floods are not only seen as a disaster by many farmers and scientists. They recognize that floods bring multiple benefits, including fertile sediment, fish spawning, aquatic products, pest control, improved water quality, water provision, reduced fire risk, and ecological drivers. These benefits are seen as replenishing and revitalizing for the agricultural land. However, high floods can result in loss of life and cause millions of dollars worth of damage to houses, infrastructure, and crops. The costs of these damages have been increasing due to higher economic development and an increasing population.</t>
+          <t>Theo kết quả phỏng vấn, 47% số hộ dân có thống nhất thời gian lấy nước canh tác với các nông hộ lân cận. Việc lấy nước không đồng loạt có thể gây ra khó khăn. Cụ thể, những hộ lấy nước trước có thể lấy đủ thậm chí là nhiều hơn so với nhu cầu thực của cây lúa, trong khi những hộ lấy nước sau có thể thiếu nước ngọt. Hơn nữa, trong thời gian diễn ra xâm nhập mặn, việc đóng và mở cống không thường xuyên và không đủ nước ngọt phục vụ cho canh tác của vùng.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -624,46 +620,46 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how farmers in the researched area manage their water resources and farming schedules. It also discusses the benefits and challenges they face. The answer is comprehensive and accurate, but it could be slightly more concise.</t>
+          <t>The generated answer is relevant to the user query and provides a detailed explanation of the impact of not synchronizing water collection for farming. However, without a reference answer, it's hard to verify the accuracy of the specific percentage mentioned (47%).</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Based on the research paper, what challenges were identified in the management of Water Resources at the beginning of 2016?</t>
+          <t>Theo nghiên cứu, hãy mô tả những khó khăn và trở ngại mà công tác quản lý nguồn Tài Nguyên Nước đã gặp phải vào đầu năm 2016? Hãy đưa ra ít nhất ba điểm.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>The context does not provide specific information about the challenges identified in the management of Water Resources at the beginning of 2016.</t>
+          <t>Công tác quản lý nguồn Tài Nguyên Nước đã gặp phải một số khó khăn và trở ngại. Đầu tiên, mức độ tham gia của người dân trong việc khai thác nguồn tài nguyên nước chưa cao. Mặc dù 90% số hộ dân được phỏng vấn biết quy định thực hiện đăng ký trong khai thác nguồn tài nguyên nước, nhưng mức độ tham gia của họ vẫn còn hạn chế. Thứ hai, việc đăng ký và kiểm soát khai thác nguồn tài nguyên nước vẫn còn một số hạn chế. Cuối cùng, công tác nạo vét, bảo dưỡng công trình cần được quan tâm, nhất là vào mùa khô.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and does not contain any factual errors. However, it does not provide a specific answer to the question, which may be due to the lack of information provided in the user query.</t>
+          <t>The generated answer is relevant and correct. It provides three points of difficulties and obstacles that water resource management faced in early 2016. However, it could be more specific about the context of 2016.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>According to the paper, why is it important to enhance the interaction and exchange between management staff and the local people in the context of water resource management?</t>
+          <t>Theo nội dung của bài nghiên cứu, hãy giải thích tầm quan trọng của việc thống nhất lịch canh tác giữa các hộ nông dân và những lợi ích mà việc này mang lại.</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>The paper emphasizes the importance of enhancing interaction and exchange between management staff and local people in water resource management because current adaptation strategies to hazards like salinity intrusion, freshwater scarcity, and ebb tide influences have limitations. These strategies often do not fully consider the differences in ecological, social, and economic environments, which are crucial factors as the vulnerability of people highly depends on these conditions. Therefore, to develop more effective and beneficial strategies, especially for the most vulnerable groups, it is important to understand and incorporate the needs and capacities of the local communities. This can be achieved through better interaction and exchange between management staff and local people.</t>
+          <t>Việc thống nhất lịch canh tác giữa các hộ nông dân rất quan trọng. Khoảng 73% số hộ dân đã thống nhất lịch canh tác với các nông hộ lân cận. Điều này phần lớn phụ thuộc vào thời gian máy cày đến ruộng và nguồn nước ngọt. Việc xuống giống đồng loạt giúp cho việc mua bán sau khi thu hoạch dễ dàng hơn. Điều này cho thấy việc thống nhất về lịch thời vụ được thực hiện khá tốt tại vùng nghiên cứu.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -678,24 +674,20 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of why it's important to enhance the interaction and exchange between management staff and local people in the context of water resource management. It correctly identifies the limitations of current strategies and the need to understand local conditions and needs for more effective strategies.</t>
+          <t>The generated answer is relevant and mostly correct. It explains the importance of synchronizing the farming schedule among farmers and the benefits it brings, such as easier post-harvest trading. However, it could have provided more detailed benefits to fully answer the user's query.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>According to the research paper, what were the main hazards identified that have been increasing in recent years in the Mekong Delta region? Discuss the strategies and measures developed by the governments and local people to cope with these hazards.</t>
+          <t>Theo nghiên cứu, những hiểm họa nào được xác định là quan trọng nhất ở đồng bằng sông Cửu Long và chúng đã thay đổi như thế nào trong những năm gần đây?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>The main hazards identified in the Mekong Delta region that have been increasing in recent years include major flooding, salinity intrusion, and water quality problems. These issues are exacerbated by factors such as climate change, dam construction, and anthropogenic activities. 
-Major flooding is now likely to occur more frequently than the previous average of "once in two or three years". This is due to large water discharges from upstream, long and heavy rainfall in the Mekong Delta itself, and high tides that lead to high water levels in the rivers and canal system, preventing easy drainage. 
-Salinity intrusion occurs when not enough river discharge is flowing to the low-lying estuaries, and instead, salt water flows into the land. This is influenced by factors such as the amplitude and period of tides, the amount of local rainfall and runoff, the slope of the river bed, wind velocity and direction, and the depth of the estuary. 
-Water quality problems are also a significant issue, with many wells experiencing quality problems such as high pH, high iron content, salinity, and odours. 
-To cope with these hazards, computer modelling is widely used as a powerful tool in water resources engineering. This allows for the estimation of extreme floods or severe saline intrusion in the Mekong Delta under various scenarios, assisting with decision-making in water planning and management. The results from these models can be used as a technical prerequisite for the development of a regional strategy and action plan to prepare for flood loss prevention and salinity management for the vulnerable agricultural sector. 
-Furthermore, some farmers have adapted their activities to correspond with salinity intrusion, implementing a more varied production scheme to raise shrimp during the dry season. This adaptation takes advantage of the positive effect of salinity intrusion in reducing acidity in potential acid sulphate soil land.</t>
+          <t>Những hiểm họa quan trọng nhất ở đồng bằng sông Cửu Long bao gồm hiện tượng nóng lên toàn cầu, sự tan băng và nước biển dâng, cùng với những tác động từ hoạt động công nghiệp và nông nghiệp trong khu vực. Những hiện tượng này có thể dẫn đến việc ít nhất 25% diện tích các vùng đất thấp ven biển có nguy cơ bị chìm ngập, 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn vào mùa khô và khoảng 30-40% diện tích nông nghiệp bị ảnh hưởng của nước mặn ngay cả trong mùa mưa. 
+Trong những năm gần đây, tần suất và cường độ các hiện tượng thời tiết cực đoan đã tăng lên, làm gia tăng mối đe dọa an ninh lương thực và tạo ra những biến động tiêu cực cho khu vực nông thôn. Đồng thời, dự báo cho thấy trong thập kỷ 2030-2040, nhiệt độ trung bình cũng như nhiệt độ lớn nhất và nhỏ nhất trong vùng đều sẽ gia tăng, phổ biến tăng khoảng 20˚C. Tổng lượng mưa trung bình trong vùng cũng sẽ sụt giảm, phổ biến từ 10 đến 20%, khiến việc cung cấp nước ngọt cho canh tác lúa thêm khó khăn.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -710,19 +702,21 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the main hazards identified in the Mekong Delta region, as well as the strategies and measures developed to cope with these hazards. It does not contain any noticeable mistakes. The only reason it does not receive a perfect score is because it could have included more specific examples of government initiatives or policies.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate response. It identifies the main hazards in the Mekong Delta, including global warming, melting ice and rising sea levels, and the impacts of industrial and agricultural activities. It also explains how these hazards have changed in recent years, with an increase in extreme weather events and predictions for future temperature and rainfall changes.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>The paper mentions some limitations of the current adaptation strategies. What are these limitations and how does the paper suggest future adaptation strategies should be improved to benefit different social groups, especially the most vulnerable?</t>
+          <t>Hãy mô tả những biện pháp thích ứng mà chính quyền và người dân địa phương đã và đang phát triển để đối phó với các hiểm họa này. Theo nghiên cứu, những biện pháp này còn bất cập gì và những chiến lược thích ứng trong tương lai cần xây dựng như thế nào?</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>The current adaptation strategies to hazards such as salinity intrusion and freshwater scarcity have some limitations. They do not fully consider the differences in terms of ecological, social, and economic environment. However, the vulnerability of people highly depends on these conditions. To improve future adaptation strategies, the paper suggests that these strategies should take into account the ecological, social, and economic environment. This would ensure that the strategies benefit different social groups, especially the most vulnerable. One suitable method for building future adaptation programs is the Participatory Vulnerability Assessment (PVA) approach. This approach helps identify vulnerable groups that need assistance and assess their capacity, thereby developing appropriate adaptation strategies. Furthermore, this approach enhances people's awareness of natural disasters and disaster mitigation, especially in the context of global climate change.</t>
+          <t>Các biện pháp thích ứng mà chính quyền và người dân địa phương đã và đang phát triển để đối phó với các hiểm họa này chưa được triển khai một cách hiệu quả. Cụ thể, việc hiểu và triển khai Nghị quyết 120 sau gần 2 năm ban hành vẫn còn lúng túng. Nhiều địa phương chưa thực sự đổi mới theo tinh thần Nghị quyết, còn trông chờ vào hướng dẫn và nguồn lực hỗ trợ từ Trung ương. Việc hoàn thiện thể chế, chính sách triển khai thực hiện các nhiệm vụ theo Nghị quyết 120 vẫn còn chậm. 
+Một trong những bất cập lớn là việc thiếu quy định về cơ chế phối hợp, chia sẻ thông tin giữa các cơ quan liên quan. Đặc biệt, tư duy ưu tiên lựa chọn giải pháp công trình ở các cấp/ngành vẫn nhiều hơn là các chọn lựa giải pháp phi công trình.
+Đối với chiến lược thích ứng trong tương lai, một trong những phương pháp phù hợp là cách tiếp cận đánh giá tổn thương có sự tham gia của cộng đồng (PVA). PVA giúp nhận ra những nhóm dễ bị tổn thương cần giúp đỡ và đánh giá được năng lực của họ để từ đó phát triển các chiến lược thích ứng phù hợp. Thông qua cách tiếp cận này sẽ nâng cao được nhận thức của người dân về thiên tai và công tác phòng chống giảm nhẹ thiên tai, nhất là trong bối cảnh biến đổi khí hậu toàn cầu như hiện nay.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -737,24 +731,27 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the limitations of current adaptation strategies and how future strategies could be improved. It also specifically addresses the need to benefit different social groups, especially the most vulnerable. However, it could have been more specific about the types of social groups that are most vulnerable.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed response. It discusses the current measures, their shortcomings, and future strategies for adaptation. However, it could have been more specific about the hazards being referred to in the user query.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Based on the research paper, what are the factors that have a positive relationship with the livelihood output of coastal households in the Mekong Delta?</t>
+          <t>Theo nghiên cứu, những yếu tố nào có ảnh hưởng đến kết quả sinh kế của nông hộ ven biển đồng bằng sông Cửu Long? Hãy phân tích và giải thích ảnh hưởng của từng yếu tố.</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>The research paper does not provide specific information on the factors that have a positive relationship with the livelihood output of coastal households in the Mekong Delta.</t>
+          <t>Có nhiều yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn, bao gồm số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, hỗ trợ của địa phương, và việc vay vốn. 
+Số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, và hỗ trợ của địa phương đều có mối quan hệ cùng chiều với thu nhập của hộ gia đình, tức là khi các yếu tố này tăng lên, thu nhập của hộ gia đình cũng tăng theo. 
+Tuy nhiên, việc vay vốn lại có mối quan hệ trái chiều với thu nhập của hộ gia đình. Điều này có thể được giải thích là do việc vay vốn thường đi kèm với lãi suất, và nếu không quản lý tốt, nó có thể dẫn đến tình trạng nợ nên thu nhập thực tế của hộ gia đình giảm đi.
+Ngoài ra, hiện tượng nóng lên toàn cầu và sự tăng lên của mực nước biển cũng ảnh hưởng đến sinh kế của cư dân vùng hạn mặn. Sự tăng lên của mực nước biển có thể dẫn đến xâm nhập mặn, làm giảm năng suất nông nghiệp và ảnh hưởng đến nguồn thu nhập của hộ gia đình.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -764,19 +761,20 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query but it does not provide any information about the factors that have a positive relationship with the livelihood output of coastal households in the Mekong Delta. It's unclear whether this is due to the research paper not containing this information or the chatbot's inability to extract it.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the factors affecting the livelihoods of households in the Mekong Delta coastal region. It correctly identifies and explains the impact of various factors such as production means, production experience, labor force, income sources, local support, and borrowing. It also correctly identifies the impact of global warming and sea level rise. However, it does not specifically address the context of the Mekong Delta coastal region, which is why it does not receive a perfect score.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>According to the paper, how does climate change and rising sea levels affect the current farming systems and the lives of people, especially in coastal areas of the Mekong Delta?</t>
+          <t>Trình bày về tác động của biến đổi khí hậu và mực nước biển dâng đối với hệ thống canh tác và đời sống người dân ở vùng ven biển đồng bằng sông Cửu Long.</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>The paper does not provide specific information on how climate change and rising sea levels affect the current farming systems and the lives of people in the coastal areas of the Mekong Delta.</t>
+          <t>Biến đổi khí hậu và mực nước biển dâng có tác động nghiêm trọng đến hệ thống canh tác và đời sống người dân ở vùng ven biển đồng bằng sông Cửu Long. Hiện tượng nóng lên toàn cầu gây ra sự tan băng và nước biển dâng, khiến nhiều vùng đất thấp có nguy cơ bị ngập chìm và xâm nhập mặn. Điều này có thể dẫn đến việc ít nhất 25% diện tích các vùng đất thấp ven biển có nguy cơ bị chìm ngập, khoảng 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn vào mùa khô và khoảng 30-40% diện tích nông nghiệp bị ảnh hưởng của nước mặn ngay cả trong mùa mưa, khó có thể trồng lúa và một số canh tác khác như chăn nuôi.
+Ngoài ra, vùng đồng bằng còn chịu tác động từ những hoạt động phát triển công nghiệp và nông nghiệp trong khu vực. Nước biển từ các cửa sông sẽ chảy theo sông và kênh vào phía trong nội đồng, làm cho đất bị ngập úng và nhiễm mặn. Các huyện ven biển như thành phố Bạc Liêu, huyện Đông Hải, huyện Hòa Bình do kinh tế chủ yếu là nuôi thủy sản nên việc lấy nguồn nước biển thường xuyên phải mở thêm nhiều kênh rạch, làm cho nước biển đi vào sâu phía trong được thuận lợi. Các vùng phía trong quốc lộ 1A như huyện Giá Rai, huyện Phước Long mấy năm gần đây do người dân tự ý chuyển đổi từ trồng lúa qua nuôi tôm phá vỡ việc vận hành của hệ thống cống ngăn mặn, làm cho nước biển vào sâu trong nội đồng nguy cơ ngập ngày càng thể hiện rõ diện tích ngập tăng lên.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -791,19 +789,21 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the topic of climate change and its effects on farming systems and people's lives in the Mekong Delta. However, it does not provide any specific information or details, which makes it difficult to determine its correctness.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of climate change and rising sea levels on the agricultural system and the lives of people in the coastal areas of the Mekong Delta. It also includes specific examples and statistics to support the points made. However, it could be improved by providing more specific solutions or strategies to mitigate these impacts.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Based on the research paper, what are the various livelihood strategies employed by the coastal communities, and how do these strategies change during periods of saline intrusion and non-saline periods?</t>
+          <t>Hãy mô tả chiến lược sinh kế của người dân vùng ven biển và những khó khăn mà họ đang đối mặt với nguồn vốn sinh kế của mình.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>The coastal communities employ various strategies to cope with and adapt to hazards such as salinity intrusion. These strategies include the construction of dykes, changes in farming techniques, financial support for production recovery from disasters, exploitation of underground water, and diversification of income sources. However, these strategies have shown some limitations as they do not fully consider the differences in ecological, social, and economic environments. The vulnerability of people highly depends on these conditions. Therefore, future adaptation strategies should take these issues into account to benefit different social groups, especially the most vulnerable.</t>
+          <t>Người dân vùng ven biển có nhiều chiến lược sinh kế khác nhau, bao gồm trồng lúa, nuôi tôm, chăn nuôi, và làm thuê trong lĩnh vực nông nghiệp và phi nông nghiệp, đáp ứng cho cả thời gian xâm nhập mặn và thời gian không mặn. Tuy nhiên, họ đang đối mặt với một số khó khăn liên quan đến nguồn vốn sinh kế của mình. 
+Vốn con người có lực lượng lao động dồi dào nhưng tỷ lệ lao động phụ thuộc cao và trình độ học vấn thấp, đặc biệt trong độ tuổi lao động. Nguồn vốn xã hội còn hạn chế với tỷ lệ tham gia vào các tổ chức thấp. Nguồn vốn tự nhiên, bao gồm đất đai, khá cao nhưng nguồn vốn vật chất thì thiếu hụt, đặc biệt đối với những hộ nghèo. Nguồn vốn tài chính cũng chưa cao, với thu nhập chủ yếu trong thời gian xâm nhập mặn. 
+Kinh nghiệm và vay vốn có ảnh hưởng tiêu cực đến kết quả sinh kế nông hộ, trong khi đó, các yếu tố khác như diện tích đất, đầu tư sản xuất và tổng giá trị phương tiện phục vụ sản xuất và sinh hoạt có ảnh hưởng tích cực. Để cải thiện tình hình, vốn vật chất và tài chính cần được đầu tư và hỗ trợ thêm.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -818,19 +818,19 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query, providing a detailed explanation of the various strategies employed by coastal communities during periods of saline intrusion. However, it does not explicitly mention how these strategies change during non-saline periods, which was part of the user's question.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed description of the livelihood strategies of coastal residents and the challenges they face with their livelihood capital. It covers various aspects such as human capital, social capital, natural capital, and financial capital. The answer also suggests some solutions to improve the situation. However, it could be more specific about the challenges related to each type of capital.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>According to the research, how does saline intrusion due to climate change impact rice cultivation in Soc Trang? Compare the impact under two climate change scenarios in 2004 and 2030, specifically focusing on the changes in the affected areas of rice-shrimp rotation crop, double rice crop, and triple rice crop.</t>
+          <t>Trình bày về tác động của xâm nhập mặn do biến đổi khí hậu đối với hiện trạng canh tác lúa tại tỉnh Sóc Trăng theo hai kịch bản biến đổi khí hậu năm 2004 và 2030.</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>The research indicates that saline intrusion due to climate change significantly impacts rice cultivation in Soc Trang. Under two climate change scenarios in 2004 and 2030, the impact of saline intrusion is primarily distributed to three districts: My Xuyen, Long Phu, and Tran De. The affected area of rice-shrimp rotation crop in My Xuyen increased by 14.7 hectares between the two scenarios. Conversely, the affected areas of double rice crop in Tran De and those of triple rice crop in Long Phu decreased by 155.5 hectares and 35.5 hectares, respectively.</t>
+          <t>Tác động của xâm nhập mặn do biến đổi khí hậu đã gây ra những thay đổi đáng kể đối với hiện trạng canh tác lúa tại tỉnh Sóc Trăng. Theo hai kịch bản biến đổi khí hậu năm 2004 và 2030, có ba hệ thống canh tác lúa chính bao gồm canh tác lúa ba vụ (99,182.2 ha, chiếm 30.3% tổng diện tích), canh tác lúa hai vụ (69,484.2 ha, chiếm 21.2% tổng diện tích) và canh tác lúa-tôm luân phiên (69,484.2 ha, chiếm 4.3% tổng diện tích). Tác động của xâm nhập mặn chủ yếu tập trung vào ba huyện là Mỹ Xuyên, Long Phú và Trần Đề. Khi so sánh kịch bản biến đổi khí hậu năm 2004 và năm 2030, diện tích bị ảnh hưởng của canh tác lúa-tôm luân phiên tại Mỹ Xuyên tăng thêm 14.7 ha; trong khi đó, diện tích bị ảnh hưởng của canh tác lúa hai vụ tại Trần Đề và canh tác lúa ba vụ tại Long Phú giảm lần lượt 155.5 ha và 35.5 ha.</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -845,24 +845,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides specific details about the impact of saline intrusion on different types of rice crops in Soc Trang under two climate change scenarios. However, it does not provide a comparative analysis between the two scenarios, which was asked in the query.</t>
+          <t>The generated answer is highly relevant to the user query and provides detailed information about the impact of saltwater intrusion due to climate change on rice cultivation in Soc Trang province according to two climate change scenarios in 2004 and 2030. It also provides specific data on the affected areas and the changes in different rice cultivation systems. However, without a reference answer, it's hard to confirm the accuracy of the data provided.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Based on the research findings, how has the agricultural structure in Sóc Trăng and other BĐSCL provinces changed before and after 2005? What factors contributed to this change?</t>
+          <t>Trước năm 2005, nông dân ở tỉnh Sóc Trăng và các tỉnh BĐSCL đã thực hiện biện pháp nào để đáp ứng nhu cầu lương thực và quy hoạch của địa phương?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on how the agricultural structure in Sóc Trăng and other BĐSCL provinces has changed before and after 2005, nor does it mention the factors that contributed to this change.</t>
+          <t>The context does not provide information on the measures taken by farmers in Soc Trang province and other Mekong Delta provinces before 2005 to meet local food needs and planning.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -872,19 +872,19 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant information or answer to the user's query.</t>
+          <t>The generated answer is relevant to the user query as it addresses the topic of measures taken by farmers in Soc Trang province and other Mekong Delta provinces. However, it does not provide any specific information or details, which makes it incomplete and not fully correct.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>According to the Bộ Khoa học và Công nghê (2016), what is the standard salinity level in drinking water and how does it affect the growth of regular rice varieties? Can you name any rice varieties that are resistant to salinity?</t>
+          <t>Theo kết quả nghiên cứu, hãy mô tả sự thay đổi diện tích canh tác lúa và diện tích các kiểu sử dụng thuộc vùng sinh thái mặn, lợ từ năm 2004 đến năm 2030 và 2050 dưới tác động của biến đổi khí hậu.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>The context does not provide information on the standard salinity level in drinking water according to the Bộ Khoa học và Công nghê (2016), how it affects the growth of regular rice varieties, or any rice varieties that are resistant to salinity.</t>
+          <t>Rất tiếc, nhưng thông tin được cung cấp không đề cập đến sự thay đổi diện tích canh tác lúa và diện tích các kiểu sử dụng thuộc vùng sinh thái mặn, lợ từ năm 2004 đến năm 2030 và 2050 dưới tác động của biến đổi khí hậu.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -899,19 +899,19 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information relevant to the user's query. It simply states that the information is not available, which does not answer the user's question.</t>
+          <t>The generated answer is relevant to the user query as it addresses the topic of changes in rice cultivation area and usage of different types of saline and brackish ecological zones under the impact of climate change. However, it does not provide any specific information or details about these changes, stating that the provided information does not mention these changes. Therefore, it is not fully correct or helpful in answering the user's question.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Based on the research conducted using MODIS remote sensing images, which three main rice cultivation statuses were identified in Sóc Trăng province? What were the reliability measures for this research?</t>
+          <t>Hãy mô tả cách nghiên cứu sử dụng ảnh viễn thám MODIS để xây dựng bản đồ hiện trạng canh tác lúa tỉnh Sóc Trăng và nêu rõ 3 hiện trạng canh tác lúa chính được xác định trong nghiên cứu.</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>The research identified three main rice cultivation statuses in Sóc Trăng province: triple rice crop, double rice crop, and rice-shrimp rotation crop. The reliability measures for this research were a confidence level of 80.8% and a Kappa value of 0.78.</t>
+          <t>Nghiên cứu đã sử dụng ảnh viễn thám MODIS để xây dựng bản đồ hiện trạng canh tác lúa tỉnh Sóc Trăng với độ tin cậy cao. Trong quá trình nghiên cứu, ba hiện trạng canh tác lúa chính đã được xác định, bao gồm lúa 3 vụ, lúa 2 vụ và lúa tôm luân canh.</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -926,19 +926,19 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and seems to be correct, providing specific details about the rice cultivation statuses identified in Sóc Trăng province and the reliability measures for the research. However, without a reference answer, it's not possible to confirm the absolute accuracy of these details.</t>
+          <t>The generated answer is relevant to the user query and provides a correct response. It describes the use of MODIS remote sensing images in the research to map the current state of rice cultivation in Soc Trang province and identifies the three main rice cultivation states determined in the study. However, it does not provide a detailed description of the research process, which is why it does not receive a full score of 5.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>According to the paper by Dũng and Thuận (2021), what factors were found to have a positive correlation with the livelihood outcome of residents in the salty drought area? What factor had a negative correlation?</t>
+          <t>Trong nghiên cứu của Dũng và Thuận (2021), họ đã chỉ ra những yếu tố nào ảnh hưởng đến thu nhập của cư dân vùng hạn mặn? Hãy phân tích mối quan hệ giữa các yếu tố này và thu nhập.</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>The factors found to have a positive correlation with the livelihood outcome of residents in the salty drought area include the number of production means, production experience, the number of main laborers, the number of income sources, and local support. On the other hand, borrowing was the factor that had a negative correlation with the livelihood outcome.</t>
+          <t>Các yếu tố ảnh hưởng đến thu nhập của cư dân vùng hạn mặn bao gồm số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, hỗ trợ của địa phương, và việc vay vốn. Đa số các yếu tố này có mối quan hệ cùng chiều với thu nhập của hộ gia đình, tức là khi các yếu tố này tăng lên, thu nhập của hộ gia đình cũng tăng theo. Tuy nhiên, yếu tố vay vốn lại có mối quan hệ trái chiều, tức là khi số tiền vay vốn tăng lên, thu nhập của hộ gia đình lại giảm đi.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -948,30 +948,24 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and appears to be fully correct, providing specific factors that have a positive correlation and the one factor that has a negative correlation with the livelihood outcome of residents in the salty drought area, as per the paper by Dũng and Thuận (2021).</t>
+          <t>The generated answer is relevant and seems to be correct, providing a detailed analysis of the factors affecting the income of residents in salt-affected areas and their relationship with income. However, without a reference answer, it's hard to confirm the absolute correctness of the information.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Based on the text, what factors were identified as influencing the livelihood outcomes of residents in salt-affected areas? Please list and briefly explain their relationship with household income.</t>
+          <t>Theo nghiên cứu trong tài liệu, hãy liệt kê các yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn và giải thích mối quan hệ giữa các yếu tố này với thu nhập của hộ gia đình.</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Several factors were identified as influencing the livelihood outcomes of residents in salt-affected areas:
-1. Agricultural Production: Higher salinity decreases the productivity and revenue share of rice crop and aquaculture production, but increases the revenue share of industrial crops, such as coconut, a salt-resistant crop. This suggests that farmers are adopting new crops and switching crops as mechanisms for risk diversification to secure their income against salinization shocks.
-2. Agricultural Land Use: Higher salinity intrusion is associated with decreases in farmers’ land used for rice and in their general land used reported for agriculture. This reduction in land use could potentially impact the income generated from farming activities.
-3. Labor Supply: Salinity shock is estimated to decrease labor supply in agriculture for those without agricultural land, but labor supply for those with agricultural land does not respond to higher salinity. This could affect the income of those who rely on agricultural labor for their livelihood.
-4. Household Income and Consumption: Salinization is found to reduce farmer households’ income and consumption, which directly impacts the livelihood of these households.
-5. Education: The estimated effect on household spending on education is positive, implying farmers’ increased investment to acquire new skills. This could potentially lead to income diversification and improved livelihood outcomes in the long run.
-6. Migration and Credit Access: While the evidence on out-migration for off-farm work in urban centers is mixed, a more developed local credit market is found to play a positive role in easing the income losses incurred by farmers during salinization shocks. This suggests that access to credit and the ability to migrate for work can influence the livelihood outcomes of residents in salt-affected areas.</t>
+          <t>Các yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn bao gồm số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, hỗ trợ của địa phương, và vay vốn. Đa số các yếu tố này có mối quan hệ cùng chiều với thu nhập của hộ gia đình, tức là khi các yếu tố này tăng lên, thu nhập của hộ gia đình cũng tăng theo. Tuy nhiên, yếu tố vay vốn lại có mối quan hệ trái chiều, tức là khi số tiền vay vốn tăng lên, thu nhập của hộ gia đình lại giảm đi.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -986,19 +980,19 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive list of factors influencing the livelihood outcomes of residents in salt-affected areas. It also explains their relationship with household income in a clear and detailed manner. The answer is fully correct and well-structured, making it easy to understand.</t>
+          <t>The generated answer is relevant and appears to be correct, providing a detailed list of factors that influence the livelihood outcomes of residents in salt-affected areas and explaining the relationship between these factors and household income. However, without a reference answer, it's difficult to confirm the absolute correctness of the information.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Discuss the role of local support in the livelihoods of people living in salt-affected areas as mentioned in the text. Can you provide examples of such support?</t>
+          <t>Trình bày về vai trò của sự hỗ trợ từ địa phương đối với sinh kế của người dân ở vùng hạn mặn, kèm theo các ví dụ cụ thể được đề cập trong tài liệu.</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Local support plays a significant role in the livelihoods of people living in salt-affected areas. For instance, in the Mekong Delta, the government and local people have developed various strategies and measures to cope with and adapt to hazards such as salinity intrusion and freshwater scarcity. These include the construction of dykes, changes in farming techniques, financial support for production recovery from disasters, exploitation of underground water, and diversification of income sources. However, it's noted that these adaptation options have some limitations as they do not fully consider the differences in terms of ecological, social, and economic environment. Therefore, future adaptation strategies should take into account these issues to benefit different social groups, especially the most vulnerable.</t>
+          <t>Sự hỗ trợ từ địa phương đóng một vai trò tích cực trong việc cải thiện sinh kế của người dân ở vùng hạn mặn. Trong thực tế, người dân ở các địa phương này đã nhận được nhiều sự hỗ trợ từ chính quyền. Một số hình thức hỗ trợ cụ thể bao gồm việc cung cấp vốn vay với lãi suất ưu đãi, tổ chức các khóa tập huấn về chăn nuôi và nuôi trồng thủy sản, cũng như hỗ trợ giống lúa chịu mặn. Những hỗ trợ này đã góp phần quan trọng vào việc nâng cao năng lực sản xuất và cải thiện sinh kế cho người dân ở vùng hạn mặn.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1013,25 +1007,21 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the role of local support in the livelihoods of people living in salt-affected areas. It also provides specific examples, as requested by the user. The answer is comprehensive and appears to be correct, even in the absence of a reference answer.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the role of local support in improving the livelihoods of people in salt-affected areas. It also provides specific examples of the types of support provided, such as preferential loans, training courses, and salt-resistant rice varieties. However, without a reference answer, it's hard to judge if it's fully correct.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Based on the research paper, what are the various factors that influence the livelihood outcomes of residents in saline intrusion areas? Can you explain the relationship between these factors and the household income?</t>
+          <t>Hãy liệt kê và giải thích các yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn mà nghiên cứu đã chỉ ra. Trong số đó, yếu tố nào có mối quan hệ trái chiều với thu nhập của hộ gia đình?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>The livelihood outcomes of residents in saline intrusion areas, such as the Vietnamese Mekong delta (MKD), are influenced by several factors. 
-Firstly, agricultural production is significantly affected by salinization. Higher salinity decreases the productivity and revenue share of rice crops and aquaculture production. However, it increases the revenue share of industrial crops, such as coconut, which are salt-resistant. This suggests that farmers are adopting new crops and switching crops as a risk diversification strategy to secure their income against salinization shocks.
-Secondly, salinization impacts the agricultural land used. Higher salinity intrusion is associated with decreases in farmers’ land used for rice and their general land used for agriculture.
-Thirdly, salinization affects labor supply. Salinity shock is estimated to decrease labor supply in agriculture for those without agricultural land, but labor supply for those with agricultural land does not respond to higher salinity.
-Fourthly, salinization reduces farmer households’ income and consumption. However, it is found to increase household spending on education, potentially implying farmers’ increased investment to acquire new skills.
-Lastly, the study tests two channels for adaptation smoothing: migration and credit access. The evidence on out-migration for off-farm work in urban centers is mixed, but the results support the hypothesis that a more developed local credit market plays a positive role in easing the income losses incurred by farmers during salinization shocks.
-In summary, salinization affects agricultural production, land use, labor supply, and household income and consumption. However, farmers are adapting to these changes through crop switching, acquiring new skills, and accessing credit.</t>
+          <t>Các yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn bao gồm số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, hỗ trợ của địa phương, và vay vốn. 
+Số phương tiện sản xuất và số lao động chính liên quan đến khả năng sản xuất của hộ gia đình. Kinh nghiệm sản xuất cho phép người dân thích ứng với hạn mặn và rút ra kinh nghiệm từ những thất bại trước đó để sản xuất tốt hơn. Số nguồn thu nhập cũng quan trọng vì nó cung cấp tài chính cho hoạt động sản xuất. Hỗ trợ của địa phương, như vay vốn với lãi suất ưu đãi, tập huấn chăn nuôi, nuôi trồng thủy sản, hỗ trợ giống lúa chịu mặn, cũng đóng góp tích cực vào sinh kế của người dân.
+Trong số các yếu tố trên, chỉ có yếu tố vay vốn có mối quan hệ trái chiều với thu nhập của hộ gia đình. Điều này có thể do việc vay vốn tạo ra nợ và có thể giảm thu nhập ròng của hộ gia đình.</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1046,19 +1036,21 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive and detailed explanation of the various factors that influence the livelihood outcomes of residents in saline intrusion areas. It also explains the relationship between these factors and household income. The answer is well-structured, clear, and accurate, demonstrating a deep understanding of the topic.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the factors affecting the livelihood outcomes of residents in salt-affected areas. It also correctly identifies borrowing as the factor that has an inverse relationship with household income. However, without a reference answer, it's hard to confirm the absolute correctness of the information.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>According to the paper titled "Ảnh hưởng của xâm nhập mặn đến công tác quản lý và sử dụng nguồn tài nguyên nước dưới đất tại vùng ven biển tỉnh sóc trăng" by Hằng et al., how does saline intrusion affect the management of groundwater resources in Tran De district and its usage in aquaculture and rice farming areas?</t>
+          <t>Dựa trên nghiên cứu, hãy mô tả cách xâm nhập mặn ảnh hưởng đến việc quản lý và sử dụng nguồn tài nguyên nước dưới đất tại vùng ven biển tỉnh Sóc Trăng. Đặc biệt, hãy so sánh ảnh hưởng của xâm nhập mặn đối với người trồng tôm và người trồng lúa.</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>During periods influenced by salt, particularly in the dry season of 2016, saline intrusion posed challenges to the management of groundwater resources in Tran De district, especially in controlling the extraction and use of groundwater. In areas of aquaculture, shrimp farmers increased their extraction of groundwater to reduce the salinity concentration of surface water. However, for rice farmers, primarily in the Long Phu district, saline intrusion did not affect the demand for or extraction of groundwater.</t>
+          <t>Trong thời gian bị ảnh hưởng bởi xâm nhập mặn, đặc biệt trong mùa khô năm 2016, xâm nhập mặn đã gây ra khó khăn trong việc quản lý nguồn tài nguyên nước dưới đất, chủ yếu ở huyện Trần Đề. Điều này đặc biệt khó khăn trong việc kiểm soát việc khai thác và sử dụng nguồn nước dưới đất. 
+Đối với người nuôi tôm ở các khu vực nuôi trồng thủy sản, họ đã tăng cường khai thác nước dưới đất để giảm nồng độ mặn của nước mặt. Ngược lại, đối với người trồng lúa, chủ yếu ở huyện Long Phú, xâm nhập mặn không gây ảnh hưởng đến nhu cầu sử dụng và khai thác nước dưới đất. 
+Tuy nhiên, xâm nhập mặn đã gây ra khó khăn trong việc cung cấp nước ngọt đủ cho vụ lúa Xuân - Hè đầu năm 2016. Khô hạn kéo dài đã làm tăng nhu cầu sử dụng nước cho sản xuất lúa. Mặc dù vấn đề khai thác nước dưới đất được quản lý tốt, nhưng do hạn chế trong việc tiếp xúc giữa người dân và chính quyền địa phương, các quy định chưa được áp dụng một cách rộng rãi.</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1073,19 +1065,20 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how saline intrusion affects the management of groundwater resources in Tran De district and its usage in aquaculture and rice farming areas. However, it does not fully address the impact on rice farming areas as specified in the query, hence the slight deduction.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how saltwater intrusion affects the management and use of groundwater resources in coastal areas of Soc Trang province. It also compares the impact of saltwater intrusion on shrimp farmers and rice farmers, as requested by the user. The answer is comprehensive and seems accurate, although without a reference answer, it's hard to confirm the exact details. The score is not a perfect 5 because the answer could be more concise and better structured.</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>According to the research paper, how did saline intrusion during the dry season of 2016 affect the management and use of groundwater resources in the coastal areas of Soc Trang province, particularly in Tran De district and Long Phu district?</t>
+          <t>Theo nghiên cứu, xâm nhập mặn đã gây ra những khó khăn gì trong công tác quản lý và sử dụng nguồn tài nguyên nước dưới đất ở huyện Trần Đề? Và tác động của xâm nhập mặn đối với người trồng lúa ở huyện Long Phú là gì?</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>During the dry season of 2016, saline intrusion posed significant challenges to the management and use of groundwater resources, especially in the Tran De district. In aquaculture areas, shrimp farmers increased their extraction of groundwater to reduce the salinity concentration of surface water. However, for rice farmers in the Long Phu district, saline intrusion did not affect their demand for or extraction of groundwater.</t>
+          <t>Trong thời gian xâm nhập mặn, đặc biệt là mùa khô năm 2016, xâm nhập mặn đã gây ra khó khăn trong công tác quản lý nguồn tài nguyên nước dưới đất ở huyện Trần Đề. Cụ thể là việc kiểm soát khai thác và sử dụng nguồn tài nguyên này. Các khu vực nuôi trồng thủy sản, người nuôi tôm đã tăng cường khai thác nước dưới đất để pha loãng nồng độ mặn của nước mặt trên các kênh sông/rạch.
+Đối với người trồng lúa ở huyện Long Phú, xâm nhập mặn đã làm giảm đáng kể diện tích trồng lúa. Cụ thể ở Long Phú, diện tích đất trồng lúa giảm gần 1⁄2 (6.500 ha) vụ Xuân Hè (diện tích trồng lúa hàng năm của huyện xấp xỉ trên 13.000 ha) và gây thiệt hại hơn 4.000 ha (mức độ thiệt hại được thống kê từ 30% - 70%) do không đủ nguồn nước tưới cho cây lúa.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1100,19 +1093,21 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how saline intrusion affected the management and use of groundwater resources in the specified areas. It loses half a point for not providing more specific details or data to support the statements.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate response to both parts of the question. It discusses the difficulties in managing and using underground water resources in Trần Đề district due to saltwater intrusion, and the impact of saltwater intrusion on rice farmers in Long Phú district.</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>The paper discusses the impact of saline intrusion on agricultural production, specifically rice farming. Can you explain how this phenomenon affected the rice cultivation area in Long Phu, and what were the consequences?</t>
+          <t>Biến đổi khí hậu và nước biển dâng đã tác động như thế nào đến đồng bằng sông Cửu Long? Hãy nêu rõ những hậu quả mà xâm nhập mặn có thể gây ra trong mùa khô.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>The impact of saline intrusion on rice cultivation in Long Phu was significant. According to the climate change scenarios studied for 2004 and 2030, the area affected by saline intrusion for triple rice crop in Long Phu decreased by 35.5 hectares. This suggests that the saline intrusion has led to a reduction in the area suitable for rice cultivation. The consequences of this include a decrease in the productivity and revenue share of rice crops, a decrease in aquaculture production, and an increase in the revenue share of industrial crops like coconut, which are salt-resistant. This has led to farmers adopting new crops and switching crops as a risk diversification strategy to secure their income against salinization shocks.</t>
+          <t>Biến đổi khí hậu và nước biển dâng đã tạo ra những tác động nghiêm trọng đối với đồng bằng sông Cửu Long. Một trong những hậu quả nghiêm trọng nhất là sự tan băng và nước biển dâng, khiến nhiều vùng đất thấp có nguy cơ bị ngập chìm và xâm nhập mặn. Đặc biệt, nếu không có những chuyển biến tích cực kiểm soát khả năng nóng lên toàn cầu, có thể sẽ có ít nhất 25% diện tích các vùng đất thấp ven biển có nguy cơ bị chìm ngập do nước biển dâng và lún sụt đồng bằng. 
+Trong mùa khô, khoảng 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn. Điều này có thể gây ra những hậu quả nghiêm trọng cho nền nông nghiệp, với khoảng 30-40% diện tích nông nghiệp bị ảnh hưởng của nước mặn ngay cả trong mùa mưa, khó có thể trồng lúa và một số canh tác khác như chăn nuôi. 
+Ngoài ra, các vùng ven biển như thành phố Bạc Liêu, huyện Đông Hải, huyện Hòa Bình do kinh tế chủ yếu là nuôi thủy sản nên việc lấy nguồn nước biển thường xuyên phải mở thêm nhiều kênh rạch làm cho nước biển đi vào sâu phía trong được thuận lợi. Các vùng phía trong quốc lộ 1A như huyện Giá Rai, huyện Phước Long mấy năm gần đây do người dân tự ý chuyển đổi từ trồng lúa qua nuôi tôm phá vỡ việc vận hành của hệ thống cống ngăn mặn. Từ đó càng làm cho nước biển vào sâu trong nội đồng nguy cơ ngập ngày càng thể hiện rõ diện tích ngập tăng lên.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1127,19 +1122,19 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of saline intrusion on rice cultivation in Long Phu. It also discusses the consequences of this phenomenon. However, it lacks specific data or sources to support its claims, which prevents it from receiving a perfect score.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of climate change and sea level rise on the Mekong Delta. It also clearly outlines the consequences of saltwater intrusion during the dry season. The answer could be improved by providing more specific examples or data, but overall it is very accurate and informative.</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Explain the impact of the 2016 salinity crisis on aquaculture and rice production in Long Phú, as discussed in the document "researched_paper_cleanup.txt". What measures were taken by shrimp farmers to mitigate the effects of high salinity levels?</t>
+          <t>Theo nghiên cứu, hạn mặn năm 2016 đã ảnh hưởng như thế nào đến diện tích đất sản xuất lúa ở Long Phú và việc nuôi trồng thủy sản? Hãy giải thích nguyên nhân.</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>The document does not provide specific information on the impact of the 2016 salinity crisis on aquaculture and rice production in Long Phú, nor does it discuss any measures taken by shrimp farmers to mitigate the effects of high salinity levels.</t>
+          <t>Hạn mặn năm 2016 đã gây thiệt hại cho diện tích đất sản xuất lúa ở Long Phú. Tuy nhiên, nó ít ảnh hưởng đến việc nuôi trồng thủy sản, chủ yếu là nuôi cá nước ngọt, do phần lớn diện tích đất canh tác ở vùng này được sử dụng cho việc trồng lúa. Nguyên nhân là do người nuôi tôm đã sử dụng biện pháp bơm nước giếng khoan vào ao nuôi để pha loãng nồng độ mặn trong nước, giúp giảm ảnh hưởng của hạn mặn.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1154,19 +1149,19 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the topic of the 2016 salinity crisis and its impact on aquaculture and rice production in Long Phú. However, it does not provide any specific information or details, which makes it impossible to judge its correctness.</t>
+          <t>The generated answer is relevant and provides a detailed explanation of the impact of the 2016 saltwater intrusion on rice production and aquaculture in Long Phu. It also explains the reason why aquaculture was less affected. However, it could have been more specific about the extent of the damage to the rice fields.</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>The document mentions a regulation (Decree No. 33/2017/NĐ-CP) in relation to the use of well water in shrimp farming. Discuss the conflict between this regulation and the practical needs of shrimp farmers in harsh weather conditions. How does prolonged salinity crisis affect the management of water resources, especially in local areas?</t>
+          <t>Giải pháp mà người nuôi tôm sử dụng để hạ độ mặn trong nước là gì? Việc này có vi phạm quy định xử phạt quy phạm hành chính trong lĩnh vực tài nguyên nước và khoáng sản không? Nếu có, hãy trình bày về quy định đó và lý do tại sao người dân vẫn tiếp tục vi phạm.</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>The context provided does not mention any specific regulation such as Decree No. 33/2017/NĐ-CP in relation to the use of well water in shrimp farming. It also does not discuss any conflict between this regulation and the practical needs of shrimp farmers in harsh weather conditions. Furthermore, the context does not provide specific information on how a prolonged salinity crisis affects the management of water resources, especially in local areas.</t>
+          <t>Người nuôi tôm thường sử dụng phương pháp bơm nước giếng khoan vào ao nuôi để pha loãng nồng độ mặn trong nước. Tuy nhiên, việc này thực sự vi phạm quy định xử phạt quy phạm hành chính trong lĩnh vực tài nguyên nước và khoáng sản, theo điều 7 của Nghị định số 33/2017/NĐ-CP. Mặc dù vậy, việc thực thi quy định này ở địa phương thực sự khó khăn. Lý do chính là chi phí đầu tư vào các ao nuôi tôm rất cao. Trong điều kiện thời tiết khắc nghiệt, nếu không có giải pháp bơm thêm nước giếng khoan để pha loãng nồng độ mặn, các ao nuôi tôm có thể gặp nguy hiểm và dẫn đến chết tôm.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1176,24 +1171,24 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>The generated answer is not relevant to the user query. It does not provide any information about the regulation, the conflict with the needs of shrimp farmers, or the effects of a prolonged salinity crisis on water resource management. Instead, it simply states that the context does not provide this information, which is not helpful or informative.</t>
+          <t>The generated answer is highly relevant and accurate. It correctly addresses the user's query about the solution shrimp farmers use to reduce salinity in water, whether this violates any administrative regulations in the field of water and mineral resources, and if so, what those regulations are and why people continue to violate them. The answer is comprehensive and provides a clear explanation for all parts of the query.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Based on the research findings, what percentage of households surveyed were aware of the regulations for exploiting groundwater resources, and what percentage understood the consequences of over-exploitation?</t>
+          <t>Theo kết quả nghiên cứu trong bài báo, hãy phân tích mức độ tham gia và hiểu biết của người dân về việc khai thác nguồn tài nguyên nước dưới đất (NDĐ) và những hậu quả có thể xảy ra khi khai thác quá mức?</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>90% of the households surveyed were aware of the regulations for exploiting groundwater resources. However, only 3% of the households understood that over-exploitation of these resources could lead to land subsidence.</t>
+          <t>Theo kết quả nghiên cứu, 90% số hộ dân được phỏng vấn biết đến quy định về việc đăng ký khai thác nguồn nước dưới đất (NDĐ). Tuy nhiên, chỉ có 3% số hộ dân hiểu rằng việc khai thác NDĐ quá mức có thể gây sụt lún. Trong khi đó, 63% hộ dân cho rằng việc khai thác NDĐ quá mức không gây sụt lún và 34% số hộ dân không quan tâm đến vấn đề này. Điều này cho thấy mức độ tham gia và hiểu biết của người dân về việc khai thác NDĐ và hậu quả của việc khai thác quá mức còn hạn chế.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1203,26 +1198,25 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides specific percentages for both parts of the question. It is not possible to verify the correctness without a reference answer, but the response is detailed and seems plausible.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the public's participation and understanding of the exploitation of underground water resources and the potential consequences of over-exploitation. It provides specific statistics and concludes with an overall assessment, which aligns perfectly with the user's request.</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Discuss the impact of saltwater intrusion on rice cultivation and aquaculture, as mentioned in the document. How does the management and use of groundwater resources factor into this issue?</t>
+          <t>Trình bày những khó khăn và trở ngại trong công tác quản lý khai thác và sử dụng nguồn tài nguyên NDĐ? Đề xuất một số giải pháp để cải thiện tình hình.</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Saltwater intrusion has a significant impact on rice cultivation and aquaculture. The research shows that exposure to higher salinity decreases the productivity and revenue share of rice crops. It also decreases aquaculture production. However, it increases the revenue share of industrial crops, such as coconut, which are salt-resistant. This suggests that farmers are adopting new crops and switching crops as a risk diversification strategy to secure their income against salinization shocks. 
-In terms of land use, higher salinity intrusion is associated with decreases not only in farmers’ land used for rice but also in their general land used for agriculture. Salinization also affects labor supply, reducing it in agriculture for those without agricultural land, while labor supply for those with agricultural land does not respond to higher salinity.
-The document does not provide specific information on the management and use of groundwater resources in relation to saltwater intrusion. However, it does mention that the operation of sluice gates, which can slow the intrusion of saltwater, is likely correlated with the development of local agricultural production.</t>
+          <t>Công tác quản lý khai thác và sử dụng nguồn tài nguyên NDĐ gặp phải một số khó khăn và trở ngại. Một trong số đó là việc quản lý chủ yếu tập trung ở cấp chính quyền, mức độ tham gia của người dân chưa cao. Thêm vào đó, việc đăng ký và kiểm soát khai thác NDĐ vẫn còn một số hạn chế. Hiệu quả hoạt động của hệ thống thủy lợi là cốt yếu trong việc cung cấp nguồn nước và duy trì hệ thống canh tác của vùng, vì thế công tác nạo vét, bảo dưỡng công trình cần được quan tâm, nhất là vào mùa khô. 
+Để cải thiện tình hình, một số giải pháp có thể được đề xuất. Đầu tiên, việc phổ biến các quy định trong khai thác và sử dụng nguồn NDĐ cần được tiến hành theo chiều sâu để các chính sách được thực hiện một cách có hiệu quả, hạn chế tình trạng khai thác quá mức nguồn NDĐ. Thứ hai, cần thay đổi tư duy và tiếp cận, không chỉ dựa vào hướng dẫn và nguồn lực hỗ trợ từ Trung ương mà cần đề cao nội lực và huy động sự tham gia rộng rãi của các tổ chức, doanh nghiệp, người dân. Cuối cùng, việc hoàn thiện thể chế, chính sách triển khai thực hiện các nhiệm vụ cũng rất quan trọng, cần tăng tốc độ và đồng bộ hóa với nguồn lực thực hiện.</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1237,46 +1231,48 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of saltwater intrusion on rice cultivation and aquaculture. It also attempts to address the part of the query about groundwater resources, although it admits that the document does not provide specific information on this. The answer could be improved by providing more general information on how groundwater management might affect saltwater intrusion, even if the document does not provide specifics.</t>
+          <t>The generated answer is highly relevant to the user query and provides a comprehensive response. It correctly identifies the challenges in managing and exploiting NDĐ resources and proposes several solutions to improve the situation. The answer is well-structured and detailed, making it a high-quality response.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Explain the proposed model for simulating the impact of sea level rise on agricultural production areas, as discussed in the paper by Hiển et al. What are the key components of this model and how does it predict future scenarios?</t>
+          <t>Hãy mô tả quá trình nước biển dâng xâm lấn vào nội đồng diễn biến như thế nào? Hãy nêu rõ các yếu tố ảnh hưởng đến quá trình này.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>The context does not provide information on a proposed model for simulating the impact of sea level rise on agricultural production areas, as discussed in a paper by Hiển et al. Therefore, I cannot provide details on the key components of this model or how it predicts future scenarios.</t>
+          <t>Quá trình nước biển dâng xâm lấn vào nội đồng diễn ra khi nước biển từ các cửa sông chảy theo sông và kênh vào phía trong nội đồng. Khi càng đi sâu vào, lượng nước sẽ giảm do tràn và thấm vào đất, tương ứng với hệ số dòng sông và kênh giảm. Nước biển chảy theo sông/kênh sẽ thấm vào đất hoặc tràn lên đất (nếu mực nước cao hơn độ cao của địa hình) làm cho đất bị ngập úng và nhiễm mặn.
+Các yếu tố ảnh hưởng đến quá trình này bao gồm việc xây dựng hệ thống cống, hệ thống đê, việc mở thêm nhiều kênh rạch ở các vùng ven biển như thành phố Bạc Liêu, huyện Đông Hải, huyện Hòa Bình để lấy nguồn nước biển cho nuôi thủy sản. Đồng thời, việc người dân tự ý chuyển đổi từ trồng lúa qua nuôi tôm ở các vùng phía trong quốc lộ 1A như huyện Giá Rai, huyện Phước Long trong mấy năm gần đây cũng phá vỡ việc vận hành của hệ thống cống ngăn mặn, làm cho nước biển vào sâu trong nội đồng và nguy cơ ngập ngày càng thể hiện rõ.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>The generated answer is not relevant to the user query as it does not provide any information about the proposed model for simulating the impact of sea level rise on agricultural production areas, as discussed in the paper by Hiển et al.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the process of sea water intrusion into the inland delta. It also clearly outlines the factors affecting this process. The answer is comprehensive and appears to be correct, even without a reference answer for comparison.</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Based on the findings of the paper, discuss the effects of sea level rise on coastal and inland districts. How does the construction of sea barriers and the change from rice cultivation to shrimp farming by locals affect the infiltration of sea water into the inland areas?</t>
+          <t>Dựa vào kết quả mô phỏng, hãy phân tích tình hình ngập úng và nhiễm mặn ở các huyện ven biển và các huyện phía trong. Hãy đưa ra các nguyên nhân dẫn đến sự khác biệt này.</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on the effects of sea level rise on coastal and inland districts, the construction of sea barriers, or the change from rice cultivation to shrimp farming by locals and its effect on the infiltration of sea water into the inland areas.</t>
+          <t>Kết quả mô phỏng cho thấy các huyện ven biển như thành phố Bạc Liêu, huyện Đông Hải, huyện Hòa Bình thường bị ngập ở mức cao hơn so với các huyện phía trong. Một nguyên nhân chính là do kinh tế của các huyện này chủ yếu dựa vào nuôi thủy sản, nên việc lấy nguồn nước biển thường xuyên phải mở thêm nhiều kênh rạch, làm cho nước biển dễ dàng xâm nhập vào phía trong. 
+Trong khi đó, các vùng phía trong quốc lộ 1A như huyện Giá Rai, huyện Phước Long trong những năm gần đây cũng đang đối mặt với tình trạng ngập úng và nhiễm mặn tăng lên. Điều này chủ yếu do người dân tự ý chuyển đổi từ trồng lúa qua nuôi tôm, phá vỡ việc vận hành của hệ thống cống ngăn mặn, làm cho nước biển dễ dàng xâm nhập vào sâu trong nội đồng.</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1291,20 +1287,20 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant information or answer to the user's query. It simply states that the context does not provide the necessary information, which is not helpful or informative.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the flooding and salinity situation in coastal and inland districts. It also provides reasons for the differences observed. The answer is accurate and comprehensive, but it could be slightly more concise.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Based on the research paper, what are the projected impacts of sea level rise on agricultural production in the Bạc Liêu province from 2016 to 2050?</t>
+          <t>Hãy mô tả kịch bản nước biển dâng xâm lấn vào nội đồng giai đoạn năm 2016 đến năm 2050 mà tác giả đã đề xuất. Theo kịch bản này, những vấn đề gì sẽ xảy ra với sản xuất nông nghiệp và cuộc sống của người dân tỉnh Bạc Liêu?</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>The projected impacts of sea level rise on agricultural production in the Bạc Liêu province from 2016 to 2050 are quite severe. The rising sea levels are expected to increasingly affect the agricultural production areas each year, posing complex risks. The simulation results of the flood risk map for the highest flood months for the years 2020, 2030, 2040, 2050 under low, medium, and high scenarios show this. 
-In the future, if the system of dikes and dams is properly planned, it will reduce the adverse effects of rising sea levels. However, agricultural production in the dry season will be very difficult due to severe drought and lack of fresh water. This situation could lead to poverty, food shortages, lack of fresh water for living, economic downturn, and many other negative consequences. Therefore, measures to remedy the flooding situation are needed, such as re-planning the canal system, dredging canals to create flow to share the water volume on the rivers with each other; building a reasonable dike system to prevent sea water and a salt prevention dam system to prevent sea water from invading the fields, reducing damage caused by saline intrusion.</t>
+          <t>Theo kịch bản nước biển dâng xâm lấn vào nội đồng từ năm 2016 đến năm 2050, mức độ ảnh hưởng của nước biển dâng đến vùng sản xuất nông nghiệp sẽ tăng lên rất cao theo từng năm, tiềm ẩn nguy cơ phức tạp. Các mô phỏng bản đồ nguy cơ ngập cho thấy tình trạng ngập lụt sẽ tăng lên vào các năm 2020, 2030, 2040, 2050 theo kịch bản mức thấp, mức trung bình và mức cao.
+Tình trạng ngập lụt chung cho tỉnh Bạc Liêu sẽ ảnh hưởng đến các khu vực huyện trong tỉnh. Nếu không có quy hoạch hệ thống đê và đập hợp lý, tình trạng nước biển dâng sẽ gây ra những ảnh hưởng không tốt. Sản xuất nông nghiệp vào mùa khô sẽ trở nên khó khăn do khô hạn và thiếu nước ngọt. Điều này dẫn đến nghèo đói, thiếu lương thực, thiếu nguồn nước ngọt để sinh hoạt, kinh tế đi xuống và nhiều hệ lụy xấu khác.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1319,19 +1315,20 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the projected impacts of sea level rise on agricultural production in the Bạc Liêu province from 2016 to 2050. It also suggests potential solutions to mitigate these impacts. The answer is comprehensive and seems accurate, but without a reference answer, it's hard to confirm its complete correctness.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed description of the scenario of sea level rise invading the mainland from 2016 to 2050. It also correctly identifies the potential problems that will occur with agricultural production and the lives of the people in Bac Lieu province. The only reason it doesn't get a perfect score is because it could have provided more specific examples or data to support its points.</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>What are the proposed solutions to mitigate the negative effects of sea level rise and saltwater intrusion into farmlands in the Bạc Liêu province as mentioned in the document?</t>
+          <t>Theo nội dung bài viết, hãy liệt kê và giải thích các biện pháp mà tác giả đề xuất để khắc phục tình trạng ngập lụt do nước biển dâng tại tỉnh Bạc Liêu.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>The document suggests several solutions to mitigate the negative effects of sea level rise and saltwater intrusion into farmlands. Firstly, it emphasizes the need to increase awareness and understanding of the importance of Resolution 120 and the Planning Law No. 21/2017/QH14 among leaders, officials, and citizens. Secondly, it proposes a review of outdated or inappropriate plans and projects, especially those with significant ecological and biodiversity impacts. Thirdly, it recommends comprehensive assessments of the economic, social, and environmental aspects of large projects implemented in the past. Fourthly, it advocates for a firm stance against expanding dyke areas, aiming to maintain and restore freshwater storage areas during the flood season. Fifthly, it suggests reducing the number of coal-fired power plants and encouraging investment in renewable energy sources such as solar, wind, biomass, wave, and tidal power. Lastly, it calls for enhanced international cooperation, particularly between Vietnam and the Netherlands, in adapting to climate change and water management.</t>
+          <t>Tác giả đề xuất một số biện pháp để khắc phục tình trạng ngập lụt do nước biển dâng tại tỉnh Bạc Liêu. Đầu tiên, tác giả đề cập đến việc quy hoạch lại hệ thống kênh, vét kênh tạo dòng chảy nhằm chia sẻ lượng nước trên các con sông với nhau. Điều này giúp cân đối lượng nước, giảm thiểu nguy cơ ngập lụt khi có biến động về mực nước biển.
+Tiếp theo, tác giả cũng đề nghị xây dựng hệ thống đê điều hợp lý ngăn nước biển và hệ thống đập ngăn mặn ngăn nước biển xâm nhập vào đồng ruộng. Việc này không chỉ giúp giảm thiệt hại do xâm nhập mặn gây ra mà còn bảo vệ các khu vực sản xuất nông nghiệp, giảm thiểu nguy cơ thiếu nước ngọt trong sinh hoạt và sản xuất.</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1346,20 +1343,20 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed list of proposed solutions to mitigate the negative effects of sea level rise and saltwater intrusion into farmlands in the Bạc Liêu province. It does not contain any noticeable mistakes. However, it could be more concise.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the measures proposed by the author to address the issue of flooding due to sea level rise in Bac Lieu province. The answer is also correct as it accurately reflects the content of the user's query.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>In the context of the Mekong Delta region's vulnerability to sea level rise, describe the simulation model researched to understand the impact on agricultural production areas. How does the model account for the various geographical and infrastructural elements in the region?</t>
+          <t>Trong nghiên cứu mô phỏng mô hình xâm lấn do nước biển dâng ảnh hưởng đến khu vực sản xuất nông nghiệp tại khu vực ĐBSCL, hãy mô tả quá trình xác định hướng nước biển xâm lấn và cách thức xây dựng bản đồ số thể hiện quá trình ngập úng, ngập mặn địa hình.</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>The simulation model used to understand the impact on agricultural production areas in the Mekong Delta region due to sea level rise is a hydrodynamic model. This model uses flow data related to physical data such as river and canal cross-sections, banks or fields. The model aims to improve the description of flood propagation over the floodplain, water exchange between the floodplains and the river channels, the effect of topography and infrastructure on flooding, morphological changes, and bank erosion potential and changes over time. 
-When it comes to saline intrusion, the model takes into account the low slopes of the Mekong and its tributaries’ river beds and the complex of a two tidal regime. This makes the modelling of salinity intrusion for the whole system quite complicated. The results from these models can be used as a technical prerequisite for the development of a regional strategy and action plan to prepare for flood loss prevention and salinity management for the vulnerable agricultural sector.</t>
+          <t>Quá trình xác định hướng nước biển xâm lấn được mô tả như sau: Nước biển từ các cửa sông sẽ chảy theo sông và kênh vào phía trong nội đồng. Càng vào trong thì lượng nước sẽ giảm do tràn và thấm vào đất tương ứng với hệ số dòng sông và kênh giảm. Nước biển chảy theo sông/kênh sẽ thấm vào đất hoặc tràn lên đất (nếu mực nước cao hơn độ cao của địa hình) làm cho đất bị ngập úng và nhiễm mặn.
+Về việc xây dựng bản đồ số thể hiện quá trình ngập úng, ngập mặn địa hình, nghiên cứu đã tiến hành xây dựng bản đồ số thể hiện quá trình ngập úng, ngập mặn địa hình do nước biển dâng xâm lấn vào vùng sản xuất nông nghiệp trong đất liền thông qua bản đồ theo thời gian. Từ đó đưa ra các thống kê về diện tích ngập theo thời gian, theo từng đơn vị hành chính (cấp tỉnh, cấp huyện) trên địa bàn một tỉnh được chọn thí điểm (tỉnh Bạc Liêu) trong khu vực ĐBSCL cũng đã được mô tả chi tiết trên cơ sở các kịch bản trong quá khứ và cho các giai đoạn trong tương lai.</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1374,19 +1371,19 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the simulation model used to understand the impact of sea level rise on agricultural production areas in the Mekong Delta region. It also explains how the model accounts for various geographical and infrastructural elements in the region. The only reason it doesn't get a perfect score is because it doesn't explicitly mention how the model accounts for infrastructural elements, although it does mention the effect of infrastructure on flooding.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the process of determining the direction of sea water intrusion and the construction of a digital map showing the process of flooding and salinization of the terrain. The answer is complete and accurate, with no errors or omissions.</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Based on the analysis and comparison of desalination technologies used in Vietnam and worldwide, which technology was identified as having the greatest potential for application in rural villages in the Mekong Delta? Explain why this technology is considered the most effective for desalinating groundwater contaminated by salinity.</t>
+          <t>Trong bối cảnh hạn và xâm nhập mặn tại Đồng bằng sông Cửu Long, công nghệ nào được đánh giá có tiềm năng ứng dụng cao nhất để khử mặn và làm ngọt hóa nguồn nước ngầm đang bị nhiễm mặn? Hãy giải thích lý do vì sao công nghệ này được lựa chọn.</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>The technology identified as having the greatest potential for application in rural villages in the Mekong Delta is electrodialysis. This technology was chosen based on an analysis and comparison of various desalination technologies used in Vietnam and worldwide. The study found that electrodialysis has the highest potential for application due to its effectiveness in desalinating groundwater that has been contaminated by salinity, thus ensuring the provision of safe and sufficient water for rural communities in the Mekong Delta.</t>
+          <t>Công nghệ ED (Electrodialysis) được đánh giá có tiềm năng ứng dụng cao nhất để khử mặn và làm ngọt hóa nguồn nước ngầm đang bị nhiễm mặn. Lý do là công nghệ ED sử dụng nguồn điện một chiều, do đó rất phù hợp để sử dụng nguồn năng lượng mặt trời (nguồn một chiều). Bởi vì tiêu thụ năng lượng ít hơn công nghệ RO (Reverse Osmosis), nên chi phí đầu tư cho hệ thống điện năng lượng mặt trời sẽ ít hơn. Hơn nữa, chi phí đầu tư và vận hành hệ thống khử mặn nước lợ với tổng chất rắn hòa tan-TDS- dưới 5000mg/lít, thì sử dụng công nghệ ED có chi phí rẻ hơn loại công nghệ RO.</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1401,19 +1398,19 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and appears to be correct, providing a specific technology (electrodialysis) and explaining why it is considered effective for desalinating groundwater contaminated by salinity in the Mekong Delta. However, without a reference answer, it's not possible to confirm the absolute correctness of the information.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of why the ED (Electrodialysis) technology is considered to have the highest potential for desalination and sweetening of saline-contaminated groundwater. The answer could be improved by providing more context or examples, but overall it is very informative and accurate.</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>What are the two types of desalination technologies mentioned in the text and how do they differ in terms of energy consumption and suitability for use in rural areas of Vietnam?</t>
+          <t>Theo nghiên cứu, công nghệ khử mặn nào có chi phí đầu tư và vận hành rẻ hơn khi xử lý nước lợ với tổng chất rắn hòa tan (TDS) dưới 5000mg/lít? Vì sao công nghệ này lại có chi phí rẻ hơn?</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>The two types of desalination technologies mentioned in the text are thermal and membrane. The text specifically highlights electrodialysis (ED), a type of membrane technology, as having the greatest potential for application in rural areas of Vietnam. ED uses direct current electricity, making it suitable for use with solar energy, a direct current source. Because it consumes less energy than reverse osmosis (RO) technology, the investment cost for a solar power system would be lower when using ED.</t>
+          <t>Công nghệ khử mặn ED (Electrodialysis) có chi phí đầu tư và vận hành rẻ hơn khi xử lý nước lợ với tổng chất rắn hòa tan (TDS) dưới 5000mg/lít so với công nghệ RO (Reverse Osmosis). Lý do là công nghệ ED sử dụng nguồn điện một chiều, do đó rất phù hợp để sử dụng nguồn năng lượng mặt trời (nguồn một chiều). Vì tiêu thụ năng lượng ít hơn công nghệ RO, nên chi phí đầu tư cho hệ thống điện năng lượng mặt trời sẽ ít hơn.</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1428,48 +1425,46 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and accurate. It correctly identifies the two types of desalination technologies mentioned in the query and provides a detailed explanation of their energy consumption and suitability for use in rural areas of Vietnam. The only reason it doesn't get a perfect score is because it doesn't explicitly compare the energy consumption of thermal and membrane technologies.</t>
+          <t>The generated answer is relevant and correct. It accurately identifies Electrodialysis (ED) as a desalination technology with lower investment and operating costs for treating brackish water with a total dissolved solids (TDS) under 5000mg/liter compared to Reverse Osmosis (RO). It also provides a valid reason for the lower cost, which is the lower energy consumption of ED technology, making it suitable for using solar energy. The answer could be improved by providing more detailed cost comparisons or more specific data to support the claim.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Based on the six standards mentioned in the text, describe the requirements for a desalination system to be effective and economically viable in rural communities in Vietnam.</t>
+          <t>Liệt kê và giải thích 6 tiêu chuẩn được áp dụng cho một hệ thống khử mặn quy mô cụm dân cư nông thôn ĐBSCL theo nghiên cứu.</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>An effective and economically viable desalination system in rural communities in Vietnam would need to adhere to several standards. Firstly, it should enhance awareness and understanding among leaders, officials, and people about the importance of Resolution 120 and the Planning Law No. 21/2017/QH14. Secondly, it should review and halt the implementation of outdated or inappropriate plans, especially those that have significant impacts on a wide area and affect the ecosystem, biodiversity, and natural conditions of the Mekong Delta.
-Thirdly, comprehensive assessments of the economic, social, and environmental aspects of large projects implemented in the past should be conducted to learn lessons before considering other large projects. Fourthly, it should decisively prevent the expansion of dyke areas to maintain and restore freshwater storage areas during the flood season. Fifthly, it should reduce the number of coal-fired power plants and encourage and facilitate investment in the development of renewable energy sources such as solar, wind, biomass, wave, and tidal power.
-Lastly, it should enhance international cooperation, especially between Vietnam and the Netherlands, according to the strategic partnership agreement on climate change adaptation and water management.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không đề cập đến 6 tiêu chuẩn được áp dụng cho một hệ thống khử mặn quy mô cụm dân cư nông thôn ĐBSCL.</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>The generated answer is somewhat relevant to the user query as it discusses standards for environmental projects in Vietnam. However, it does not specifically address the requirements for a desalination system to be effective and economically viable in rural communities in Vietnam. The answer seems to be more focused on general environmental and energy policies rather than on the specifics of desalination systems.</t>
+          <t>The generated answer is not relevant to the user query as it does not provide any information about the 6 standards applied to a desalination system for a rural residential cluster in the Mekong Delta region as per the research.</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Based on the research paper "Lựa chọn mô hình sản xuất của hộ trồng lúa trong điều kiện xâm nhập mặn ở đồng bằng sông cửu long" by Khôi and Khải, what are the key factors that influence a rice farmer's decision to choose integrated rice farming in the Mekong River Delta?</t>
+          <t>Theo nghiên cứu, công nghệ nào được đề xuất để khử mặn cho các cụm dân cư nông thôn vùng ĐBSCL? Hãy nêu các lý do mà nghiên cứu đưa ra để lựa chọn công nghệ này.</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>The key factors that influence a rice farmer's decision to choose integrated rice farming in the Mekong River Delta include land area, levels of education, members generating main income, saline intrusion, sources of water for irrigation, and bank loan status. Among these, land area and saline intrusion are the most significant factors.</t>
+          <t>Công nghệ điện thẩm tách (Electrodialysis – ED) được đề xuất để khử mặn cho các cụm dân cư nông thôn vùng ĐBSCL. Các lý do mà nghiên cứu đưa ra để lựa chọn công nghệ này bao gồm: công nghệ ED có chi phí rẻ hơn công nghệ RO khi xử lý nước lợ có tổng chất rắn hòa tan (TDS) dưới 5000mg/lít; công nghệ ED sử dụng nguồn điện một chiều, phù hợp để sử dụng nguồn năng lượng mặt trời; và do tiêu thụ năng lượng ít hơn công nghệ RO, nên chi phí đầu tư cho hệ thống điện năng lượng mặt trời sẽ ít hơn.</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1484,19 +1479,19 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed and comprehensive list of factors that influence a rice farmer's decision to choose integrated rice farming in the Mekong River Delta. It also highlights the most significant factors among them.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and correct response. It correctly identifies the technology proposed for desalination in rural communities in the Mekong Delta region and provides the reasons for this choice as requested in the query.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>According to the data from the Disaster Prevention and Mitigation Center of the Ministry of Agriculture and Rural Development, what is the salinity level considered as saline intrusion and how far has this salinity intrusion been measured in the Tiền and Hậu rivers?</t>
+          <t>Trong nghiên cứu "Lựa chọn mô hình sản xuất của hộ trồng lúa trong điều kiện xâm nhập mặn ở đồng bằng sông cửu long" của Khôi và Khải, hãy liệt kê các yếu tố ảnh hưởng đến xác suất chuyển đổi từ mô hình chuyên canh lúa sang lúa – tôm và lúa – cá.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>The context does not provide information on the salinity level considered as saline intrusion according to the Disaster Prevention and Mitigation Center of the Ministry of Agriculture and Rural Development, nor does it mention how far this salinity intrusion has been measured in the Tiền and Hậu rivers.</t>
+          <t>Các yếu tố ảnh hưởng đến xác suất chuyển đổi từ mô hình chuyên canh lúa sang lúa – tôm bao gồm diện tích đất, trình độ học vấn, lao động chính, nhập mặn, nguồn nước và vay vốn. Đối với mô hình lúa – cá, các yếu tố tác động đến xác suất chuyển đổi bao gồm trình độ học vấn, nhập mặn, và nguồn nước.</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1506,26 +1501,24 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant or correct information in response to the user's query. It simply states that the information is not available, which does not answer the question.</t>
+          <t>The generated answer is relevant and appears to be fully correct, providing a detailed list of factors that influence the probability of transitioning from a rice farming model to a rice-shrimp or rice-fish model. It directly addresses the user's query without any noticeable errors or omissions.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>What are some of the national solutions that have been implemented to control salt intrusion, as mentioned in the document? How effective have these solutions been, particularly in coastal provinces like Cà Mau, Sóc Trăng, and Trà Vinh?</t>
+          <t>Theo Trung tâm phòng tránh và giảm nhẹ thiên tai thuộc Bộ Nông nghiệp và Phát triển Nông thôn, mức độ mặn nào được xem là bị xâm nhập mặn? Hãy mô tả tình hình xâm nhập mặn ở sông Tiền và sông Hậu.</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Several national solutions have been implemented to control salt intrusion. These include enhancing awareness and understanding of the importance of Resolution 120 and the Planning Law No. 21/2017/QH14 among leaders, officials, and citizens. There has also been a review of old plans and projects that are no longer suitable or contrary to the spirit of the Resolution, with a particular focus on large projects that have a significant impact on a wide area and affect the ecosystem, biodiversity, and natural conditions of the Mekong Delta.
-Other measures include comprehensive assessments of the economic, social, and environmental aspects of large projects that have been implemented in the past, to learn lessons before considering other large projects. There is a firm stance against expanding dyke areas, in order to maintain and restore freshwater storage areas during the flood season. The number of coal-fired power plants is being reduced, while encouraging and facilitating investment in the development of renewable energy sources such as solar, wind, biomass, wave, and tidal power. International cooperation is also being strengthened, especially between Vietnam and the Netherlands, according to a strategic partnership agreement on climate change adaptation and water management.
-However, the effectiveness of these solutions has not been fully evaluated in the context. The document does mention that current adaptation options have some limitations, as they do not fully consider the differences in terms of ecological, social, and economic environment. The vulnerability of people highly depends on these conditions, so future adaptation strategies should take these issues into account to benefit different social groups, especially the most vulnerable.</t>
+          <t>Mức độ mặn 4‰ được Trung tâm phòng tránh và giảm nhẹ thiên tai thuộc Bộ Nông nghiệp và Phát triển Nông thôn xác định là bị xâm nhập mặn. Tuy nhiên, tình hình ở sông Tiền và sông Hậu nghiêm trọng hơn nhiều, với số liệu đo độ mặn cho kết quả trên 45‰. Độ mặn này kéo dài và xâm nhập sâu tới 70 km tính từ cửa sông, thậm chí có thời điểm độ mặn xâm nhập sâu đến 85 km.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1540,23 +1533,19 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the national solutions implemented to control salt intrusion. It also discusses the effectiveness of these solutions, although it does not specifically mention the coastal provinces like Cà Mau, Sóc Trăng, and Trà Vinh. The answer is comprehensive and accurate, but the lack of specific information about the mentioned provinces prevents it from receiving a perfect score.</t>
+          <t>The generated answer is relevant and appears to be correct, providing specific information about the salinity level considered as salt intrusion and describing the situation in the Tien and Hau rivers. However, without a reference answer, it's difficult to confirm the absolute accuracy of the details provided.</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Based on the research findings, how has salt intrusion affected the quality of the environment and the agricultural practices of farmers? How do the studies of Gbetibouo &amp; Hassan (2005), and Seo &amp; Mendelsohn (2007) support the trend of adapting production to natural conditions and proactively reducing the impact of climate change?</t>
+          <t>Hãy nêu một số giải pháp cấp quốc gia đã được áp dụng để kiểm soát xâm nhập mặn? Tại sao các tỉnh ven biển như Cà Mau, Sóc Trăng và Trà Vinh lại dễ bị tổn thương bởi xâm nhập mặn?</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Salt intrusion has had a significant impact on the environment and agricultural practices in the Mekong Delta. It has been found to decrease the productivity and revenue share of rice crops, as well as aquaculture production. However, it has also led to an increase in the revenue share of industrial crops, particularly coconut, which is a salt-resistant crop. This suggests that farmers are adopting new crops and switching crops as a mechanism for risk diversification, helping them secure their income against salinization shocks.
-In terms of land use, higher salinity intrusion is associated with decreases in farmers' land used for rice and their general land used for agriculture. Salinization has also been found to affect labor supply, reducing it in agriculture for those without agricultural land, while those with agricultural land do not see a change in labor supply due to higher salinity.
-Salinization also reduces farmer households' income and consumption. However, it has been found to increase household spending on education, potentially indicating farmers' increased investment to acquire new skills. 
-In terms of adaptation, the evidence on out-migration for off-farm work in urban centers is mixed, but there is support for the hypothesis that a more developed local credit market plays a positive role in easing the income losses incurred by farmers during salinization shocks.
-Unfortunately, the context does not provide information on the studies of Gbetibouo &amp; Hassan (2005), and Seo &amp; Mendelsohn (2007), so it's not possible to comment on how these studies support the trend of adapting production to natural conditions and proactively reducing the impact of climate change.</t>
+          <t>Một trong những giải pháp cấp quốc gia đã được áp dụng để kiểm soát xâm nhập mặn là dự án xây dựng hệ thống kênh rạch dẫn nước ở Đồng bằng sông Cửu Long. Các tỉnh ven biển như Cà Mau, Sóc Trăng và Trà Vinh dễ bị tổn thương bởi xâm nhập mặn do chúng có tỷ lệ hộ trồng lúa và diện tích lúa bị nhiễm mặn lớn nhất trong vùng. Các mô hình trồng lúa chuyên canh 3 vụ lúa hoặc 2 vụ lúa cũng dễ tổn thương với xâm nhập mặn do nước mặn sẽ kìm hãm sự phát triển sinh lý của cây lúa.</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1571,19 +1560,19 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>The generated answer provides a comprehensive explanation of how salt intrusion affects the environment and agricultural practices, including impacts on crop productivity, land use, labor supply, and household income. It also discusses the adaptation strategies of farmers. However, it does not address the second part of the user's query about the studies of Gbetibouo &amp; Hassan (2005), and Seo &amp; Mendelsohn (2007), which results in a slight deduction in the score.</t>
+          <t>The generated answer is relevant and mostly correct. It provides a solution that has been implemented at the national level to control saltwater intrusion and explains why coastal provinces like Ca Mau, Soc Trang, and Tra Vinh are vulnerable to saltwater intrusion. However, it could have included more diverse solutions for a more comprehensive answer.</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Based on the research findings, what are the trends in farming adaptations to climate change in South America as per the studies by Gbetibouo &amp; Hassan (2005), and Seo &amp; Mendelsohn (2007)?</t>
+          <t>Theo nghiên cứu, hãy mô tả xu hướng chuyển đổi sản xuất của nông dân ở Nam Mỹ để thích ứng với điều kiện tự nhiên và giảm bớt tác động của biến đổi khí hậu. Hãy đưa ra các ví dụ cụ thể từ các nghiên cứu của Gbetibouo &amp; Hassan (2005), Seo &amp; Mendelsohn (2007) để hỗ trợ câu trả lời của bạn.</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>The context does not provide information on the trends in farming adaptations to climate change in South America as per the studies by Gbetibouo &amp; Hassan (2005), and Seo &amp; Mendelsohn (2007).</t>
+          <t>Rất tiếc, thông tin cung cấp không đưa ra chi tiết cụ thể về xu hướng chuyển đổi sản xuất của nông dân ở Nam Mỹ để thích ứng với điều kiện tự nhiên và giảm bớt tác động của biến đổi khí hậu, cũng như không có ví dụ cụ thể từ các nghiên cứu của Gbetibouo &amp; Hassan (2005), Seo &amp; Mendelsohn (2007).</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1598,24 +1587,25 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information relevant to the user's query about the trends in farming adaptations to climate change in South America according to the specified studies.</t>
+          <t>The generated answer is not relevant to the user query. The user asked for a description of the trend of farmers in South America adapting to natural conditions and mitigating the impact of climate change, with specific examples from the studies of Gbetibouo &amp; Hassan (2005), Seo &amp; Mendelsohn (2007). The generated answer does not provide any of this information.</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Analyze the data provided on the distribution of rice farming models in the research area. What are the differences in education level and gender distribution among the households practicing monoculture and combined rice farming?</t>
+          <t>Dựa trên kết quả nghiên cứu, hãy phân tích sự khác biệt giữa các hộ trồng lúa chuyên canh và hộ trồng lúa kết hợp về tỷ lệ, mô hình sản xuất, trình độ học vấn của chủ hộ và tỷ lệ vay vốn. Hãy đưa ra giả thuyết về nguyên nhân của những khác biệt này.</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on the distribution of education level and gender among households practicing monoculture and combined rice farming.</t>
+          <t>Các hộ trồng lúa chuyên canh chiếm 51,64% trong khi hộ trồng lúa kết hợp chiếm 48,36%. Mô hình lúa-màu và lúa-cá có tỷ lệ cao hơn so với mô hình lúa-tôm. Chủ hộ trồng lúa chuyên canh có trình độ học vấn từ cấp 3 trở lên chiếm tỷ lệ thấp hơn so với nhóm hộ trồng lúa kết hợp, với tỷ lệ 32,33% so với 40,21%. Tuy nhiên, tỷ lệ phân bổ giới tính của chủ hộ thiên về nam giới với tỷ lệ trên 90% và không có sự khác biệt đáng kể giữa hai mô hình. Chủ hộ trồng lúa chuyên canh có tỷ lệ vay vốn là 86% so với tỷ lệ vay vốn 79% của nhóm hộ trồng lúa kết hợp.
+Nguyên nhân của những khác biệt này có thể do các yếu tố như diện tích đất, tuổi chủ hộ, học vấn, và nguồn nước. Các hộ có diện tích sản xuất lớn thường thực hiện chuyển đổi sang mô hình lúa – tôm nhiều hơn, do yêu cầu về diện tích canh tác và nguồn vốn đầu tư để chuyển đổi. Trong khi đó, hộ trồng lúa càng có diện tích đất sản xuất ít, sẽ không đủ điều kiện tạo ra thu nhập cho gia đình ổn định và nguồn lực để chuyển đổi.</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1625,19 +1615,19 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and correctly states that the provided context does not contain the specific information asked for. However, it does not attempt to provide any further analysis or insight, which could have improved the response.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the differences between specialized rice farming households and combined rice farming households in terms of proportion, production model, education level of the household head, and loan rate. It also hypothesizes the reasons for these differences. The answer is comprehensive and appears to be accurate, although without a reference answer, it's hard to confirm the exact accuracy. However, based on the information provided, it seems to be a well-researched and well-presented response.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Based on the research paper, how does the salinity intrusion affect the probability of transitioning from specialized rice cultivation to a rice-shrimp model? What is the significance level of this correlation?</t>
+          <t>Theo nghiên cứu, xâm nhập mặn có tương quan thuận với xác suất chuyển đổi từ lúa chuyên canh sang lúa – tôm ở mức ý nghĩa là bao nhiêu phần trăm? Hãy giải thích tác động biên của xâm nhập mặn đối với xác suất chuyển đổi này.</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>The research paper does not provide specific information on the impact of salinity intrusion on the probability of transitioning from specialized rice cultivation to a rice-shrimp model, nor does it mention the significance level of such a correlation.</t>
+          <t>Xâm nhập mặn có tương quan thuận với xác suất chuyển đổi từ lúa chuyên canh sang lúa – tôm ở mức ý nghĩa là 1%. Tác động biên của xâm nhập mặn cho thấy xác suất chuyển đổi từ lúa chuyên canh sang lúa tôm cao hơn hộ trồng lúa trong điều kiện không xâm nhập mặn là 13,8 điểm phần trăm.</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1652,24 +1642,25 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query, but it does not provide a definitive answer to the question. It is possible that the information is not available in the research paper, but without a reference answer or the actual paper, it's hard to confirm the correctness of the response.</t>
+          <t>The generated answer is relevant to the user query and provides specific information about the correlation between saltwater intrusion and the probability of conversion from specialized rice cultivation to rice-shrimp farming. However, without a reference answer, it's hard to verify the correctness of the specific percentages provided.</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>According to the document, what are the significant variables that explain the probability of transitioning from specialized rice cultivation to a rice-shrimp model? How do land area and salinity intrusion influence this transition?</t>
+          <t>Liệt kê các biến có ý nghĩa giải thích cho xác suất chuyển đổi mô hình từ chuyên canh lúa sang lúa – màu theo nghiên cứu. Trình bày cách mà diện tích đất và xâm nhập mặn ảnh hưởng đến quyết định chuyển đổi mô hình canh tác.</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>The document does not provide specific information on the significant variables that explain the probability of transitioning from specialized rice cultivation to a rice-shrimp model, nor does it detail how land area and salinity intrusion influence this transition.</t>
+          <t>Các biến có ý nghĩa giải thích cho xác suất chuyển đổi mô hình từ chuyên canh lúa sang lúa – màu bao gồm: diện tích đất, tuổi chủ hộ, học vấn cấp 1, học vấn cấp 2, và nguồn nước.
+Diện tích đất và xâm nhập mặn đều ảnh hưởng đến xác suất chuyển đổi từ mô hình chuyên canh lúa sang mô hình lúa kết hợp. Những hộ có diện tích sản xuất lớn thường thực hiện chuyển đổi sang mô hình lúa – tôm nhiều hơn, do yêu cầu về diện tích canh tác và nguồn vốn đầu tư để chuyển đổi sang mô hình tôm – lúa. Trong khi đó, hộ trồng lúa càng có diện tích đất sản xuất ít, sẽ không đủ điều kiện tạo ra thu nhập cho gia đình ổn định và nguồn lực để chuyển đổi để có thể chuyển đổi cơ cấu sản xuất nhằm tạo ra thu nhập cao hơn trong tương lai.</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1679,46 +1670,46 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query, but it's not possible to determine its correctness without a reference answer or the original document. The answer is also somewhat vague, stating that the document doesn't provide the requested information without offering any additional details or context.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the variables that influence the probability of transitioning from rice cultivation to a rice-shrimp model. It also explains how land area and saltwater intrusion affect this decision. However, it does not fully explain how saltwater intrusion specifically impacts the decision, which is why it does not receive a perfect score.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>What are the key factors that influence the probability of transitioning from specialized rice farming to the rice-shrimp model, as identified in the research paper "Nghiên cứu vận hành công trình thủy lợi trong điều kiện xâm nhập mặn: trường hợp nghiên cứu tại huyện vũng liêm, tỉnh vĩnh long" by Lavane et al.?</t>
+          <t>Theo nghiên cứu, yếu tố nào quan trọng nhất tác động trực tiếp đến quyết định chuyển đổi mô hình sản xuất từ lúa chuyên canh sang lúa tôm và lúa cá?</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>The context does not provide information on the key factors that influence the probability of transitioning from specialized rice farming to the rice-shrimp model as identified in the research paper "Nghiên cứu vận hành công trình thủy lợi trong điều kiện xâm nhập mặn: trường hợp nghiên cứu tại huyện vũng liêm, tỉnh vĩnh long" by Lavane et al.</t>
+          <t>Yếu tố quan trọng nhất tác động trực tiếp đến quyết định chuyển đổi mô hình sản xuất từ lúa chuyên canh sang lúa tôm và lúa cá là xâm nhập mặn và diện tích đất.</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the topic of the research paper mentioned. However, it does not provide any specific factors that influence the transition from specialized rice farming to the rice-shrimp model, which is what the user asked for. Therefore, it is not fully correct.</t>
+          <t>The generated answer is relevant and seems correct, providing specific factors that could influence the decision to switch from specialized rice cultivation to shrimp and fish rice. However, without a reference answer, it's hard to confirm the absolute correctness of the response.</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>According to the same research, how do land area and salinity intrusion affect the trend of transitioning to the rice-shrimp or rice-fish model? What contradictions in economic benefits of these models are suggested in the context of salinity intrusion in the region?</t>
+          <t>Theo kết quả nghiên cứu, diện tích đất và nhiễm mặn có ảnh hưởng như thế nào đến xu hướng chuyển đổi sang mô hình lúa – tôm hoặc lúa – cá?</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on how land area and salinity intrusion affect the trend of transitioning to the rice-shrimp or rice-fish model. Similarly, it does not mention any contradictions in economic benefits of these models in the context of salinity intrusion in the region.</t>
+          <t>Diện tích đất và nhiễm mặn có ảnh hưởng trái ngược nhau đối với xu hướng chuyển đổi sang mô hình lúa – tôm hoặc lúa – cá. Cụ thể, diện tích đất lớn thường thúc đẩy xu hướng chuyển đổi sang mô hình lúa – tôm, do yêu cầu về diện tích canh tác và nguồn vốn đầu tư để chuyển đổi sang mô hình này. Ngược lại, nếu diện tích đất sản xuất ít, hộ sẽ không đủ điều kiện tạo ra thu nhập ổn định cho gia đình và nguồn lực để chuyển đổi, do đó hạn chế xu hướng chuyển đổi. Trong khi đó, nhiễm mặn có ảnh hưởng đến xu hướng chuyển đổi mô hình canh tác, nhưng không rõ ràng ảnh hưởng đến xu hướng chuyển đổi sang mô hình lúa – màu.</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1733,19 +1724,19 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information or answer to the user's query. It simply states that the context does not provide the necessary information, which is not helpful or relevant to the user's question.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how land area and salinity affect the trend of transitioning to rice-shrimp or rice-fish farming models. However, there is a minor mistake in the last sentence where it mentions "rice-color" model which seems to be a mistranslation or typo.</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Based on the research paper, what were the two conditions under which the Nang Am sluice-gate was operated from 2015-2021?</t>
+          <t>Trình bày các điều kiện đã được đặt ra để vận hành cống Nàng Âm trong giai đoạn 2015-2021 trong nghiên cứu về vận hành công trình thủy lợi trong điều kiện xâm nhập mặn tại huyện Vũng Liêm, tỉnh Vĩnh Long?</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>The Nang Am sluice-gate was operated from 2015-2021 under two conditions: the water level and the salinity, with a salinity threshold of 1 g/L.</t>
+          <t>Cống Nàng Âm được vận hành trong giai đoạn 2015-2021 dựa trên hai điều kiện chính. Đầu tiên là mực nước, và thứ hai là độ mặn, với ngưỡng mặn được đặt ở 1 g/L.</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1760,46 +1751,47 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and seems to be correct, providing specific conditions under which the Nang Am sluice-gate was operated. However, without a reference answer, it's hard to confirm the absolute correctness of the information.</t>
+          <t>The generated answer is relevant to the user query and seems to be correct, providing two main conditions for the operation of the Nàng Âm culvert during the period 2015-2021. However, without a reference answer, it's hard to confirm the full accuracy.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>According to the climate change scenarios of the Ministry of Natural Resources and Environment (2016), how do the predicted water levels in 2030 and 2050 under the three scenarios RCP2.6, RCP4.5 and RCP 8.5 compare to the dike-crest elevation?</t>
+          <t>Theo kết quả nghiên cứu, hãy so sánh mực nước trạm Mỹ Thuận hiện tại với mực nước dự báo năm 2030 và 2050 theo ba kịch bản RCP2.6, RCP4.5 và RCP 8.5.</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>The context does not provide information on the comparison of predicted water levels in 2030 and 2050 under the three scenarios RCP2.6, RCP4.5, and RCP 8.5 to the dike-crest elevation according to the climate change scenarios of the Ministry of Natural Resources and Environment (2016).</t>
+          <t>Rất tiếc, nhưng thông tin cung cấp không đưa ra dữ liệu cụ thể về mực nước trạm Mỹ Thuận hiện tại so với mực nước dự báo năm 2030 và 2050 theo ba kịch bản RCP2.6, RCP4.5 và RCP 8.5.</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and does not contain any factual errors. However, it does not provide a direct answer to the question, instead stating that the necessary information is not available.</t>
+          <t>The generated answer is relevant to the user query as it addresses the comparison of water levels at My Thuan station. However, it does not provide the specific information requested, hence it's not fully correct.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Based on the research conducted in Vũng Liêm, Vĩnh Long, what are the current conditions of the irrigation system and how does it relate to the operation of the sluice gates during the dry season under saline intrusion conditions?</t>
+          <t>Hãy mô tả hiện trạng thủy lợi tại huyện Vũng Liêm, tỉnh Vĩnh Long và giải thích tại sao hệ thống đê cần được nâng cấp?</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>The irrigation system in Vũng Liêm, Vĩnh Long was digitised using QGIS and the dyke elevations were evaluated based on the water level of the My Thuan station, as predicted from climate change scenarios. The Nang Am sluice-gate was chosen for operation from 2015 to 2021 under two conditions: water level and salinity, with a salinity threshold of 1 g/L. The results indicated that the current water level of the My Thuan station, with a frequency of 3%, 5%, and 10%, is lower than the dike-crest elevation (+2.20 m). However, the projected water levels for 2030 and 2050 under three scenarios (RCP2.6, RCP4.5, and RCP 8.5) are higher than the dike-crest elevation. In years with high salinity, such as 2016, 2020, and 2021, the sluice gate was closed for over 25% of the time during the dry months.</t>
+          <t>Hiện trạng công trình thủy lợi tại huyện Vũng Liêm, tỉnh Vĩnh Long đã được số hóa bằng QGIS và các cao trình đê bao được đánh giá theo mực nước trạm Mỹ Thuận dự báo từ các kịch bản biến đổi khí hậu. Cống Nàng Âm được chọn để vận hành theo điều kiện mực nước và độ mặn. Mực nước trạm Mỹ Thuận hiện tại với tần suất 3%, 5% và 10% thấp hơn cao trình đỉnh đê (+2,20 m). Tuy nhiên, mực nước tương ứng năm 2030 và 2050 theo ba kịch bản RCP2.6, RCP4.5 và RCP 8.5 đều cao hơn cao trình đỉnh đê. Trong những năm có độ mặn cao như 2016, 2020 và 2021 thì thời gian đóng cống trong các tháng mùa khô là trên 25%.
+Hệ thống đê cần được nâng cấp vì mực nước dự báo trong tương lai theo các kịch bản biến đổi khí hậu sẽ cao hơn cao trình đỉnh đê. Điều này có thể gây ra nguy cơ ngập lụt, đặc biệt trong bối cảnh biến đổi khí hậu và xâm nhập mặn ngày càng nghiêm trọng.</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1814,23 +1806,19 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the current conditions of the irrigation system in Vũng Liêm, Vĩnh Long. It also explains how the operation of the sluice gates during the dry season is affected by saline intrusion conditions. The answer is comprehensive and appears to be accurate, although without a reference answer, it's not possible to confirm every detail. The score is not a perfect 5 due to the lack of a reference answer for complete verification.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed description of the current state of irrigation in Vũng Liêm district, Vĩnh Long province. It also explains why the dike system needs to be upgraded, citing future water level predictions and climate change scenarios. The answer is accurate and comprehensive, but it could be slightly more concise.</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>In the paper titled "Quản lý tài nguyên nước bền vững, ứng phó với biến đổi khí hậu ở Đồng bằng sông Cửu Long" by PGS. TS Lê Anh Tuấn, what are the key challenges faced by the Mekong Delta and what are the key findings from the various technical reports related to water resource management and climate change adaptation?</t>
+          <t>Theo bài viết "Quản lý tài nguyên nước bền vững, ứng phó với biến đổi khí hậu ở Đồng bằng sông Cửu Long" của PGS. TS Lê Anh Tuấn, ĐBSCL đang đối mặt với những vấn đề gì và Thủ tướng Nguyễn Xuân Phúc đã có những hành động nào để giải quyết những vấn đề này?</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>The Mekong Delta faces several key challenges, including salinity intrusion, freshwater scarcity, and ebb tide influences, which have been increasing in recent years. These hazards have a direct impact on production and the livelihoods of the local people. Other challenges include unpredictable weather changes, market price fluctuations, environmental pollution, and shrimp diseases, which further complicate production.
-To cope with these hazards, the local government and people have developed strategies such as dyke building, farming technical changes, financial support for production recovery from disasters, underground water exploitation, and income diversification. However, these adaptation options have limitations as they do not fully consider the differences in ecological, social, and economic environments. The vulnerability of people highly depends on these conditions.
-In terms of water resource management, the planning in the Mekong Delta is quite "top-down", with villagers and farmers playing a minor role. The water control infrastructure systems suffer from many shortcomings and challenges in terms of both their structure and management. There are two water quantity problems and three main water quality problems that limit agricultural production: Salinity intrusion, floods, acid sulfate soils, polluted water, and fresh water shortages.
-Regarding floods, the Mekong Delta, due to its location, receives the total volume of floodwaters from upstream. About 50 percent of the Mekong Delta experiences flooding, and these areas are susceptible to serious damage by floods about every five years. Major flooding is now likely to occur even more frequently than the “once in two or three years” average. High floods result in loss of life and cause millions of dollars worth of damage to houses, infrastructure, and crops. However, floods are also perceived by many farmers and scientists not only as a “disaster” but also as a natural phenomenon that brings multiple replenishing and revitalizing benefits.
-The paper suggests that future adaptation strategies should take into account the above issues in order to benefit different social groups, especially the most vulnerable.</t>
+          <t>Đồng bằng sông Cửu Long (ĐBSCL) đang đối mặt với nhiều vấn đề như tranh chấp nước giữa các địa phương sử dụng chung hệ thống thủy lợi, tình trạng biến đổi khí hậu và xâm nhập mặn cực đoan, mất diện tích tưới tiêu do úng, nhiễm mặn, khai thác quá tải nước ngầm và sự phát triển của đô thị. Để giải quyết những vấn đề này, Thủ tướng Chính phủ đã ký Quyết định số 417/QĐ-TTg về việc ban hành Chương trình hành động tổng thể thực hiện Nghị quyết số 120/NQ-CP về phát triển bền vững ĐBSCL thích ứng với biến đổi khí hậu. Chương trình này đề ra 6 nhóm nhiệm vụ và giải pháp cụ thể chính, bao gồm rà soát, hoàn thiện và bổ sung hệ thống cơ chế, chính sách, cập nhật và hệ thống hóa số liệu, dữ liệu liên ngành, xây dựng quy hoạch và tổ chức không gian lãnh thổ, xây dựng cơ cấu kinh tế hợp lý thích ứng với biến đổi khí hậu, đầu tư và phát triển hạ tầng, và phát triển và huy động nguồn lực.</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1845,20 +1833,19 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive overview of the key challenges faced by the Mekong Delta as well as the findings from technical reports related to water resource management and climate change adaptation. The answer could be slightly more concise, hence the score is not a perfect 5.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the issues facing the Mekong Delta and the actions taken by Prime Minister Nguyen Xuan Phuc to address these issues. The answer could be improved by providing more specific examples or details about the actions taken.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Based on the text, what are the two main impacts on the flow in the Mekong Delta region, and how do they affect the region during different times of the year?</t>
+          <t>Hãy mô tả hai tác động dòng chảy mà Đồng bằng sông Cửu Long đang chịu và thời gian diễn ra của chúng trong năm?</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>The two main impacts on the flow in the Mekong Delta region are flooding and salinity intrusion. Flooding is a significant issue, particularly during the yearly September-October flood period, known locally as mùa nước nổi (water rising season). This flooding can cause loss of life and significant damage to houses, infrastructure, and crops. However, it also brings benefits such as fertile sediment, fish spawning, and improved water quality. 
-On the other hand, salinity intrusion, which is particularly prevalent from March to May, occurs when not enough river discharge is flowing to the low-lying estuaries, allowing salt water to flow into the land. This intrusion can restrict the use of canal water for domestic and industrial uses, cause corrosion of metal materials, and make vegetables and other crops scarce in the affected areas. However, it also has some positive effects, such as reducing acidity in potential acid sulphate soil land and enabling farmers to implement a more varied production scheme to raise shrimp during the dry season.</t>
+          <t>Đồng bằng sông Cửu Long đang chịu hai tác động dòng chảy. Một là dòng chảy của sông Mekong từ thượng nguồn đổ về. Thứ hai là dòng triều do tác động biển xâm nhập vào đất liền. Thời gian bị ngập lũ, thường do dòng chảy của sông Mekong, diễn ra từ tháng 8 đến tháng 10. Trong khi đó, từ tháng 1 đến tháng 4 là thời gian bị tác động mạnh mẽ của hiện tượng xâm nhập mặn và khô hạn, thường do dòng triều biển.</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1873,19 +1860,19 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate explanation of the two main impacts on the flow in the Mekong Delta region, including how they affect the region during different times of the year. It also provides additional context and details that enhance the understanding of the topic.</t>
+          <t>The generated answer is relevant and accurate. It correctly describes the two types of water flow impacts that the Mekong Delta is experiencing and the time of year they occur. The only reason it doesn't get a perfect score is because it could be a bit more detailed in describing the impacts of these phenomena.</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>According to the mathematical models mentioned in the text, what changes are predicted for the Mekong Delta region in terms of average temperature and rainfall in the next 30 years, and how might these changes affect agriculture in the region?</t>
+          <t>Theo kết quả phỏng đoán từ các mô hình toán, hãy nêu những thay đổi về nhiệt độ và lượng mưa trung bình dự kiến sẽ xảy ra trong thập niên 2030-2040 ở Đồng bằng sông Cửu Long?</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>The text does not provide specific information on the predicted changes in average temperature and rainfall in the Mekong Delta region over the next 30 years according to mathematical models, nor does it discuss how such changes might affect agriculture in the region.</t>
+          <t>Trong thập kỷ 2030-2040, nhiệt độ trung bình cũng như nhiệt độ lớn nhất và nhỏ nhất tại Đồng bằng sông Cửu Long dự kiến sẽ tăng, với mức tăng phổ biến khoảng 20˚C. Đồng thời, tổng lượng mưa trung bình trong khu vực này cũng dự đoán sẽ giảm, phổ biến từ 10 đến 20%, làm tăng khó khăn trong việc cung cấp nước ngọt cho canh tác lúa.</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1900,19 +1887,19 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and it is correct in stating that the text does not provide the specific information asked for. However, it could have been more helpful by suggesting where such information might be found or by providing general information on the effects of temperature and rainfall changes on agriculture.</t>
+          <t>The generated answer is relevant to the user query and provides a detailed prediction for the changes in temperature and rainfall in the Mekong Delta region for the decade 2030-2040. However, the prediction of a 20˚C increase in temperature seems a bit extreme and might be a mistake.</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>What are the potential impacts of global warming and rising sea levels on low-lying coastal areas, specifically in the Mekong Delta region, as discussed in the document "researched_paper_cleanup.txt"?</t>
+          <t>Theo Ủy ban Liên chính phủ về BĐKH, vùng nào là một trong ba vùng đồng bằng ven biển sẽ bị tác động nghiêm trọng nhất do BĐKH và nước biển dâng so với các nơi khác trên thế giới?</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>The document does not provide specific information on the impacts of global warming and rising sea levels on low-lying coastal areas, particularly in the Mekong Delta region.</t>
+          <t>Vùng ĐBSCL là một trong ba vùng đồng bằng ven biển sẽ bị tác động nghiêm trọng nhất do BĐKH và nước biển dâng so với các nơi khác trên thế giới, theo Ủy ban Liên chính phủ về BĐKH.</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1927,21 +1914,19 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the topic of global warming and rising sea levels' impact on the Mekong Delta region. However, it does not provide any specific information or details, which makes it impossible to judge its correctness.</t>
+          <t>The generated answer is relevant and correct, providing the information that the Mekong Delta (ĐBSCL) is one of the three coastal plains most severely affected by climate change and sea level rise, according to the Intergovernmental Panel on Climate Change (Ủy ban Liên chính phủ về BĐKH). The answer could be slightly more detailed, hence the score is not a full 5.</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>According to the document, what are the dual impacts that the delta region is facing, and how do industrial and agricultural activities in the region contribute to these impacts?</t>
+          <t>Theo dự đoán, nếu không kiểm soát được hiện tượng nóng lên toàn cầu, hậu quả nào có thể xảy ra đối với các vùng đất thấp ven biển ĐBSCL vào cuối thế kỷ XXI?</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>The delta region is facing the dual impacts of floods and salinity intrusion. Floods occur when excess water upstream flows over river banks or dykes to the floodplain, and they can cause prolonged deep inundation, river bank erosion, and transportation difficulties. However, they also have multiple replenishing and revitalizing benefits such as providing fertile sediment, aiding fish spawning, improving water quality, and reducing fire risk. 
-On the other hand, salinity intrusion occurs when not enough river discharge is flowing to the low-lying estuaries and instead salt water flows into the land. This can damage crops, restrict the use of canal water for domestic and industrial uses, and cause corrosion of metal materials. However, it also has a positive effect of reducing acidity in potential acid sulphate soil land and enabling farmers to implement a more varied production scheme to raise shrimp during the dry season.
-Industrial and agricultural activities in the region contribute to these impacts in several ways. For instance, the construction of dams, climate change, and water poor quality are some of the anthropogenic stressors that endanger the Lower Mekong River. Additionally, water resources planning in the Mekong Delta is quite "top-down", with villagers and farmers playing a very minor role in water planning and natural prevention projection processes. This could potentially exacerbate the impacts of floods and salinity intrusion.</t>
+          <t>Nếu không kiểm soát được hiện tượng nóng lên toàn cầu, vào cuối thế kỷ XXI, có thể sẽ có ít nhất 25% diện tích các vùng đất thấp ven biển ĐBSCL có nguy cơ bị chìm ngập do nước biển dâng và lún sụt đồng bằng. Khoảng 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn vào mùa khô và khoảng 30-40% diện tích nông nghiệp bị ảnh hưởng của nước mặn ngay cả trong mùa mưa, khó có thể trồng lúa và một số canh tác khác như chăn nuôi được.</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1956,19 +1941,25 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive and detailed explanation of the dual impacts that the delta region is facing, as well as how industrial and agricultural activities contribute to these impacts. The answer is well-structured, clear, and appears to be fully correct, with no mistakes or inaccuracies evident.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed prediction of the potential consequences of global warming on low-lying coastal areas in the Mekong Delta by the end of the 21st century. It includes specific percentages and impacts on agriculture, which adds to its correctness. However, without a reference answer, it's hard to confirm the exact accuracy of these figures, hence the score is not a perfect 5.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>What are the six specific tasks and solutions proposed in the comprehensive action program to implement Resolution 120/NQ-CP on sustainable development, as issued by the Vietnamese government?</t>
+          <t>Hãy liệt kê 6 nhóm nhiệm vụ và giải pháp cụ thể chính được đề ra trong Chương trình hành động tổng thể thực hiện Nghị quyết số 120/NQ-CP về phát triển bền vững ĐBSCL thích ứng BĐKH.</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>The six specific tasks and solutions proposed in the comprehensive action program to implement Resolution 120/NQ-CP on sustainable development are: (1) Reviewing, perfecting and supplementing the system of mechanisms and policies; (2) Updating and systematizing cross-sectoral data, enhancing basic surveys; (3) Developing planning and organizing territorial space; (4) Building an appropriate economic structure adapted to climate change; (5) Investing and developing infrastructure; (6) Developing and mobilizing resources.</t>
+          <t>Sáu nhóm nhiệm vụ và giải pháp cụ thể chính được đề ra trong Chương trình hành động tổng thể thực hiện Nghị quyết số 120/NQ-CP về phát triển bền vững ĐBSCL thích ứng BĐKH bao gồm: 
+1. Rà soát, hoàn thiện và bổ sung hệ thống cơ chế, chính sách.
+2. Cập nhật và hệ thống hóa số liệu, dữ liệu liên ngành, tăng cường điều tra cơ bản.
+3. Xây dựng quy hoạch và tổ chức không gian lãnh thổ.
+4. Xây dựng cơ cấu kinh tế hợp lý thích ứng với BĐKH.
+5. Đầu tư và phát triển hạ tầng.
+6. Phát triển và huy động nguồn lực.</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1983,19 +1974,19 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate response to the question asked. It lists all six tasks and solutions proposed in the comprehensive action program to implement Resolution 120/NQ-CP on sustainable development, as issued by the Vietnamese government.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and correct response. It lists the six main tasks and solutions proposed in the overall action program to implement Resolution No. 120/NQ-CP on sustainable development of the Mekong Delta in response to climate change, which is exactly what the user asked for.</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>What are the priority issues to be addressed by 2020 according to Resolution 120/NQ-CP, and how does it plan to deal with the rapid and increasingly serious issues of coastal erosion, riverbank erosion, and land subsidence?</t>
+          <t>Trong giai đoạn từ nay đến năm 2020, vấn đề nào được ưu tiên giải quyết theo Nghị quyết 120?</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>The priority issues to be addressed by 2020 according to Resolution 120/NQ-CP include the rapid and increasingly serious issues of coastal erosion, riverbank erosion, and land subsidence. The plan to deal with these issues involves implementing urgent tasks outlined in the resolution. This includes prioritizing the resolution of coastal and riverbank erosion and land subsidence, which are occurring at a rapid pace. Additionally, the plan involves deploying planning and designing large-scale investment projects for the next phase to implement the region's socio-economic model in a sustainable and proactive manner that adapts to climate change.</t>
+          <t>Vấn đề được ưu tiên giải quyết theo Nghị quyết 120 trong giai đoạn từ nay đến năm 2020 là sạt lở bờ biển, bờ sông, rạch và sụt lún đất trong vùng đang diễn ra rất nhanh và ngày càng trầm trọng.</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2010,19 +2001,19 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and appears to be correct, providing a detailed response to the user's query about the priority issues addressed by Resolution 120/NQ-CP and the plan to deal with coastal erosion, riverbank erosion, and land subsidence. However, without a reference answer, it's difficult to confirm the complete accuracy of the information.</t>
+          <t>The generated answer is relevant and appears to be fully correct, providing specific details about the issues prioritized by Resolution 120 from now until 2020.</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Based on the text, what challenges have been identified in the implementation of Resolution 120, and how have these affected the involvement of organizations, businesses, and individuals?</t>
+          <t>Theo nội dung trong đoạn văn, hãy nêu những khó khăn mà các địa phương đang gặp phải trong việc hiểu và triển khai Nghị quyết 120?</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>The implementation of Resolution 120 has faced several challenges. Understanding and applying the resolution in practice has been difficult, with many localities not fully innovating in line with the spirit of the resolution. Instead, they rely on guidance and support resources from the central government. The approach based on internal strength has not been emphasized, and there has been a lack of widespread participation from organizations, businesses, and individuals. Additionally, the completion of the institutional framework and policies to carry out tasks according to Resolution 120 has been slow, especially policies to promote the development of key sectors and fields. Some policies have been issued but have not been integrated into daily life due to a lack of synchronization with implementation resources. There is also a lack of regulations on coordination mechanisms and information sharing among relevant agencies. Particularly, the mindset of prioritizing the selection of construction solutions at all levels/sectors is still more prevalent than choosing non-construction solutions. These challenges have hindered the active involvement of organizations, businesses, and individuals in the implementation of the resolution.</t>
+          <t>Các địa phương đang gặp phải nhiều khó khăn trong việc hiểu và triển khai Nghị quyết 120. Một số vấn đề bao gồm việc chưa thực sự đổi mới theo tinh thần Nghị quyết, còn trông chờ vào hướng dẫn và nguồn lực hỗ trợ từ Trung ương. Cách tiếp cận dựa vào nội lực chưa được đề cao, chưa huy động được sự tham gia rộng rãi của các tổ chức, doanh nghiệp, người dân. Việc hoàn thiện thể chế, chính sách triển khai thực hiện các nhiệm vụ theo Nghị quyết 120 vẫn còn chậm, nhất là các chính sách đẩy mạnh phát triển các ngành, lĩnh vực then chốt. Một số chính sách đã được ban hành nhưng chưa đi vào cuộc sống vì chưa đồng bộ với nguồn lực thực hiện; còn thiếu quy định về cơ chế phối hợp, chia sẻ thông tin giữa các cơ quan liên quan. Đặc biệt, tư duy ưu tiên lựa chọn giải pháp công trình ở các cấp/ngành vằn nhiều hơn là các chọn lựa giải pháp phi công trình.</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2032,26 +2023,24 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the challenges faced in the implementation of Resolution 120. It also clearly outlines how these challenges have affected the involvement of organizations, businesses, and individuals. The answer is comprehensive and appears to be correct, even without a reference answer for comparison.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the difficulties localities are facing in understanding and implementing Resolution 120. It does not contain any mistakes or inaccuracies.</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Discuss the issues related to policy synchronization and information sharing among related agencies as mentioned in the text. How do these issues impact the selection of solutions for projects?</t>
+          <t>Theo ngữ cảnh đã cho, hãy phân tích và giải thích vì sao việc hoàn thiện thể chế, chính sách triển khai thực hiện các nhiệm vụ theo Nghị quyết 120 lại diễn ra chậm?</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>The text indicates that there are significant issues related to policy synchronization and information sharing among related agencies. The implementation of Resolution 120, for instance, has been problematic, with many localities not innovating in line with the resolution's spirit and instead waiting for guidance and support from the central government. The approach based on internal strength has not been emphasized, and the widespread participation of organizations, businesses, and people has not been mobilized. 
-Moreover, the perfection of mechanisms and policies to carry out tasks according to Resolution 120 has been slow, especially policies to promote the development of key sectors and fields. Some policies have been issued but have not been integrated into life because they are not synchronized with the resources for implementation. There is a lack of regulations on the coordination mechanism and information sharing among related agencies.
-These issues have a significant impact on the selection of solutions for projects. The text suggests that there is a prevailing mindset of prioritizing the selection of construction solutions over non-construction solutions. This could be due to the lack of coordination and information sharing, which may limit the understanding of the full range of possible solutions and their potential impacts.</t>
+          <t>Việc hoàn thiện thể chế, chính sách triển khai thực hiện các nhiệm vụ theo Nghị quyết 120 diễn ra chậm do một số lý do. Đầu tiên, nhiều địa phương chưa thực sự đổi mới theo tinh thần Nghị quyết và vẫn đang chờ đợi hướng dẫn và nguồn lực hỗ trợ từ Trung ương. Thứ hai, cách tiếp cận dựa vào nội lực chưa được đề cao, chưa huy động được sự tham gia rộng rãi của các tổ chức, doanh nghiệp, người dân. Thứ ba, một số chính sách đã được ban hành nhưng chưa đi vào cuộc sống vì chưa đồng bộ với nguồn lực thực hiện. Cuối cùng, còn thiếu quy định về cơ chế phối hợp, chia sẻ thông tin giữa các cơ quan liên quan.</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2066,22 +2055,20 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed discussion on the issues related to policy synchronization and information sharing among related agencies. It also explains how these issues impact the selection of solutions for projects. The answer could be slightly more specific in terms of the impact on project solution selection, hence the score is not a perfect 5.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of why the implementation of tasks according to Resolution 120 is slow. It lists several reasons, including lack of innovation in localities, lack of internal resources, policies not being implemented effectively, and lack of coordination among relevant agencies. The answer is comprehensive and correct, hence the perfect score.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Based on the research paper "The Salinization of Agricultural Hubs: Impacts and Adjustments to Intensifying Saltwater Intrusion in the Mekong Delta", what are the observed effects of salinization on rice production, land use, labor supply, and household income in the Mekong Delta region?</t>
+          <t>Theo bài viết, tác giả đề xuất những giải pháp nào để thực hiện ý kiến chỉ đạo của Thủ tướng về việc thích ứng với tình hình mặn hóa ở Đồng bằng sông Cửu Long?</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>The research paper outlines several effects of salinization in the Mekong Delta region. For agricultural production, higher salinity decreases the productivity and revenue share of rice crops, as well as aquaculture production. However, it increases the revenue share of industrial crops, such as coconut, which is a salt-resistant crop. 
-In terms of land use, higher salinity intrusion is associated with decreases in farmers’ land used for rice and their general land used for agriculture. 
-Regarding labor supply, salinity shock is estimated to decrease labor supply in agriculture for those without agricultural land, but labor supply for those with agricultural land does not respond to higher salinity.
-Finally, salinization is found to reduce farmer households’ income and consumption. However, it seems to increase household spending on education, potentially indicating farmers’ increased investment to acquire new skills.</t>
+          <t>Tác giả đề xuất một số giải pháp để thích ứng với tình hình mặn hóa ở Đồng bằng sông Cửu Long. Đầu tiên, họ đề cử việc vận hành thông minh hệ thống thủy lợi liên tỉnh dựa trên nền tảng công nghệ Internet of Things (IoT) để nâng cao năng suất nước và bảo vệ môi trường sinh thái. Thứ hai, họ khuyến nghị tăng hiệu quả sử dụng tài nguyên đất và nước thông qua các giải pháp nâng cao hiệu quả quản lý khai thác các công trình thuỷ lợi. 
+Ngoài ra, tác giả cũng đề cử một số chiến lược khác như xây dựng đê bao, thay đổi biện pháp canh tác, chính sách hỗ trợ khắc phục sản xuất, khai thác nguồn nước ngầm và đa dạng hóa nguồn thu nhập. Tuy nhiên, tác giả cũng nhấn mạnh rằng các chương trình thích ứng trong tương lai cần phải xây dựng trên cơ sở nhu cầu và năng lực của cộng đồng.</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2096,19 +2083,19 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and appears to be fully correct. It provides detailed information on the effects of salinization on rice production, land use, labor supply, and household income in the Mekong Delta region, as requested by the user.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and comprehensive response to the question about the author's proposed solutions to adapt to the salinization situation in the Mekong Delta. The answer is correct and complete, covering various strategies and emphasizing the need for future adaptation programs to be based on community needs and capabilities.</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>In the context of the Vietnamese Mekong Delta, discuss the role of credit access and labor migration to urban areas as potential adaptation mechanisms in response to the challenges posed by salinization. Provide evidence from the research paper to support your answer.</t>
+          <t>Trong bài nghiên cứu "The Salinization of Agricultural Hubs: Impacts and Adjustments to Intensifying Saltwater Intrusion in the Mekong Delta", tác giả đã chỉ ra những tác động nào của mặn hóa đối với sản xuất nông nghiệp, quyết định lao động và phúc lợi của các hộ nông dân ở Đồng bằng sông Cửu Long?</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>The research paper discusses two potential adaptation mechanisms in response to salinization in the Vietnamese Mekong Delta: credit access and labor migration to urban areas. The evidence on labor migration for off-farm work in urban centers is mixed, suggesting that it may not be a consistent or reliable adaptation strategy for all farmers affected by salinization. On the other hand, the study supports the hypothesis that a more developed local credit market plays a positive role in easing the income losses incurred by farmers during salinization shocks. This suggests that access to credit can provide farmers with the financial resources needed to adapt their farming practices or invest in new, more salt-resistant crops.</t>
+          <t>Tác giả đã chỉ ra rằng mặn hóa có ảnh hưởng tiêu cực đáng kể đến sản xuất lúa, làm giảm diện tích đất sử dụng và một phần nguồn cung lao động trong nông nghiệp. Mặn hóa cũng được cho là làm tăng sản xuất các loại cây công nghiệp chịu mặn. Trong khi ảnh hưởng đến thu nhập và tiêu dùng của hộ gia đình là tiêu cực, tác giả cũng chỉ ra rằng có dấu hiệu cho thấy việc tăng chi tiêu cho giáo dục như một phản ứng trước những cú sốc do mặn hóa. Đối với các biện pháp thích ứng, tác giả tìm thấy bằng chứng không rõ ràng về việc di cư lao động đến các khu vực đô thị để làm việc ngoài nông nghiệp và có dấu hiệu cho thấy vai trò của việc tiếp cận tín dụng trong việc giảm thiểu mất mát thu nhập của nông dân.</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2123,24 +2110,22 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the role of credit access and labor migration as potential adaptation mechanisms in response to salinization in the Vietnamese Mekong Delta. It also provides evidence from the research paper to support its points. However, it could have been more specific about the evidence from the research paper.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impacts of salinization on agricultural production, labor decisions, and the welfare of farming households in the Mekong Delta, as outlined in the research paper. The answer could be slightly more concise, hence the score is not a perfect 5.</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Based on the research conducted on the Vietnamese Mekong delta, explain how salinization impacts agricultural production, labor decisions, and the welfare of farmer households. Discuss the five main results of the analysis in detail.</t>
+          <t>Hãy mô tả ảnh hưởng của sự mặn hóa đối với sản xuất nông nghiệp, quyết định lao động và phúc lợi của các hộ nông dân ở đồng bằng sông Cửu Long, Việt Nam theo nghiên cứu này. Đặc biệt, hãy nêu rõ về sự thay đổi trong sản xuất và sử dụng đất nông nghiệp, cung cấp lao động, thu nhập và tiêu dùng của hộ nông dân, cũng như các kênh thích ứng như di cư và tiếp cận tín dụng.</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Salinization has a significant impact on agricultural production, labor decisions, and the welfare of farmer households in the Vietnamese Mekong delta. The analysis of these impacts yielded five main results.
-Firstly, in terms of agricultural production, higher salinity was found to decrease the productivity and revenue share of rice crops, which is a significant concern given that the Mekong delta contributes to over 90% of national rice exports. Higher salinity also decreases aquaculture production. However, it increases the revenue share of industrial crops, particularly coconut, which is a salt-resistant crop. This suggests that farmers may be adopting new crops or switching crops as a risk diversification strategy to secure their income against salinization shocks.
-Secondly, higher salinity intrusion was associated with decreases in farmers’ land used for rice and their general land used for agriculture. This suggests that salinization may be leading to a reduction in agricultural land use.
-Thirdly, salinization was found to affect labor supply. While salinity shock was estimated to decrease labor supply in agriculture for those without agricultural land, labor supply for those with agricultural land did not respond to higher salinity. This indicates that salinization may be influencing labor decisions in the agricultural sector.
-Fourthly, salinization was found to reduce farmer households’ income and consumption, indicating a negative impact on their welfare. However, the estimated effect on household spending on education was positive, which could imply that farmers are investing more in acquiring new skills in response to the challenges posed by salinization.
-Lastly, the study tested two channels for adaptation smoothing: migration and credit access. The evidence on out-migration for off-farm work in urban centers was mixed, but the results supported the hypothesis that a more developed local credit market plays a positive role in easing the income losses incurred by farmers during salinization shocks. This suggests that financial mechanisms may be an important part of the response to salinization.</t>
+          <t>Sự mặn hóa có ảnh hưởng lớn đến sản xuất nông nghiệp, quyết định lao động và phúc lợi của các hộ nông dân ở đồng bằng sông Cửu Long, Việt Nam. Cụ thể, thu nhập từ hoạt động nuôi trồng và đánh bắt thủy sản có thể cao hơn so với hoạt động nông nghiệp, nhưng rủi ro cũng rất cao. Có nhiều hộ gia đình làm giàu nhờ hoạt động này, nhưng cũng có không ít hộ gia đình trắng tay sau những lần rủi ro.
+Những người có kinh nghiệm sản xuất trên 10 năm thường có thu nhập từ khá trở lên, trong khi những người có kinh nghiệm sản xuất dưới 10 năm thường có thu nhập từ trung bình trở xuống. Khi người dân có kinh nghiệm trong sản xuất, họ có thể chủ động thích ứng với hạn mặn và thông qua những thất bại trước đó, họ có thể rút ra kinh nghiệm sản xuất tốt hơn.
+Hỗ trợ của địa phương cũng đóng góp tích cực vào sinh kế của người dân ở vùng hạn mặn. Trong những năm qua, người dân ở các địa phương đã nhận được nhiều sự hỗ trợ của chính quyền, như vay vốn với lãi suất ưu đãi, tập huấn chăn nuôi, nuôi trồng thủy sản, hỗ trợ giống lúa chịu mặn.
+Tuy nhiên, sự mặn hóa cũng ảnh hưởng đến việc sử dụng đất nông nghiệp. Quá trình nước biển dâng xâm lấn vào nội đồng làm cho đất bị ngập úng và nhiễm mặn, ảnh hưởng đến sản xuất nông nghiệp. Các vùng ven biển như thành phố Bạc Liêu, huyện Đông Hải, huyện Hòa Bình do kinh tế chủ yếu là nuôi thủy sản nên việc lấy nguồn nước biển thường xuyên phải mở thêm nhiều kênh rạch, làm cho nước biển đi vào sâu phía trong được thuận lợi. Các vùng phía trong quốc lộ 1A như huyện Giá Rai, huyện Phước Long mấy năm gần đây do người dân tự ý chuyển đổi từ trồng lúa qua nuôi tôm phá vỡ việc vận hành của hệ thống cống ngăn mặn, làm cho nước biển vào sâu trong nội đồng nguy cơ ngập ngày càng thể hiện rõ diện tích ngập tăng lên.</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2155,20 +2140,19 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed and comprehensive explanation of the impact of salinization on agricultural production, labor decisions, and the welfare of farmer households in the Vietnamese Mekong delta. It also successfully discusses the five main results of the analysis in detail, as requested by the user. The answer is well-structured, clear, and appears to be accurate, making it a high-quality response.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of salinization on agricultural production, labor decisions, and the welfare of farming households in the Mekong Delta, Vietnam. It also discusses changes in agricultural production and land use, labor supply, income and consumption of farming households, as well as adaptation channels such as migration and access to credit. However, it could have been more specific in discussing the changes in labor supply and consumption of farming households.</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The study mentions two channels for adaptation smoothing: migration and credit access. Can you elaborate on these channels and how they play a role in easing the income losses incurred by farmers during salinization shocks?</t>
+          <t>Trong nghiên cứu này, tác giả đã chỉ ra một số hạn chế liên quan đến việc đo lường mức độ mặn của sông. Hãy mô tả những hạn chế này và giải thích tại sao chúng có thể gây ra vấn đề trong việc xác định sự lan truyền của mặn.</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>The study suggests that migration and credit access are two potential channels for adaptation smoothing in response to salinization shocks. Migration refers to the movement of individuals from rural areas to urban centers for off-farm work. This can help to supplement income lost due to decreased agricultural productivity from salinization. However, the evidence for this channel is mixed, indicating that it may not always be a viable or effective strategy for all farmers.
-On the other hand, credit access refers to the availability and development of local credit markets. The study found that a more developed local credit market can play a positive role in easing the income losses incurred by farmers during salinization shocks. This is because access to credit can provide farmers with the necessary funds to invest in adaptive strategies, such as switching to salt-resistant crops or investing in new farming technologies. This can help to mitigate the negative impacts of salinization on their income.</t>
+          <t>Tác giả không chỉ ra bất kỳ hạn chế nào liên quan đến việc đo lường mức độ mặn của sông trong nghiên cứu này. Tuy nhiên, tác giả đã chỉ ra rằng mức độ mặn của sông đã tăng lên trong thời gian, với một số trường hợp mặn tăng lên đến 45‰, cao hơn nhiều so với mức 4‰ mà Trung tâm phòng tránh và giảm nhẹ thiên tai xem là mức xâm nhập mặn. Độ mặn này không chỉ kéo dài mà còn xâm nhập sâu vào đất liền, tới 70 km từ cửa sông và thậm chí có thời điểm đạt đến 85 km. Điều này có thể gây ra vấn đề trong việc xác định sự lan truyền của mặn do mức độ mặn thực tế có thể cao hơn nhiều so với những gì được đo lường hoặc dự đoán.</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2183,21 +2167,21 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the two channels for adaptation smoothing: migration and credit access. It also explains how these channels can help ease the income losses incurred by farmers during salinization shocks. The answer is accurate and comprehensive, making it deserving of a perfect score.</t>
+          <t>The generated answer is somewhat relevant to the user query, but it does not directly address the question about the limitations of measuring the salinity of rivers. Instead, it provides information about the increase in river salinity and the problems this can cause. The answer could be improved by directly addressing the limitations of salinity measurement and explaining why these limitations could cause problems in determining the spread of salinity.</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Based on the research findings in the document, explain the impact of salinization on total farm revenue and the adaptive measures farmers are taking in response to salinity shock in the Mekong Delta, Vietnam.</t>
+          <t>Theo nghiên cứu, hãy mô tả những tác động của sự mặn hóa đối với sản xuất nông nghiệp tại đồng bằng sông Cửu Long, cũng như những biện pháp thích ứng mà người dân địa phương đã áp dụng.</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Salinization does not have a significant impact on total farm revenue from all crops and aquaculture in the Mekong Delta, Vietnam. However, it does affect the productivity and revenue share of specific crops. For instance, higher salinity decreases the productivity and revenue share of rice crops and aquaculture production. On the other hand, it increases the revenue share of industrial crops, particularly coconut, which is a salt-resistant crop. 
-In response to salinity shock, farmers are adopting new crops and switching to salt-resistant industrial crops as a risk diversification strategy. This helps them secure their income against salinization shocks. Additionally, there is evidence of farmers reducing their agricultural land and labor supply in agriculture due to salinization. 
-Other adaptive measures include migration for off-farm work in urban centers and accessing credit markets. The development of local credit markets has been found to play a positive role in easing the income losses incurred by farmers during salinization shocks. There is also an increased investment in education, potentially implying farmers' efforts to acquire new skills to adapt to the changing environment.</t>
+          <t>Sự mặn hóa đã gây ra nhiều khó khăn cho sản xuất nông nghiệp tại đồng bằng sông Cửu Long. Một trong những vấn đề lớn nhất là sự suy giảm đáng kể của nguồn nước ngọt, điều này đã ảnh hưởng đến việc canh tác lúa. Tuy nhiên, người dân địa phương đã thích ứng với tình hình này bằng cách thống nhất lịch canh tác, điều này phụ thuộc vào thời gian máy cày đến ruộng và nguồn nước ngọt. Việc xuống giống đồng loạt cũng giúp việc mua bán sau khi thu hoạch dễ dàng hơn.
+Ngoài ra, chính quyền địa phương đã không cho phép sử dụng Nước Dưới Đất để duy trì diện tích lúa, do đó không có nông hộ nào sử dụng Nước Dưới Đất cho canh tác lúa mà chỉ sử dụng cho mục đích sinh hoạt. Điều này cho thấy sự hợp tác giữa người dân và các cấp quản lý cấp xã và huyện trong việc sử dụng nguồn tài nguyên Nước Dưới Đất.
+Nghiên cứu cũng cho thấy rằng người dân có kinh nghiệm sản xuất trên 10 năm có thể chủ động thích ứng với hạn mặn và thông qua những thất bại trước đó, họ có thể rút ra kinh nghiệm sản xuất tốt hơn. Hỗ trợ của địa phương, như vay vốn với lãi suất ưu đãi, tập huấn chăn nuôi, nuôi trồng thủy sản, hỗ trợ giống lúa chịu mặn, cũng đã đóng góp tích cực vào sinh kế của người dân ở vùng hạn mặn.</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2212,21 +2196,19 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of salinization on total farm revenue and the adaptive measures farmers are taking in response to salinity shock in the Mekong Delta, Vietnam. It does not contain any noticeable mistakes. The only reason it does not receive a perfect score is because it could be more concise.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impacts of salinization on agriculture in the Mekong Delta, as well as the adaptive measures that local people have implemented. It does not contain any noticeable errors or inaccuracies. However, it could be slightly more concise and clear in its presentation of information.</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>The paper discusses the concept of flood and salinity intrusion in the Mekong Delta. Discuss how these natural phenomena are perceived by the local people and the mitigation strategies suggested in the paper to deal with these issues.</t>
+          <t>Trình bày về vấn đề quản lý lũ lụt và xâm nhập mặn tại đồng bằng sông Cửu Long theo bài báo "Flood and Salinity Management in the Mekong Delta, Vietnam" của Le Anh Tuan. Hãy đề cập đến những hạn chế và thách thức trong việc xây dựng và quản lý hệ thống cơ sở hạ tầng kiểm soát nước.</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Floods in the Mekong Delta are perceived by many farmers and scientists not only as a disaster but also as a natural occurrence that brings multiple benefits. These benefits include fertile sediment, fish spawning, aquatic products, flushing effect, pest control, water quality, water provision, reduced fire risk, and ecological drivers. However, floods can also cause loss of life and property, and can lead to issues such as bank erosion, navigation hazards, pests, invasive exotic plants, and health risks.
-Salinity intrusion, on the other hand, occurs when not enough river discharge is flowing to the low-lying estuaries and instead, salt water flows into the land. This can cause damage to crops and restrict the use of canal water for domestic and industrial uses. However, it also has a positive effect of reducing acidity in potential acid sulphate soil land, leading to higher pH in water. This enables farmers to implement a more varied production scheme, such as raising shrimp during the dry season.
-To mitigate these issues, the paper suggests the use of computer modelling as a powerful tool in water resources engineering. This can help in understanding changes in water quantity and quality over time, and assist with decision-making in water planning and management. The results from these models can be used as a technical prerequisite for the development of a regional strategy and action plan to prepare for flood loss prevention and salinity management for the vulnerable agricultural sector.</t>
+          <t>Đồng bằng sông Cửu Long đang phải đối mặt với những hiểm họa như xâm nhập mặn, thiếu nước ngọt và ảnh hưởng của triều cường, những vấn đề này đã tăng lên trong những năm gần đây. Để đối phó và thích ứng với những hiểm họa này, chính quyền và người dân địa phương đã phát triển nhiều chiến lược và biện pháp như xây dựng đê bao, thay đổi kỹ thuật canh tác, hỗ trợ tài chính để khôi phục sản xuất sau thảm họa, khai thác nước ngầm và đa dạng hóa nguồn thu nhập. Tuy nhiên, những biện pháp thích ứng hiện tại có một số hạn chế, chẳng hạn như không đầy đủ xem xét sự khác biệt về môi trường sinh thái, xã hội và kinh tế. Kết quả của việc đánh giá tổn thương cho thấy rằng sự tổn thương của người dân phụ thuộc nhiều vào những điều kiện này. Do đó, các chiến lược thích ứng trong tương lai nên xem xét những vấn đề trên để hỗ trợ các nhóm xã hội khác nhau, đặc biệt là những nhóm dễ bị tổn thương nhất.</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2241,49 +2223,46 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive and accurate response. It discusses the perception of floods and salinity intrusion by the local people in the Mekong Delta and also outlines the mitigation strategies suggested in the paper. The answer is well-structured and detailed, providing a thorough understanding of the topic.</t>
+          <t>The generated answer is highly relevant to the user query and provides a comprehensive overview of the flood and salinity management issues in the Mekong Delta, as well as the challenges in building and managing water control infrastructure. It also mentions the limitations of current adaptation measures. However, it does not specifically reference the article "Flood and Salinity Management in the Mekong Delta, Vietnam" by Le Anh Tuan, which was asked for in the query.</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Explain the different types of floods as distinguished in the Vietnamese language and how each type impacts the Mekong Delta region.</t>
+          <t>Trình bày sự khác biệt giữa các loại lũ lụt được phân biệt trong tiếng Việt: lũ, lụt và ngập. Đồng thời, giải thích nguyên nhân gây ra từng loại lũ lụt này.</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>In the Vietnamese language, there are several types of floods distinguished. The term 'lũ' refers to a flood, which occurs when excess water upstream flows over river banks or dykes to the floodplain. 'Lụt' refers to inundation, which is affected by floods. 'Ngập' refers to submergence, a phenomenon that occurs when water levels in the plain, such as fields or land of the inner dyke or depression areas or wetlands, are higher than the ground surface level at a certain period. Submergence may be caused by high floods, heavy rainfall, a strong tide, or uprising groundwater.
-The term 'bão lũ' or storm-flood refers to a serious disaster when the basin is affected by strong storms and continuous heavy rainfall. These storm-floods frequently occur in North and Central Vietnam, but rarely in the South. 
-In the Mekong Delta, due to its location in the most downstream part of the basin, it receives the total volume of floodwaters from upstream. The flooded area ranges from 1.2 to 1.4 million hectares in years of low and medium flooding, and around 1.9 million hectares in years of high flooding. About 50 percent of the Mekong delta experiences flooding and these areas are also susceptible to serious damage by floods about every five years. High floods are caused when three simultaneous factors happen: large water discharges occur originating from upstream as affected by typhoons or tropical low pressures; long and heavy rainfall occurs in the Mekong Delta itself; and, high tides that lead to high water levels in the rivers and canal system prevent easy drainage. These floods result in loss of life, especially amongst children, and cause millions of dollars worth of damage to houses, infrastructure, and crops.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không chứa chi tiết về sự khác biệt giữa các loại lũ lụt như lũ, lụt và ngập, cũng như nguyên nhân gây ra từng loại lũ lụt này.</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of the different types of floods as distinguished in the Vietnamese language. It also thoroughly explains how each type impacts the Mekong Delta region. The answer is accurate and detailed, making it a perfect response to the user's query.</t>
+          <t>The generated answer is not relevant to the user query as it does not provide any information about the differences between the types of floods or their causes.</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Discuss the dual nature of floods in the Mekong Delta, highlighting both the damaging effects and the potential benefits they bring to the region.</t>
+          <t>Lũ lụt không chỉ gây ra thiệt hại mà còn mang lại những lợi ích gì cho đồng bằng sông Cửu Long? Hãy liệt kê và giải thích các lợi ích này.</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Floods in the Mekong Delta have a dual nature, bringing both damaging effects and potential benefits to the region. On the damaging side, high floods result in loss of life, particularly among children, and cause significant damage to houses, infrastructure, and crops. The cost of this damage can reach into the millions of dollars. Other indirect damages include economic losses due to interruption of economic activities, anxiety, inconvenience, ill health, and loss of cultural significance. There are also other recorded damages affecting rural communities and the commercial sector directly, such as bank erosion, navigation hazards, pests, invasive exotic plants, and health risks.
-On the other hand, floods are not only perceived as a disaster. They are historically linked with the natural form of the Mekong River delta region and bring multiple replenishing and revitalizing benefits. These include the deposit of fertile sediment, which enriches the soil for farming, the spawning of fish and production of aquatic products, a flushing effect that cleanses the waterways, pest control, improvement of water quality, provision of water, reduction of fire risk, and serving as ecological drivers. These benefits highlight the complex relationship between the people of the Mekong Delta and their environment.</t>
+          <t>The context does not provide information on the benefits that floods bring to the Mekong Delta.</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2293,29 +2272,24 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive discussion on the dual nature of floods in the Mekong Delta. It accurately highlights both the damaging effects and the potential benefits of floods in the region, providing specific examples for each. The answer is well-structured and fully correct, hence the perfect score.</t>
+          <t>The generated answer is not relevant to the user query. The user asked for the benefits of flooding in the Mekong Delta, but the chatbot did not provide any.</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Explain the impact of salinity intrusion on the Mekong Delta and its implications for local agriculture and water supply. Discuss the potential benefits and drawbacks of this phenomenon.</t>
+          <t>Hãy mô tả những lợi ích mà lũ lụt mang lại cho vùng đồng bằng sông Cửu Long, cũng như những tác động tiêu cực mà nó gây ra.</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Salinity intrusion in the Mekong Delta has a significant impact on local agriculture and water supply. It occurs when not enough river discharge is flowing to the low-lying estuaries, causing salt water to flow into the land. This intrusion is influenced by various factors such as tides, local rainfall and runoff, the slope of the river bed, wind velocity and direction, and the depth of the estuary.
-The impact on agriculture is complex. On one hand, higher salinity decreases the productivity and revenue share of rice crops and aquaculture production. It also leads to a reduction in the land used for rice and general agricultural purposes. On the other hand, it increases the revenue share of industrial crops like coconuts, which are salt-resistant. This suggests that farmers may be adopting new crops and switching crops as a risk diversification strategy to secure their income against salinization shocks.
-Salinity intrusion also affects labor supply in agriculture. It is estimated to decrease labor supply for those without agricultural land, but those with agricultural land do not seem to be affected. Furthermore, salinization reduces farmer households' income and consumption, but it may also lead to increased spending on education, possibly indicating an investment in new skills.
-The intrusion of salt water also leads to more salinity in groundwater layers, causing quality problems in many wells, such as high iron content, salinity, and odours. This has implications for future water supply plans, which are largely based on increased groundwater withdrawal.
-Despite these challenges, salinity intrusion also has some benefits. It reduces acidity in potential acid sulphate soil land, leading to higher pH in water. It also allows farmers to implement a more varied production scheme, such as raising shrimp during the dry season. Moreover, the marine and coastal region contributes more than half of the exported aquatic value for Vietnam.
-In conclusion, while salinity intrusion presents significant challenges for the Mekong Delta, it also offers some opportunities for adaptation and diversification. It is crucial to continue studying this phenomenon and its impacts to develop effective strategies for managing its effects.</t>
+          <t>Lũ lụt ở vùng đồng bằng sông Cửu Long mang lại một số lợi ích như việc cung cấp nước cho canh tác và giúp làm giàu đất đai bằng cách mang theo chất dinh dưỡng từ thượng nguồn. Tuy nhiên, lũ lụt cũng gây ra những tác động tiêu cực. Trong khoảng từ tháng 8 đến tháng 10, vùng này thường bị ngập lụt, gây ra thiệt hại cho nông nghiệp và nhà cửa. Từ tháng 1 đến tháng 4, vùng này lại chịu tác động mạnh mẽ của hiện tượng xâm nhập mặn và khô hạn, gây khó khăn cho việc cung cấp nước ngọt cho canh tác.</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2330,27 +2304,21 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive and detailed explanation of the impact of salinity intrusion on the Mekong Delta. It discusses the implications for local agriculture and water supply, and also presents both the potential benefits and drawbacks of this phenomenon. The answer is accurate and well-structured, making it easy to understand.</t>
+          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of both the benefits and negative impacts of flooding in the Mekong Delta region. It could be slightly improved by providing more specific examples or details.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>The Lower Mekong River and its delta are facing several anthropogenic stressors. Identify and discuss these stressors, and propose potential solutions to minimize their negative impacts and ensure the sustainability of the region.</t>
+          <t>Trình bày về những yếu tố ảnh hưởng đến sự xâm nhập mặn tại đồng bằng sông Cửu Long và hậu quả của nó đối với nông nghiệp và nguồn nước ngầm.</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>The Lower Mekong River and its delta are indeed facing several anthropogenic stressors. These include the construction of dams, climate change, poor water quality, and delta subsidence. 
-The construction of large-scale hydro-power dams in the Mekong Basin, which began in the 1990s, has had significant impacts on ecosystems and human life. These dams trap up to 95% of sediments, reducing downstream sediment loads and altering the natural hydrological cycle. This results in lower flood peaks and higher dry season flows, which can have detrimental effects on the region's biodiversity and agricultural productivity.
-Climate change is another major stressor, with studies projecting increased average temperatures in the Mekong River Basin. However, the future patterns of precipitation are uncertain. This uncertainty, coupled with the potential for increased temperatures, could exacerbate existing water scarcity issues and negatively impact the region's agriculture and aquaculture industries.
-Poor water quality and delta subsidence are also significant issues. The latter is particularly concerning as it could lead to increased flooding and saltwater intrusion, which can damage crops and contaminate freshwater resources.
-To minimize these negative impacts and ensure the sustainability of the region, several measures could be taken. Firstly, future decisions regarding dam construction should carefully consider the potential environmental and socio-economic impacts. This could involve conducting comprehensive environmental impact assessments and implementing measures to mitigate potential harm.
-Secondly, efforts should be made to mitigate and adapt to climate change. This could involve implementing sustainable agricultural practices, improving water management systems, and investing in renewable energy sources.
-Thirdly, measures should be taken to improve water quality. This could involve implementing stricter regulations on industrial and agricultural pollutants, as well as investing in water treatment facilities.
-Lastly, to address delta subsidence, efforts could be made to reduce groundwater extraction, which is a major cause of land subsidence. This could involve improving water efficiency and promoting the use of alternative water sources.
-In conclusion, while the Lower Mekong River and its delta are facing several significant anthropogenic stressors, there are a range of potential solutions that could help to minimize their negative impacts and ensure the sustainability of the region.</t>
+          <t>Các yếu tố ảnh hưởng đến kết quả sinh kế của cư dân vùng hạn mặn bao gồm số phương tiện sản xuất, kinh nghiệm sản xuất, số lao động chính, số nguồn thu nhập, hỗ trợ của địa phương, và vay vốn. Trong đó, chỉ có yếu tố vay vốn có mối quan hệ trái chiều với thu nhập của hộ gia đình.
+Xâm nhập mặn chủ yếu ảnh hưởng đến canh tác lúa, cụ thể là việc lúa bị thiệt hại do không đủ nước ngọt cung cấp. Đối với nuôi trồng thủy sản, việc nuôi tôm gần như không bị ảnh hưởng bởi tình trạng hạn mặn kéo dài do có nguồn nước dưới đất hỗ trợ cho việc pha loãng nồng độ mặn.
+Xâm nhập mặn cũng gây khó khăn trong quản lý nguồn nước dưới đất, đặc biệt là việc kiểm soát việc khai thác và sử dụng nguồn nước này. Trong khu vực nuôi tôm, người nông dân đã tăng cường khai thác nguồn nước dưới đất để giảm nồng độ mặn của nước mặt. Ngược lại, đối với người trồng lúa, xâm nhập mặn không ảnh hưởng đến nhu cầu sử dụng và khai thác nguồn nước dưới đất.</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2365,22 +2333,21 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive and detailed response. It correctly identifies and discusses the anthropogenic stressors affecting the Lower Mekong River and its delta, and proposes potential solutions to minimize their negative impacts and ensure the sustainability of the region. The answer is well-structured, clear, and accurate, demonstrating a deep understanding of the topic.</t>
+          <t>The generated answer is highly relevant to the user query, providing detailed information about the factors affecting salt intrusion in the Mekong Delta and its consequences for agriculture and groundwater. However, it does not explicitly mention the factors that directly influence salt intrusion, focusing more on the effects and coping mechanisms. Therefore, it is not fully comprehensive in addressing the user's question.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>"Discuss the various anthropogenic stressors impacting the Lower Mekong River and its delta. How do these factors compare to those affecting other large rivers around the world?"</t>
+          <t>Hãy mô tả các yếu tố đang đe dọa sông Mekong dưới hạ lưu, bao gồm tác động của đập, biến đổi khí hậu, sự lún của đồng bằng sông và sự suy giảm chất lượng nước. Hãy so sánh với các sông lớn khác trên thế giới và đề xuất các quyết định tương lai để giảm thiểu tác động tiêu cực và tìm kiếm một lộ trình đảm bảo sự phát triển bền vững.</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>The Lower Mekong River and its delta are currently facing several anthropogenic stressors. These include the construction of dams, climate change, poor water quality, and the sinking of the delta. The construction of large-scale hydro-power dams, which began in the 1990s, has had significant impacts on ecosystems and human life. These dams trap up to 95% of sediments, reducing downstream sediment loads and altering the natural hydrological cycle. Climate change is also a major concern, with projections indicating increased average temperatures, although precipitation patterns remain uncertain.
-Poor water quality is another issue, with salinity intrusion being a particular problem. This occurs when not enough river discharge is flowing to the low-lying estuaries, allowing salt water to flow into the land. This intrusion affects agriculture, restricts the use of canal water for domestic and industrial uses, and causes corrosion of metal materials. However, it also has some positive effects, such as reducing acidity in potential acid sulphate soil land and enabling farmers to implement a more varied production scheme.
-The sinking of the delta is another significant issue. This is influenced by factors such as the amplitude and period of tides, the amount of local rainfall and runoff, the slope of the river bed, the wind velocity and direction, and the depth of the estuary.
-When compared to other large rivers around the world, these factors are not unique to the Lower Mekong River. Many large rivers face similar issues, such as dam construction, climate change, and poor water quality. However, the specific impacts and severity of these issues can vary depending on the geographical, topological, climatic, and hydrological characteristics of each river and its surrounding region.</t>
+          <t>Các yếu tố đang đe dọa sông Mekong dưới hạ lưu bao gồm tác động của biến đổi khí hậu và sự lún của đồng bằng sông. Biến đổi khí hậu dẫn đến tăng tần suất và cường độ các hiện tượng thời tiết cực đoan, làm gia tăng mối đe dọa an ninh lương thực và tạo ra những biến động tiêu cực lên khu vực nông thôn. Đồng thời, sự lún của đồng bằng sông cũng là một vấn đề lớn, khiến cho nhiều vùng đất thấp có nguy cơ bị ngập chìm và xâm nhập mặn.
+So với các sông lớn khác trên thế giới, sông Mekong dưới hạ lưu còn phải chịu tác động nghiêm trọng hơn từ biến đổi khí hậu và nước biển dâng. Điều này có thể dẫn đến việc ít nhất 25% diện tích các vùng đất thấp ven biển có nguy cơ bị chìm ngập và khoảng 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn vào mùa khô.
+Để giảm thiểu tác động tiêu cực và tìm kiếm một lộ trình đảm bảo sự phát triển bền vững, cần phải có những chuyển biến tích cực trong việc kiểm soát khả năng nóng lên toàn cầu. Đồng thời, cần phải xem xét lại các hoạt động phát triển công nghiệp và nông nghiệp trong khu vực để giảm thiểu tác động đến môi trường và nguồn nước.</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2395,21 +2362,23 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive discussion of the anthropogenic stressors impacting the Lower Mekong River and its delta. It also effectively compares these factors to those affecting other large rivers around the world. The answer is accurate, detailed, and well-structured, making it a high-quality response to the user's question.</t>
+          <t>The generated answer is relevant and mostly correct. It addresses the threats to the Mekong River, compares it to other rivers, and suggests future decisions for sustainable development. However, it does not mention the impact of dams and the degradation of water quality, which were specifically asked for in the user query.</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>"Explain the socio-economic features of the Lower Mekong basin and how the construction of dams in the Mekong Basin has affected the region's ecosystems and human life. What are the potential consequences of these changes?"</t>
+          <t>Hãy mô tả các đặc điểm vùng Mekong, bao gồm địa lý, cài đặt topological, điều kiện khí hậu, thủy văn, đặc điểm dân số và các hoạt động do con người. Hãy nêu rõ cách mà các yếu tố này ảnh hưởng đến sự phát triển và bảo tồn của sông Mekong.</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>The Lower Mekong basin is home to over 70 million people, a number projected to increase to 90 million by 2025. Half of this population resides within 15 kilometers of the riverbanks, and the Mekong Delta alone hosts nearly 20 million inhabitants. The region has experienced rapid economic development following a period of conflicts, leading to substantial infrastructure development, including dam construction. Agriculture and aquaculture are vital to the economy, with extensive irrigation practices in the region. The natural flooding of the lower basin during the wet season contributes to high fertility and biodiversity, including numerous fish species, and supports a significant fishery industry with substantial annual production and income.
-The construction of large-scale hydro-power dams in the Mekong Basin began in the 1990s to meet increasing electricity demands. There are currently 176 dams planned or under construction in the Mekong River Basin, with a total hydro-power capacity of approximately 60 GW. These dams have had significant impacts on ecosystems and human life. They trap up to 95% of sediments, reducing downstream sediment loads, which can influence the delta's sedimentation rates. Dam operations have also altered the natural hydrological cycle, resulting in lower flood peaks and higher dry season flows. This has affected monsoon water flows downstream and is expected to impact flood frequency and flow magnitude in specific regions.
-The potential consequences of these changes include uncertainties in post-dam sediment data, potential consequences for the delta's sedimentation rates, and varying impacts on flood and low flow hydrology. Some studies attribute low flow levels to poor rainfall and deforestation. The changes brought about by dam construction could also outweigh the impacts of projected climate changes on the region's hydrology.</t>
+          <t>Vùng Mekong có một hệ thống sông rạch phức tạp, liên kết nhau và đổ ra biển Đông và biển Tây. Hai mặt giáp biển với tổng chiều dài vùng ven biển hơn 700 km, tạo ra tác động lớn từ các dao động biển. Vùng này chịu hai tác động dòng chảy: dòng chảy của sông Mekong từ thượng nguồn và dòng triều do tác động biển xâm nhập vào đất liền. Tháng 8 đến tháng 10 là thời gian bị ngập lũ, còn từ tháng 1 đến tháng 4 là thời gian bị tác động mạnh mẽ của hiện tượng xâm nhập mặn và khô hạn.
+Tần suất và cường độ các hiện tượng thời tiết cực đoan đang gia tăng, đe dọa an ninh lương thực và tạo ra những biến động tiêu cực lên khu vực nông thôn, như suy giảm nguồn tài nguyên thiên nhiên, thu hẹp diện tích canh tác và cư trú. Di cư từ nông thôn lên các vùng đô thị đang diễn ra nhanh hơn, tạo ra hệ lụy xấu về mặt xã hội và môi trường.
+Dự báo cho thập kỷ 2030-2040, nhiệt độ trung bình cũng như nhiệt độ lớn nhất và nhỏ nhất trong vùng sẽ gia tăng, phổ biến tăng khoảng 20˚C. Tổng lượng mưa trung bình cũng sẽ giảm, từ 10 đến 20%, khiến việc cung cấp nước ngọt cho canh tác lúa thêm khó khăn.
+Hiện tượng nóng lên toàn cầu và nước biển dâng đang tác động nghiêm trọng đến vùng này. Ít nhất 25% diện tích các vùng đất thấp ven biển có nguy cơ bị chìm ngập do nước biển dâng và lún sụt đồng bằng, khoảng 50-75% diện tích canh tác hiện nay sẽ bị nhiễm mặn vào mùa khô và khoảng 30-40% diện tích nông nghiệp bị ảnh hưởng của nước mặn ngay cả trong mùa mưa.
+Vùng đồng bằng sẽ bị ảnh hưởng kép, từ những tác động thay đổi tự nhiên mang tính toàn cầu và từ những hoạt động phát triển công nghiệp và nông nghiệp trong khu vực. Những thách thức này đang và sẽ là những thách thức lớn uy hiếp sự phát triển bền vững của nền nông nghiệp vùng Mekong.</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2424,108 +2393,100 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of the socio-economic features of the Lower Mekong basin, the impact of dam construction on the region's ecosystems and human life, and the potential consequences of these changes. It is well-structured and detailed, but it could be slightly more concise.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed description of the Mekong region, including its geography, climate conditions, hydrology, population characteristics, and human activities. It also explains how these factors affect the development and conservation of the Mekong River. However, it does not explicitly mention the topological setup, which was part of the user's query.</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>"Discuss the impact of dam construction on the hydrological cycle and sediment loads in the Mekong River Basin. How do these changes potentially affect the region's socio-economic aspects?"</t>
+          <t>Theo nghiên cứu, đập nước đã tác động như thế nào đến chu kỳ thủy văn tự nhiên và làm thay đổi lưu lượng nước trong mùa mưa và mùa khô? Hãy nêu rõ các hậu quả của việc xây dựng đập lên lưu lượng nước và tần suất lũ lụt ở các khu vực cụ thể.</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Dam construction in the Mekong River Basin has significantly altered the natural hydrological cycle. This alteration has resulted in lower flood peaks and higher dry season flows. The impacts on flood and low flow hydrology vary, with some studies attribiting low flow levels to poor rainfall and deforestation. Upstream dams and reservoirs have also affected monsoon water flows downstream, and dam development is expected to impact flood frequency and flow magnitude in specific regions.
-In terms of sediment loads, dams trap up to 95% of sediments, leading to a reduction in downstream sediment loads. The reduction in sediment discharge was particularly observed after the construction of the Manwan dam in China. The locations and quantities of dams influence sediment reduction, which can have potential consequences for the delta's sedimentation rates.
-These changes in the hydrological cycle and sediment loads can have significant impacts on the socio-economic aspects of the region. The lower flood peaks and higher dry season flows can affect agriculture and aquaculture, which are essential to the region's economy. The reduction in sediment loads can lead to uncertainties in post-dam sediment data, potentially affecting the stability of the Mekong Delta, which is home to 20 million people and plays a crucial role in rice production and export for Vietnam. Furthermore, the changes in flood frequency and flow magnitude can increase flood risks in certain areas, posing threats to local communities and infrastructure.</t>
+          <t>Rất tiếc, thông tin được cung cấp không đề cập đến tác động của đập nước đối với chu kỳ thủy văn tự nhiên hoặc làm thay đổi lưu lượng nước trong mùa mưa và mùa khô. Do đó, không thể nêu rõ hậu quả của việc xây dựng đập lên lưu lượng nước và tần suất lũ lụt ở các khu vực cụ thể.</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and appears to be fully correct. It provides a comprehensive discussion on the impact of dam construction on the hydrological cycle and sediment loads in the Mekong River Basin, and how these changes potentially affect the region's socio-economic aspects. The answer is detailed, well-structured, and covers all aspects of the query.</t>
+          <t>The generated answer is not relevant to the user query. The user asked for the impact of dams on the natural hydrological cycle and how they change water flow in rainy and dry seasons, as well as the consequences of dam construction on water flow and flood frequency in specific areas. The generated answer, however, does not provide any of this information.</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>"Compare the effects of dam construction on the Amazon River and China's Huang He (Yellow) River. What are the key risks associated with the construction of megadams on large rivers, and how does the Dam Environmental Vulnerability Index (DEVI) highlight these vulnerabilities?"</t>
+          <t>Đề cập đến tình hình ô nhiễm nước tại lưu vực sông Mekong, hãy mô tả những nguy cơ tiềm ẩn đối với chất lượng nước do sự gia tăng của nước thải công nghiệp, nông nghiệp và đô thị.</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>The construction of megadams on large rivers like the Amazon and China's Huang He (Yellow) River has significant impacts. The Amazon River is heavily dammed, with numerous dams already built and many more planned. This has led to high vulnerability in several sub-basins, as highlighted by the Dam Environmental Vulnerability Index (DEVI). On the other hand, dams on China's Huang He (Yellow) River have resulted in decreased sediment deposition and increased erosion downstream.
-The key risks associated with the construction of megadams on large rivers include downstream sediment and nutrient reductions, changes in flood patterns, and reservoir siltation. These risks can have significant environmental impacts and can disrupt the natural balance of the river ecosystem. The DEVI is a tool that helps to highlight these vulnerabilities by assessing the potential environmental risks associated with dam construction in different river basins.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không đề cập đến tình hình ô nhiễm nước tại lưu vực sông Mekong hoặc nguy cơ tiềm ẩn đối với chất lượng nước do sự gia tăng của nước thải công nghiệp, nông nghiệp và đô thị.</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive comparison of the effects of dam construction on the Amazon River and China's Huang He (Yellow) River. It also accurately describes the key risks associated with the construction of megadams on large rivers and explains how the Dam Environmental Vulnerability Index (DEVI) highlights these vulnerabilities. The only reason it does not receive a perfect score is because it does not provide specific examples or data to support its claims.</t>
+          <t>The generated answer is not relevant to the user query. The user asked for a description of the potential risks to water quality in the Mekong River basin due to the increase in industrial, agricultural, and urban wastewater, but the chatbot did not provide any information on this topic.</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>"Discuss the potential impacts of climate change on large rivers, such as the Mekong, Amazon, and Nile. How might these impacts vary depending on the specific characteristics of each river basin?"</t>
+          <t>Hãy mô tả những tác động tiêu cực của việc xây dựng đập lớn đối với các dòng sông lớn trên thế giới, đặc biệt là sông Amazon và sông Huang He (Yellow) của Trung Quốc.</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Climate change can have a variety of impacts on large rivers like the Mekong, Amazon, and Nile. For instance, studies in the Mekong River Basin have projected increased average temperatures, but the patterns of precipitation remain uncertain. This could potentially affect the hydrological cycle of the river, including the monomodal flood pulse, which is a key feature of the Mekong.
-In the case of the Amazon River, climate change is expected to intensify the hydrological cycle, potentially leading to an increase in extreme events during short periods. This could result in increased flood magnitude and return period. Similarly, atmospheric rivers, which transport moisture, may also be influenced by climate change, impacting the river flow regimes.
-For the Nile and Danube rivers, climate change might lead to decreased flood magnitude and return period. This is because these rivers might not be as affected by monsoon rainfall and glacier meltwater as others, like the Indus and Brahmaputra, which could face reduced flow due to glacier loss.
-The impacts of climate change on these rivers can vary depending on the specific characteristics of each river basin. For example, rivers like the Huang He might benefit from increased precipitation due to climate change, while Arctic rivers in Russia may experience increased flow due to ice melt and permafrost thaw. 
-In summary, climate change can have diverse impacts on large rivers, and these impacts can vary greatly depending on the specific characteristics of each river basin.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không đề cập đến tác động tiêu cực của việc xây dựng đập lớn đối với các dòng sông lớn trên thế giới, đặc biệt là sông Amazon và sông Huang He (Yellow) của Trung Quốc.</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed discussion on the potential impacts of climate change on large rivers such as the Mekong, Amazon, and Nile. It also explains how these impacts might vary depending on the specific characteristics of each river basin. However, the user didn't ask about the Danube, Huang He, or Arctic rivers in Russia, so the inclusion of these rivers is unnecessary and slightly detracts from the answer's focus.</t>
+          <t>The generated answer is not relevant to the user query. The user asked for a description of the negative impacts of building large dams on major rivers in the world, especially the Amazon and Huang He (Yellow) rivers, but the generated answer does not provide any information on this topic.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>"Explain the role of international organizations like the Mekong River Commission in promoting sustainable development and facilitating communication among countries. How can lessons from the management of other large rivers, like the Nile, inform improved management of the Mekong?"</t>
+          <t>Trình bày về những chiến lược cục bộ và khu vực được đề xuất trong bài nghiên cứu để giải quyết các vấn đề liên quan đến nguồn nước ngầm và phát triển đập.</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>International organizations such as the Mekong River Commission (MRC) play a crucial role in promoting sustainable development and facilitating communication among countries in the Mekong region. They are responsible for sharing scientific data, which can help in making informed decisions about the region's development. The MRC also reviews projects for potential development impacts, ensuring that any proposed initiatives are sustainable and beneficial for the region.
-Lessons from the management of other large rivers, like the Nile, can be used to improve the management of the Mekong. The Nile has robust international management, which can serve as a model for the Mekong. By studying the strategies and practices used in the Nile's management, the Mekong region can adopt and implement similar measures to address its unique challenges. This could include strategies for dam development, water quality improvement, and dealing with the impacts of climate change.</t>
+          <t>Bài nghiên cứu đề xuất một số chiến lược để giải quyết các vấn đề liên quan đến nguồn nước ngầm và phát triển đập. Đầu tiên, cần quy hoạch lại hệ thống kênh, vét kênh để tạo dòng chảy nhằm chia sẻ lượng nước trên các con sông với nhau. Thứ hai, xây dựng hệ thống đê điều hợp lý để ngăn nước biển và hệ thống đập ngăn mặn ngăn nước biển xâm nhập vào đồng ruộng, nhằm giảm thiệt hại do xâm nhập mặn gây ra.</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2540,19 +2501,19 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of the role of international organizations like the Mekong River Commission. It also correctly addresses how lessons from the management of other large rivers can inform improved management of the Mekong. The only reason it doesn't get a perfect score is because it could have provided more specific examples or details from the Nile's management that could be applied to the Mekong.</t>
+          <t>The generated answer is relevant to the user query and provides strategies to address the issues related to groundwater and dam development. However, it does not specifically mention local and regional strategies as asked in the query.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>In the context of the research paper "Thiết lập mô hình cân bằng nước phục vụ lập quy hoạch tổng hợp lưu vực sông Cửu Long", what is the role of the MIKE HYDRO BASIN (MHB) model in assessing the water supply's ability to meet various water usage needs in the Mekong River Basin?</t>
+          <t>Theo nghiên cứu trong bài báo, mô hình cân bằng nước MIKE HYDRO BASIN (MHB) được áp dụng để đánh giá khả năng đáp ứng của nguồn nước cho những nhu cầu sử dụng nước nào tại lưu vực sông Cửu Long?</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>The MIKE HYDRO BASIN (MHB) model is used to evaluate the ability of the water supply to meet various water usage needs in the Mekong River Basin. The entire basin is divided into 120 comprehensive water resource management areas. Water usage needs are calculated for six purposes including living, industry, cultivation, livestock, aquaculture, and other needs, and are limited to freshwater. The MHB model calculates the water balance on a daily basis for the current year 2020, to determine in detail the total water shortage throughout the year, the time of water shortage in the year, the months of water shortage throughout the basin and in the 120 comprehensive water resource management areas. The results show that the total water shortage throughout the year in the entire basin accounts for about 11.4% of the total water usage needs, with the most shortage occurring in February to April (19.1-19.6%), and the area with the most shortage is the Ca Mau peninsula. The MHB model applied to the Mekong River Basin can be used as a quick and convenient assessment tool to evaluate the water supply's ability to respond to different planning scenarios, thereby forming the basis for selecting appropriate water allocation options. The river network established in the MHB model includes 130 rivers and channels, of which 43 rivers are part of the comprehensive planning of the Mekong River Basin and are inter-provincial rivers and water sources. The selected rivers and channels are all major channels or the boundaries of water use areas.</t>
+          <t>Mô hình cân bằng nước MIKE HYDRO BASIN (MHB) được áp dụng để đánh giá khả năng đáp ứng của nguồn nước dựa trên số lượng nước. Mô hình này phụ thuộc lớn vào các quy tắc được thiết lập để phân bổ dòng chảy, bao gồm các quy tắc về phân bổ lượng nước nội sinh từ mưa vào các sông/kênh, tỉ lệ phân lưu giữa các nhánh sông/kênh, phân bổ nhu cầu nước đối với từng nguồn cấp, phân bổ nguồn cấp cho từng đối tượng sử dụng nước, và phân bổ dòng chảy hồi quy trở lại từng nguồn cấp. Tuy nhiên, mô hình này không xem xét đến chất lượng nước và độ mặn.</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2562,24 +2523,24 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the role of the MIKE HYDRO BASIN (MHB) model in assessing the water supply's ability to meet various water usage needs in the Mekong River Basin. It includes specific details about the model's application, the division of the basin, the calculation of water usage needs, and the results of the model's application. The answer is fully correct and comprehensive, providing a clear and thorough response to the user's question.</t>
+          <t>The generated answer is relevant to the user query and provides a detailed explanation of how the MIKE HYDRO BASIN (MHB) model is used to evaluate the water supply's ability to meet various water usage needs. However, it does not specifically mention the Mekong Delta (Cửu Long River Basin), which was part of the user's question.</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>According to the document, how do international organizations like the Mekong River Commission (MRC) contribute to sustainable development and communication among Mekong countries?</t>
+          <t>Theo kết quả tính toán từ mô hình MHB, thời gian thiếu nước nhiều nhất trong năm ở lưu vực sông Cửu Long là vào những tháng nào và khu vực nào thiếu nước nhiều nhất?</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>International organizations like the Mekong River Commission (MRC) contribute to sustainable development and communication among Mekong countries by sharing scientific data, promoting sustainable development practices, and facilitating communication. The MRC also reviews projects for potential development impacts.</t>
+          <t>Thời gian thiếu nước nhiều nhất trong năm ở lưu vực sông Cửu Long là vào các tháng 2–4. Khu vực thiếu nước nhiều nhất là vùng bán đảo Cà Mau, đặc biệt là vùng Nam bán đảo Cà Mau, với tỉ lệ thiếu trung bình 25,5%.</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2594,19 +2555,19 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and appears to be correct, providing specific ways in which the MRC contributes to sustainable development and communication among Mekong countries. However, without a reference answer, it's difficult to confirm the absolute accuracy of the information.</t>
+          <t>The generated answer is highly relevant to the user query and provides specific and detailed information about the time of year and the area where water shortage is most severe in the Mekong Delta, according to the MHB model.</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Explain the impact of the East Sea and West Sea tides on the flow in the LVSCL river system, including Tan Chau and Chau Doc. How does this two-way flow (negative or positive flow rate) depend on the tide?</t>
+          <t>Hãy mô tả đặc điểm của dòng chảy trong hệ thống sông, kênh vùng LVSCL, bao gồm cả dòng chảy tại Tân Châu và Châu Đốc? Và giải thích tại sao mô hình MHB chỉ cho phép thiết lập dòng chảy cố định 1 chiều?</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>The flow in the LVSCL river system, including Tan Chau and Chau Doc, is significantly influenced by the tides of the East Sea and West Sea. This results in a two-way flow, meaning the flow can either be negative or positive depending on whether the tide is rising or falling. The tidal regime is semi-diurnal or irregular semi-diurnal, which means there are usually two high tides and two low tides each day. The direction chosen in the river network setup is the direction of the average flow over a long period (month). This setup may not accurately simulate the actual flow regime, but it aligns with the general trend of the flow and the purpose of assessing the ability to meet fresh water needs over a long period.</t>
+          <t>Dòng chảy trong hệ thống sông, kênh vùng LVSCL, bao gồm cả dòng chảy tại Tân Châu và Châu Đốc, có đặc điểm là chịu ảnh hưởng mạnh của thủy triều biển Đông và biển Tây, nên dòng chảy là 2 chiều, phụ thuộc vào lúc triều lên hay triều rút. Trong ngày thường có 2 lần triều lên và 2 lần triều rút. Tuy nhiên, mô hình MHB chỉ cho phép thiết lập dòng chảy cố định 1 chiều. Lý do là mô hình này được thiết kế để mô phỏng xu hướng chung của dòng chảy và đánh giá khả năng đáp ứng nhu cầu nước ngọt trong thời đoạn dài, đồng thời đảm bảo sự đơn giản và linh hoạt cần thiết trong việc đánh giá các phương án, kịch bản phân bổ nguồn nước khác nhau.</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2621,46 +2582,47 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how the tides of the East Sea and West Sea influence the flow in the LVSCL river system, including Tan Chau and Chau Doc. It also explains how this results in a two-way flow, which can be either negative or positive depending on the tide. The only reason it doesn't get a perfect score is because it doesn't explicitly state how the flow rate depends on the tide, which was part of the user's question.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate explanation of the flow characteristics in the LVSCL river system, including Tan Chau and Chau Doc. It also correctly explains why the MHB model only allows for a one-way fixed flow setup.</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Describe the challenges faced in applying the MHB model to balance water in detail up to 120 regions in LVSCL. How does the model incorporate the endogenous flow from rain and groundwater sources?</t>
+          <t>Trong mô hình MHB, dòng chảy nội sinh từ mưa được đưa vào mô hình thông qua bao nhiêu nút? Và mỗi nút này đại diện cho điều gì?</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>The context does not provide information on the challenges faced in applying the MHB model to balance water in up to 120 regions in LVSCL, nor does it discuss how the model incorporates the endogenous flow from rain and groundwater sources.</t>
+          <t>Trong mô hình MHB, dòng chảy nội sinh từ mưa được đưa vào mô hình thông qua 120 nút. Mỗi nút này đại diện cho một khu sử dụng nước.</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant information or answer to the user's query. It simply states that the context does not provide information, which is not helpful or informative.</t>
+          <t>The generated answer is not relevant to the user query. The user query asks about the MHB model, but the generated answer does not provide any specific information about this model.</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Can you explain the concept of "Tỉ lệ phân lưu" (bifurcation rate) as described in the research paper "researched_paper_cleanup.txt"? How is it determined at each node in the context of river flow?</t>
+          <t>Hãy giải thích ý nghĩa của "Tỉ lệ phân lưu" và "Quy tắc lấy nước từ nhiều nút cấp" trong nghiên cứu về mạng lưới sông LVSCL.</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>The concept of "Tỉ lệ phân lưu" or bifurcation rate refers to the proportion of flow that is diverted at each node in a river network. It is determined by the ratio of the flow volume that goes into a branch river to the total flow volume that arrives at the node. This bifurcation of flow within the river network is relatively stable. The bifurcation rate is incorporated into the model as the relationship between the flow volume of the main river and its branches, determined from the results of hydraulic model calculations. This includes the influence of tides. However, in locations significantly affected by tides, the relationship between hourly or average daily flow volumes between the main river and its branches can be complex, especially when the main river and its branches are influenced by tides from different directions. The impact of border overflow also complicates the flow volume relationship between the main river and its branches. Therefore, running separate models for flood and dry seasons ensures better simulation and higher reliability due to the relatively stable direction of average daily flow or larger time spans per season.</t>
+          <t>"Tỉ lệ phân lưu" là một khái niệm liên quan đến cách dòng chảy được phân chia tại mỗi nút trong mạng lưới sông. Nó được xác định bằng cách lấy tỉ lệ giữa lưu lượng dòng chảy ra sông nhánh và tổng lưu lượng dòng chảy đến nút. Điều này cho thấy cách dòng chảy được phân phối trong mạng lưới sông.
+"Quy tắc lấy nước từ nhiều nút cấp" là một quy tắc được sử dụng trong nghiên cứu để xác định tỉ lệ nhu cầu nước của một đối tượng được lấy từ một nút cụ thể. Tỉ lệ này được xác định bằng cách lấy tỉ lệ giữa lượng nước đến tại nút cụ thể và tổng lượng nước đến tại tất cả các nút cấp cho đối tượng đang xét. Tỉ lệ này không cố định mà thay đổi theo ngày, tương ứng với sự thay đổi của lượng nước đến từng nút.</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2675,19 +2637,19 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>The generated answer provides a comprehensive explanation of the concept of "Tỉ lệ phân lưu" or bifurcation rate, and how it is determined at each node in the context of river flow. It also discusses the complexities involved in determining the bifurcation rate, such as the influence of tides and border overflow. The answer is relevant and appears to be correct, but without a reference answer, it's difficult to confirm its complete accuracy.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate explanation of the terms "Tỉ lệ phân lưu" and "Quy tắc lấy nước từ nhiều nút cấp" in the context of river network studies. The answer is clear, comprehensive, and appears to be correct, even in the absence of a reference answer.</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>According to the research paper, what is the significance of the "priority node" in water distribution? How is the water allocation for an object from a node calculated?</t>
+          <t>Theo kết quả nghiên cứu, vùng nào thiếu nước nhiều nhất và thời gian thiếu nước nhiều nhất là khi nào? Hãy nêu nguyên nhân dựa trên thông tin trong bài.</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>The "priority node" in water distribution is significant as it determines the proportion of water allocated to a specific object from a node. The water allocation for an object from a node is calculated by the ratio of the water demand of that object taken from that node (an object can take water from multiple nodes) to the total water demand of all objects taking water from that node.</t>
+          <t>Vùng Đồng Bằng Sông Cửu Long, cụ thể là tỉnh Sóc Trăng và huyện Long Phú, đã chịu ảnh hưởng nặng nề nhất về thiếu nước. Thời gian thiếu nước nhiều nhất là vào cuối năm 2015 và đầu năm 2016. Nguyên nhân chính là do xâm nhập mặn và khô hạn. Điều này đã làm giảm nguồn nước mặt dùng cho canh tác lúa, buộc nông dân phải sử dụng nước giếng, dẫn đến suy giảm nguồn tài nguyên nước dưới đất.</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2702,46 +2664,47 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and appears to be correct, providing a clear explanation of the significance of the "priority node" in water distribution and how water allocation for an object from a node is calculated. However, without a reference answer, it's difficult to confirm the absolute accuracy of the information.</t>
+          <t>The generated answer is highly relevant to the user query and provides detailed and accurate information about the region most affected by water shortage, the time when the shortage was most severe, and the reasons for the shortage.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>What are the two main obstacles that affect the validity of the water balance results using the MHB model on LVSCL and similar areas with complex river/channel networks, as mentioned in the document?</t>
+          <t>Trong nghiên cứu này, mô hình MHB đã được sử dụng để phân bổ nguồn nước. Tuy nhiên, mô hình này có hạn chế gì và tại sao việc xem xét chất lượng nước, đặc biệt là độ mặn, lại quan trọng trong bối cảnh hiện tại?</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>The document does not provide specific information on the two main obstacles that affect the validity of the water balance results using the MHB model on LVSCL and similar areas with complex river/channel networks.</t>
+          <t>Mô hình MHB được sử dụng trong nghiên cứu này chủ yếu tập trung vào việc phân bổ số lượng nước, nhưng nó không xem xét đến chất lượng nước, đặc biệt là độ mặn. Điều này là một hạn chế vì chất lượng nước, bao gồm độ mặn, có thể ảnh hưởng đến việc sử dụng nước cho các mục đích khác nhau, như sản xuất nông nghiệp. Điều này đặc biệt quan trọng trong bối cảnh hiện tại, khi mặn được dự báo sẽ thay đổi bất thường do chế độ vận hành của các thủy điện ở thượng lưu. Đối với các khu vực sử dụng nước thuộc vùng mặn và lợ thuộc vùng bán đảo Cà Mau, việc xem xét độ mặn là cần thiết, vì xâm nhập mặn có thể gây ra sự thiếu hụt nước nghiêm trọng hơn.</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query as it addresses the topic of the MHB model and its application to areas with complex river/channel networks. However, it does not provide any specific information about the two main obstacles that affect the validity of the water balance results, which was the main point of the user's question. Therefore, it is not fully correct.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the limitations of the MHB model and the importance of considering water quality, especially salinity. It also provides context for the current situation. The only reason it doesn't get a perfect score is because without a reference answer, it's hard to confirm the absolute correctness of the information.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>In the context of the document, how is the flow distribution ratio, which is input into the model, determined and what factors does it include?</t>
+          <t>Trình bày hai trở ngại chính ảnh hưởng đến tính hợp lý của kết quả cân bằng nước bằng mô hình MHB trên LVSCL và giải thích cách tỷ lệ phân lưu được xác định trong mô hình này.</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>The flow distribution ratio is determined from the results of hydraulic model calculations. It is input into the model as the relationship between the main flow and the branch flow. This ratio includes the influence of the tide. However, in locations significantly affected by the tide, the relationship between the hourly or daily average flow of the main and branch rivers is often not strict, especially when the main river and the branch river are affected by tides from two different directions. Additionally, the impact of border overflow also complicates the flow relationship between the main and branch rivers, making it difficult to strictly define. At certain times of the day, the bifurcation point can turn into an inflow point or vice versa due to the change in direction of the average flow. Therefore, separating the model for the flood season and the dry season ensures better simulation and higher reliability as the direction of the average daily flow or larger time period is quite stable for each season.</t>
+          <t>Hai trở ngại chính ảnh hưởng đến tính hợp lý của kết quả cân bằng nước bằng mô hình MHB trên LVSCL bao gồm việc xác định tỷ lệ phân lưu giữa các nhánh sông/kênh, và tỉ lệ phân bổ giữa nhiều nguồn nước cho nhiều đối tượng khác nhau. 
+Tỷ lệ phân lưu trong mô hình này được xác định dưới dạng đường quan hệ lưu lượng giữa dòng chính và dòng nhánh, được xác định từ kết quả tính toán của mô hình thủy lực, do đó đã bao gồm ảnh hưởng của triều. Cụ thể hơn, tỷ lệ phân lưu tại mỗi nút được xác định bằng tỉ lệ lưu lượng dòng chảy ra sông nhánh trên tổng lưu lượng dòng chảy đến nút. Sự phân chia dòng chảy trong mạng sông LVSCL là tương đối ổn định.</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2756,19 +2719,20 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how the flow distribution ratio is determined and the factors it includes. It mentions the influence of the tide, the impact of border overflow, and the change in direction of the average flow. The only reason it doesn't get a perfect score is because it could be more concise.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and accurate explanation of the two main obstacles affecting the validity of the water balance results using the MHB model on LVSCL and how the diversion ratio is determined in this model.</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Explain the impact of tidal influences on the relationship between the main stream and branch flow in areas with significant tidal effects, as discussed in the text. How does this relationship become more complex during flood season and dry season?</t>
+          <t>Theo nghiên cứu, hãy mô tả ảnh hưởng của triều và lũ tràn biên giới đến quan hệ lưu lượng giữa dòng chính và dòng nhánh? Vì sao việc chia mô hình chạy riêng rẽ cho mùa lũ và mùa kiệt lại quan trọng?</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>The text does not provide specific information on the impact of tidal influences on the relationship between the main stream and branch flow in areas with significant tidal effects, nor does it discuss how this relationship becomes more complex during flood season and dry season.</t>
+          <t>Triều và lũ tràn biên giới có ảnh hưởng đáng kể đến quan hệ lưu lượng giữa dòng chính và dòng nhánh. Tại các vị trí chịu ảnh hưởng triều lớn, quan hệ giữa lưu lượng giờ hoặc lưu lượng trung bình ngày giữa dòng chính và dòng nhánh thường không chặt chẽ, đặc biệt khi sông chính và sông nhánh chịu ảnh hưởng triều từ hai hướng khác nhau. Ảnh hưởng của lũ tràn biên giới cũng làm cho quan hệ lưu lượng giữa dòng chính và dòng nhánh trở nên rất phức tạp, khó chặt chẽ. Có những thời điểm trong ngày từ vị trí là điểm phân lưu biến thành nhập lưu hoặc ngược lại do dòng chảy trung bình đổi chiều. 
+Việc chia mô hình chạy riêng rẽ cho mùa lũ và mùa kiệt quan trọng vì nó đảm bảo mô phỏng tốt, độ tin cậy cao hơn do chiều dòng chảy trung bình ngày hoặc thời đoạn lớn hơn là khá ổn định theo từng mùa.</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2778,24 +2742,24 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information or explanation about the impact of tidal influences on the relationship between the main stream and branch flow in areas with significant tidal effects, nor does it discuss how this relationship becomes more complex during flood season and dry season. It simply states that the text does not provide this information, which does not answer the user's query.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the impact of tides and border floods on the flow relationship between the main stream and the branch stream. It also explains why it is important to separate the model for the flood season and the dry season. The answer seems to be correct and comprehensive, but without a reference answer, it's hard to be completely certain.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Based on the research findings in the document, identify the region with the highest water shortage and provide the average shortage percentage. Also, discuss the time of the year when the water shortage is most severe.</t>
+          <t>Dựa vào kết quả tính toán cân bằng nước, hãy phân tích tình hình thiếu nước trên lưu vực, đặc biệt là vùng bán đảo Cà Mau và các vùng giáp biển Đông và biển Tây.</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>The context does not provide specific information on the region with the highest water shortage or the average shortage percentage. It also does not discuss the time of the year when the water shortage is most severe.</t>
+          <t>Tổng lượng nước thiếu cả năm trên toàn vùng chiếm khoảng 11,4% so với tổng nhu cầu sử dụng nước. Thời gian thiếu nước nhiều nhất là vào tháng 2–4. Vùng bán đảo Cà Mau, đặc biệt là vùng Nam bán đảo Cà Mau, là khu vực thiếu nước nhiều nhất với tỉ lệ thiếu trung bình 25,5%. Các vùng khác như Tứ giác Long Xuyên, giữa sông Tiền–sông Hậu, và tả sông Tiền cũng gặp tình trạng thiếu nước, nhưng không nghiêm trọng như vùng bán đảo Cà Mau, kể cả vào mùa khô. Tuy nhiên, một số khu vực giáp biển Đông và biển Tây cũng gặp tình trạng thiếu nước do bị nhiễm mặn.</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2810,19 +2774,19 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information related to the user's query. It simply states that the information is not available, which does not help answer the user's question.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the water shortage situation in the specified areas. It also includes specific statistics and mentions the most affected periods and regions, which shows a high level of accuracy. However, without a reference answer, it's hard to confirm the exact correctness of the provided data.</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Based on the research paper "Nghiên cứu, đề xuất các mô hình sinh kế nông nghiệp thích ứng với xâm nhập mặn tại tỉnh Vĩnh Long", can you explain the impact of salt intrusion on the agricultural models in Vĩnh Long province and how the proposed models can adapt to this situation?</t>
+          <t>Trong nghiên cứu "Nghiên cứu, đề xuất các mô hình sinh kế nông nghiệp thích ứng với xâm nhập mặn tại tỉnh Vĩnh Long", tác giả đã xem xét bao nhiêu mô hình sinh kế nông nghiệp thích ứng với xâm nhập mặn và cuối cùng đã xây dựng được bao nhiêu mô hình phù hợp với tình hình canh tác tại tỉnh Vĩnh Long? Hãy liệt kê các lĩnh vực mà các mô hình này thuộc về.</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>The context does not provide information on the research paper "Nghiên cứu, đề xuất các mô hình sinh kế nông nghiệp thích ứng với xâm nhập mặn tại tỉnh Vĩnh Long", or the impact of salt intrusion on the agricultural models in Vĩnh Long province and how the proposed models can adapt to this situation.</t>
+          <t>Thông tin trong ngữ cảnh không cung cấp đủ chi tiết về số lượng mô hình sinh kế nông nghiệp được xem xét trong nghiên cứu "Nghiên cứu, đề xuất các mô hình sinh kế nông nghiệp thích ứng với xâm nhập mặn tại tỉnh Vĩnh Long", cũng như số lượng mô hình đã được xây dựng phù hợp với tình hình canh tác tại tỉnh Vĩnh Long. Cũng không có thông tin về các lĩnh vực mà các mô hình này thuộc về.</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2837,46 +2801,47 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant information or answer to the user's query. It simply states that the context does not provide the necessary information, which is not helpful or informative.</t>
+          <t>The generated answer is relevant to the user query as it addresses the question about the number of models considered and built in the research. However, it does not provide any specific information or details, stating that the context does not provide enough information. This is a limitation, but the answer is still relevant and does not contain factual errors.</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>The paper mentions the effects of salt intrusion during the dry season of 2015-2016 and 2019-2020 in Vĩnh Long province. Can you describe the extent of these effects and how they impacted different types of crops and regions within the province?</t>
+          <t>Tại tỉnh Vĩnh Long, xâm nhập mặn đã gây ảnh hưởng như thế nào đến sản xuất nông nghiệp trong mùa khô 2015-2016 và mùa khô 2019-2020? Hãy nêu rõ các con số và vùng bị ảnh hưởng nếu có.</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>The context does not provide specific information about the effects of salt intrusion during the dry season of 2015-2016 and 2019-2020 in Vĩnh Long province, or how they impacted different types of crops and regions within the province.</t>
+          <t>Rất tiếc, thông tin được cung cấp không đề cập đến ảnh hưởng của xâm nhập mặn đến sản xuất nông nghiệp tại tỉnh Vĩnh Long trong mùa khô 2015-2016 và mùa khô 2019-2020.</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any relevant information to the user's query. It simply states that the context does not provide the necessary information, which does not answer the user's question.</t>
+          <t>The generated answer is not relevant to the user query as it does not provide any information about the impact of saltwater intrusion on agricultural production in Vinh Long province during the dry seasons of 2015-2016 and 2019-2020.</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Based on the research conducted in the Vĩnh Long province, what were the key strategies implemented to enhance the effectiveness of the SKNN models adapted for XNM?</t>
+          <t>Hãy mô tả quy trình xây dựng và áp dụng 15 mô hình SXNN thích ứng XNM tại tỉnh Vĩnh Long, bao gồm các bước từ việc phân tích đặc điểm của các mô hình SKNN hiện hữu, xem xét 25 mô hình SKNN thích ứng với XNM, đến việc tổ chức tập huấn và thực tế cho nông hộ.</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>The key strategies implemented to enhance the effectiveness of the SKNN models adapted for XNM in the Vĩnh Long province included the construction of 15 SKNN models suitable for the local farming situation. These models were adapted for various sectors such as crop cultivation, livestock farming, aquaculture, and combined production. Additionally, five models were piloted at 20 households, which included rice cultivation, corn, watermelon, breeding cattle, and striped catfish farming, showing high economic efficiency and potential for expansion in similar conditions. To further enhance the application effectiveness, nearly 100 farming households in Vũng Liêm, Trà Ôn, and Mang Thít districts were trained in three conferences. A practical study tour was also organized in Bến Tre province for 30 exemplary farming households. The remaining models are recommended to be piloted in the annual agricultural promotion programs of the province, and the application of supportive policies for farming households is suggested.</t>
+          <t>Đầu tiên, các đặc điểm của các mô hình sinh kế nông nghiệp (SKNN) hiện hữu tại địa phương được phân tích. Sau đó, 25 mô hình SKNN thích ứng với xâm nhập mặn (XNM) được xem xét, những mô hình này đã được áp dụng một cách hiệu quả tại đồng bằng sông Cửu Long (ĐBSCL). Dựa trên bộ tiêu chí đánh giá tính khả thi (bao gồm 7 nhóm tiêu chí và 45 chỉ thị thành phần), 15 mô hình SXNN thích ứng XNM thuộc các lĩnh vực trồng trọt, chăn nuôi, nuôi trồng thuỷ sản (NTTS) và sản xuất kết hợp được xây dựng phù hợp với tình hình canh tác tại tỉnh Vĩnh Long.
+Để tăng cường hiệu quả ứng dụng, 3 hội nghị tập huấn cho gần 100 nông hộ tại huyện Vũng Liêm, Trà Ôn, Mang Thít và 01 chuyến tham quan, học tập thực tế tại tỉnh Bến Tre cho 30 nông hộ điển hình đã được tổ chức. Trong số các mô hình được đề xuất, 5 mô hình được triển khai thí điểm tại 20 hộ (trồng lúa, bắp nếp, dưa hấu, nuôi bò sinh sản và cá rô phi vằn) cho hiệu quả kinh tế cao cũng như tiềm năng nhân rộng tại các khu vực có điều kiện tương tự.</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2891,46 +2856,47 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the strategies implemented to enhance the effectiveness of the SKNN models in the Vĩnh Long province. It does not contain any noticeable mistakes. However, it could be slightly more concise.</t>
+          <t>The generated answer is highly relevant and accurate to the user query. It provides a detailed description of the process of building and applying 15 adaptive agricultural livelihood models in Vinh Long province, including the steps from analyzing the characteristics of existing models, considering 25 models adapted to saltwater intrusion, to organizing training and practical for households.</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>In the context of the research paper "Giải pháp vận hành thông minh hệ thống thủy lợi liên tỉnh tại vùng đồng bằng sông cửu long" by Dũng et al. (2021), what were the proposed solutions for the operation of the inter-provincial irrigation system in the Mekong Delta region?</t>
+          <t>Trong các mô hình đề xuất, 5 mô hình đã được triển khai thí điểm tại 20 hộ và cho thấy hiệu quả kinh tế cao cũng như tiềm năng nhân rộng. Hãy liệt kê và mô tả chi tiết về 5 mô hình này, bao gồm lĩnh vực hoạt động và cách thức triển khai.</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>The proposed solutions for the operation of the inter-provincial irrigation system in the Mekong Delta region, as discussed in the research paper by Dũng et al. (2021), involve the use of smart and flexible operation of the irrigation system. This is to enhance water productivity and protect the ecological environment. The solutions are based on the Internet of Things (IoT) technology. The paper also suggests that the only solution to meet the increasing demand for food in the context of limited land and water resources is to improve the efficiency of land and water use through solutions that enhance the efficiency of management and exploitation of irrigation works.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không đề cập đến 5 mô hình đã được triển khai thí điểm tại 20 hộ. Do đó, tôi không thể liệt kê và mô tả chi tiết về 5 mô hình này.</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and appears to be fully correct. It provides a detailed explanation of the proposed solutions for the operation of the inter-provincial irrigation system in the Mekong Delta region as discussed in the research paper by Dũng et al. (2021).</t>
+          <t>The generated answer is relevant to the user query and it is correct in stating that it cannot provide the requested information due to lack of specific details in the query. However, it could have been more helpful by asking for more information or suggesting where the user might find the information they are looking for.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>What are the challenges faced by the inter-provincial irrigation system in the Mekong Delta region, as discussed in the paper by Dũng et al. (2021)?</t>
+          <t>Theo bài báo, hãy mô tả những khó khăn mà hệ thống thủy lợi liên tỉnh tại vùng Đồng bằng sông Cửu Long đang gặp phải? Giải pháp nào được đề xuất để giải quyết những vấn đề này?</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>The context does not provide information on the challenges faced by the inter-provincial irrigation system in the Mekong Delta region as discussed in a paper by Dũng et al. (2021).</t>
+          <t>Hệ thống thủy lợi liên tỉnh tại vùng Đồng bằng sông Cửu Long đang gặp phải nhiều khó khăn. Một trong số đó là hiện tượng tranh chấp nước giữa các địa phương sử dụng chung hệ thống thủy lợi đang diễn ra ngày càng gay gắt. Thêm vào đó, sự phát triển của đô thị và khai thác quá tải nước ngầm đã làm giảm diện tích tưới tiêu. Đồng thời, hiện tượng xâm nhập mặn và khô hạn cũng đang tác động mạnh mẽ lên vùng này, đặc biệt là từ tháng 1 đến tháng 4 hàng năm. 
+Để giải quyết những vấn đề này, bài báo đề xuất việc nghiên cứu giải pháp để vận hành một cách thông minh, linh hoạt các công trình trong hệ thống thủy lợi nhằm nâng cao năng suất nước và bảo vệ môi trường sinh thái. Cụ thể, các giải pháp được đề xuất dựa trên nền tảng công nghệ Internet of Things (IoT). Ngoài ra, cần tăng hiệu quả sử dụng tài nguyên đất và nước thông qua các giải pháp nâng cao hiệu quả quản lý khai thác các công trình thuỷ lợi.</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2940,24 +2906,24 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>The generated answer does not provide any information relevant to the user's query about the challenges faced by the inter-provincial irrigation system in the Mekong Delta region.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the problems faced by the inter-provincial irrigation system in the Mekong Delta region. It also suggests solutions to these problems. However, without a reference answer, it's hard to confirm the absolute correctness of the information.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>According to the paper, how can the Internet of Things (IoT) technology be used to improve the operation of the inter-provincial irrigation systems in the Mekong Delta region?</t>
+          <t>Trình bày về tầm quan trọng của việc vận hành thông minh hệ thống thủy lợi liên tỉnh tại vùng Đồng bằng sông Cửu Long trong bối cảnh biến đổi khí hậu và xâm nhập mặn. Công nghệ nào được đề cập trong bài báo để hỗ trợ việc này?</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>The paper suggests that Internet of Things (IoT) technology can be used to intelligently operate inter-provincial irrigation systems in the Mekong Delta region. This would involve using IoT to manage the various water needs of different sectors such as agriculture, aquaculture, tourism, environment, and disaster prevention. The goal is to enhance water productivity and protect the ecological environment, especially in the face of increasing climate change and extreme salt intrusion. However, the paper does not provide specific details on how IoT technology would be implemented to achieve these goals.</t>
+          <t>Việc vận hành thông minh hệ thống thủy lợi liên tỉnh tại vùng Đồng bằng sông Cửu Long đóng vai trò quan trọng trong sản xuất nông nghiệp và dân sinh. Trong bối cảnh biến đổi khí hậu và xâm nhập mặn ngày càng bất lợi và khó lường, việc vận hành thông minh và linh hoạt các công trình trong hệ thống thủy lợi trở nên cần thiết hơn bao giờ hết để nâng cao năng suất nước và bảo vệ môi trường sinh thái. Công nghệ Internet of Things (IoT) được đề cập trong bài báo như một nền tảng hỗ trợ cho việc vận hành thông minh hệ thống thủy lợi.</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2972,21 +2938,22 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of how IoT technology can be used to improve the operation of inter-provincial irrigation systems in the Mekong Delta region. It loses half a point for not providing specific details on the implementation of IoT technology, as mentioned in the answer itself.</t>
+          <t>The generated answer is highly relevant to the user query and provides a comprehensive response. It correctly explains the importance of smart operation of inter-provincial irrigation systems in the Mekong Delta region in the context of climate change and saltwater intrusion. It also correctly identifies the Internet of Things (IoT) as the technology mentioned in the article to support this operation.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Based on the research directions mentioned in the document, can you explain how the application of technology in the management and operation of irrigation systems can help companies exploit water resources more efficiently and reduce operational costs?</t>
+          <t>Hãy liệt kê và giải thích 3 hướng nghiên cứu chính đã được sử dụng trong việc quản lý và khai thác công trình thủy lợi (CTTL) như được mô tả trong tài liệu.</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>The application of technology in the management and operation of irrigation systems can help companies exploit water resources more efficiently and reduce operational costs by enabling intelligent and flexible operation of the systems. This can be achieved by integrating various technologies in a scientific and synchronized manner. The focus should be on solving the problem of optimal water use, monitoring and controlling the facilities and equipment (such as pumping stations, sluices) remotely, and overseeing the entire cultivation area (from incoming to outgoing water) to support remote operation decision-making. 
-Research results have already addressed many issues related to technology and equipment, such as hydraulic simulation and remote control and monitoring devices. The use of Internet of Things (IoT) technology can also be a foundation for operating these inter-provincial irrigation systems intelligently. 
-By enhancing the efficiency of resource use through these technological solutions, companies can meet the increasing demand for food in a context where land and water resources are limited. This not only improves water productivity but also helps protect the ecological environment.</t>
+          <t>Ba hướng nghiên cứu chính đã được sử dụng trong việc quản lý và khai thác công trình thủy lợi (CTTL) như sau:
+1. Đánh giá hiện trạng thủy lợi: Đây là việc nghiên cứu và đánh giá tình hình hiện tại của các công trình thủy lợi, bao gồm hệ thống các kênh, đê bao và cống. Mục tiêu là xác định mức độ hiệu quả của các công trình hiện tại và xác định nhu cầu cho việc nâng cấp hoặc thay thế.
+2. Tính toán vận hành cống: Đây là việc nghiên cứu và tính toán cách vận hành cống trong các tháng mùa khô, dựa trên điều kiện xâm nhập mặn. Mục tiêu là tối ưu hóa việc sử dụng nước và ngăn chặn xâm nhập mặn.
+3. Nghiên cứu ứng phó với biến đổi khí hậu: Đây là việc nghiên cứu về cách quản lý tài nguyên nước để ứng phó với biến đổi khí hậu, bao gồm thay đổi đặc điểm lũ lụt và xâm nhập mặn. Mục tiêu là đảm bảo sự bền vững của các công trình thủy lợi trong bối cảnh biến đổi khí hậu.</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3001,19 +2968,20 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how technology can be applied in the management and operation of irrigation systems to exploit water resources more efficiently and reduce operational costs. It also provides examples of specific technologies and their benefits.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed and correct response. It lists and explains three main research directions used in the management and exploitation of irrigation works as requested by the user.</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Analyze the data on salinity from 2007 to 2017 at Son Doc and Huong My stations as mentioned in the document. Discuss the trend of salinity increase and its implications on the water management and irrigation systems.</t>
+          <t>Dựa trên số liệu mặn từ 2007 đến 2017 tại trạm Sơn Đốc và Hương Mỹ, hãy phân tích xu hướng biến đổi của mặn và những hậu quả mà nó gây ra cho hệ thống thủy lợi và canh tác.</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>The context does not provide specific data on salinity from 2007 to 2017 at Son Doc and Huong My stations. Therefore, it's not possible to analyze the trend of salinity increase and its implications on the water management and irrigation systems based on the provided information.</t>
+          <t>Từ 2007 đến 2017, mặn tại trạm Sơn Đốc và Hương Mỹ đã tăng với tốc độ 0.2-0.5 PSU/năm. Mặn năm 2015-2016 được đánh giá là trầm trọng nhất trong 90 năm qua, nhưng mặn năm 2019-2020 thậm chí còn nghiêm trọng hơn. Mặn năm 2019-2020 ở tất cả các nhánh sông, ngoại trừ sông Vàm Cỏ Đông, đều tăng so với năm 2015-2016, cao nhất là tăng thêm 9 km trên sông Vàm Cỏ Tây. Xu hướng mặn không chỉ tăng về nồng độ mà còn rút ngắn về thời gian xuất hiện mặn cực hạn.
+Tình trạng mặn tăng này đã gây ra những hậu quả nghiêm trọng cho hệ thống thủy lợi và canh tác. Cụ thể, việc phối hợp điều tiết phân phối nước chưa giải quyết được yêu cầu thực tế, có sự mâu thuẫn nhu cầu sử dụng nước đặc biệt vào mùa khô ở các địa phương đầu nguồn và cuối nguồn. Một số kênh trục chính đã bị nhiễm XNM, nhiễm phèn thường xuyên, trong khi đó một số khu vực không có nguồn tiếp ngọt làm cho nhiều diện tích rau màu bị ảnh hưởng nghiêm trọng.</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3023,51 +2991,52 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and correctly states that it cannot provide the requested analysis due to lack of specific data. However, it does not attempt to provide any general insights or potential implications of salinity increase on water management and irrigation systems, which could have made the response more valuable.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the salinity changes at the Son Doc and Huong My stations from 2007 to 2017. It also discusses the consequences of these changes on the irrigation system and farming. However, it includes information about the years 2019-2020, which is beyond the requested time frame, hence the slight deduction in score.</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Explain the challenges faced in the operation of hydraulic works for multiple objectives, industries, and economic subjects as mentioned in the document "researched_paper_cleanup.txt". How does the current operation process fail to address these challenges?</t>
+          <t>Theo nội dung trong tài liệu, vấn đề gì khiến công tác thủy lợi ở ĐBSCL đang ở giai đoạn "chưa thông minh" và giải pháp đề xuất để khắc phục vấn đề này là gì?</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Hydraulic works need to operate to serve multiple objectives, various industries, and different economic subjects. The information used in these operations must be accurate, sufficient, precise, and timely. The current operation processes of these hydraulic works partially meet the diverse water needs of different sectors such as agriculture, aquaculture, and the environment, especially in conditions of freshwater scarcity. However, these operation processes are primarily built based on determining a certain frequency of climatic factors, water sources, or salinity levels. This approach fails to adequately and accurately address the impacts of climate change in a timely manner. Therefore, the current stage of hydraulic works is described as "not smart". The proposed solution is to integrate various technologies in a synchronized, scientific manner, focusing on solving the problem of optimal water use, monitoring and controlling the works and equipment remotely, and monitoring the entire cultivation area to support remote operation decision-making.</t>
+          <t>Công tác thủy lợi ở ĐBSCL đang ở giai đoạn "chưa thông minh" do một số vấn đề như tranh chấp nước giữa các địa phương sử dụng chung hệ thống thủy lợi, biến đổi khí hậu, xâm nhập mặn, mất diện tích tưới tiêu do úng, nhiễm mặn, khai thác quá tải nước ngầm và sự phát triển của đô thị. Ngoài ra, quy trình vận hành công trình thủy lợi hiện nay chủ yếu được xây dựng dựa trên cơ sở xác định một tần suất nhất định của các yếu tố khí hậu, nguồn nước, hay độ mặn nên không xử lý được đúng, đủ, chính xác và kịp thời trước sự tác động của biến đổi khí hậu.
+Giải pháp đề xuất để khắc phục vấn đề này là vận hành một cách thông minh, linh hoạt các công trình trong hệ thống thủy lợi nhằm nâng cao năng suất nước và bảo vệ môi trường sinh thái. Điều này có thể được thực hiện thông qua việc kết hợp nhiều loại công nghệ một cách đồng bộ, khoa học, tập trung vào giải quyết bài toán sử dụng nước tối ưu, giám sát, điều khiển các công trình, thiết bị từ xa, giám sát toàn bộ khu vực canh tác để hỗ trợ ra quyết định vận hành công trình từ xa.</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>YES</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of the challenges faced in the operation of hydraulic works for multiple objectives, industries, and economic subjects. It also explains how the current operation process fails to address these challenges. The answer could be slightly more specific in terms of the document "researched_paper_cleanup.txt", but overall it is a very good response.</t>
+          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of the issues facing irrigation in the Mekong Delta, as well as proposed solutions to these problems. The answer is detailed, accurate, and well-structured, making it easy for the user to understand.</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Based on the research results mentioned in the document, what technological and equipment-related issues have been resolved in the field of hydraulic simulation and remote control and monitoring?</t>
+          <t>Các kết quả nghiên cứu đã giải quyết được những vấn đề gì về công nghệ và thiết bị trong lĩnh vực thủy lợi?</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>The research results have addressed several technological and equipment-related issues such as hydraulic simulation, control equipment, and remote monitoring.</t>
+          <t>Các kết quả nghiên cứu đã giải quyết được nhiều vấn đề về công nghệ và thiết bị trong lĩnh vực thủy lợi, bao gồm mô phỏng thủy lực và thiết bị điều khiển, giám sát từ xa.</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3082,22 +3051,25 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query, but it does not provide specific details about what technological and equipment-related issues have been resolved in the field of hydraulic simulation and remote control and monitoring.</t>
+          <t>The generated answer is relevant and correct. It addresses the user's query about what research has solved in terms of technology and equipment in the field of irrigation. However, it could provide more specific examples or details to fully satisfy the query.</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>What are the main challenges identified in the research regarding the current management of irrigation systems? Provide at least three examples from the text.</t>
+          <t>Theo nội dung của tài liệu nghiên cứu, hãy liệt kê những hạn chế chính của các kết quả nghiên cứu đã thực hiện trong quản lý điều hành hệ thống tưới hiện nay?</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>The main challenges identified in the research regarding the current management of irrigation systems include the following: 
-1. The water resources planning in the Mekong Delta is largely "top-down", with villagers and farmers playing a minor role in water planning and natural prevention projection processes. This means that those most affected by water management decisions often have little say in them.
-2. The water control infrastructure systems, despite receiving about 10 percent of the state budget and labor contributions from the people, suffer from many shortcomings in terms of their structure and management. 
-3. There are significant water quantity and quality problems that limit agricultural production. These include salinity intrusion, floods, acid sulfate soils, polluted water, and fresh water shortages. These issues are exacerbated by the fact that the Mekong Delta receives the total volume of floodwaters from upstream, leading to frequent and potentially damaging flooding.</t>
+          <t>Các hạn chế chính của các kết quả nghiên cứu đã thực hiện trong quản lý điều hành hệ thống tưới hiện nay bao gồm:
+1. Các phần mềm chỉ giải quyết được các vấn đề riêng lẻ, chưa tích hợp để giải quyết tổng hợp các vấn đề trong công tác quản lý điều hành hệ thống tưới.
+2. Các giải pháp quan trắc chỉ có giá trị thực tiễn khi lắp đặt đầy đủ hệ thống trạm đo tại trải khắp hệ thống.
+3. Các giải pháp mô hình được xây dựng đơn lẻ, theo kịch bản cho trước chỉ phù hợp trong việc lập quy hoạch, kế hoạch trong dài hạn, khó áp dụng trong vận hành công trình.
+4. Giải pháp vận hành, giám sát từ xa có thể áp dụng cho từng công trình cụ thể, nhưng khó áp dụng cho vận hành cả hệ thống và phân phối nước cho nhiều đối tượng dùng nước.
+5. Chưa kết hợp được bài toán phân phối nước tối ưu với các công nghệ mô phỏng thủy lực, điều khiển từ xa.
+6. Các giải pháp chỉ quan tâm đến đối tượng sử dụng là các cơ quan, tổ chức QLKT CTTL, mà chưa tạo được kết nối với toàn bộ các cá nhân, tổ chức liên quan đến hệ thống thủy lợi từ đầu mối tới mặt ruộng, như tổ chức thủy lợi cơ sở, nông dân.</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3112,19 +3084,19 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides three clear examples of challenges in the management of irrigation systems. It is detailed and well-structured. However, without a reference answer, it's hard to confirm the absolute correctness of the information provided.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed list of the main limitations of the research results in the current irrigation system management. It is comprehensive and appears to be correct, even without a reference answer for comparison.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Based on the research, what are the three main models proposed for the construction of the system, and how are they interconnected?</t>
+          <t>Giải pháp đề xuất trong nghiên cứu này sẽ giải quyết được những vấn đề gì trong công tác quản lý, điều hành hệ thống tưới, đặc biệt là các hệ thống thủy lợi liên tỉnh?</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>The system proposed in the research is constructed using three main models. These include a hydraulic model, a management model for irrigation infrastructure through an online GIS system (WebGIS), and a SCADA model. These models are interconnected through the Internet of Things (IoT).</t>
+          <t>The proposed solution in this research will address overall issues in the management and operation of irrigation systems, especially inter-provincial irrigation systems. It will modernize the management and operation of irrigation works, which is a current concern. This solution is a potential one with high practical applicability. It will serve as a scientific basis for the study and application of the operation of inter-provincial irrigation systems in the Mekong Delta region.</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3139,19 +3111,19 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and appears to be correct, providing detailed information about the three main models used for the system construction and explaining how they are interconnected. However, without a reference answer, it's not possible to confirm the absolute correctness of the specific models mentioned.</t>
+          <t>The generated answer is highly relevant to the user query and provides a detailed explanation of how the proposed solution in the research will address issues in the management and operation of irrigation systems, especially inter-provincial ones. However, it does not specify the exact problems that will be solved, which would have made the answer more precise.</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Based on the text, what are the challenges faced when applying a system on a provincial scale and how does the text suggest these challenges can be addressed?</t>
+          <t>Trong nghiên cứu này, tác giả đã đề cập đến vấn đề gì khi áp dụng cho một hệ thống có quy mô liên tỉnh và giải pháp nào được đề xuất để giải quyết vấn đề này?</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>The text does not provide specific information about the challenges faced when applying a system on a provincial scale, nor does it suggest how these challenges can be addressed.</t>
+          <t>Khi áp dụng cho một hệ thống có quy mô liên tỉnh, tác giả đã đề cập đến vấn đề dữ liệu lớn, nghĩa là rất nhiều số liệu và ở các định dạng khác nhau sẽ được truyền tải, lưu trữ và xử lý ở trung tâm, tạo ra một khối lượng dữ liệu vô cùng lớn. Để giải quyết vấn đề này, tác giả đề xuất kết hợp ứng dụng công nghệ Bigdata để hỗ trợ xử lý dữ liệu.</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3166,19 +3138,19 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and seems to be correct based on the information provided. However, without the text or a reference answer, it's hard to confirm its full accuracy.</t>
+          <t>The generated answer is relevant to the user query and seems to be correct. It addresses the problem mentioned in the query (big data) and provides a solution (using Bigdata technology). However, without a reference answer, it's hard to confirm the absolute correctness.</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>In the context of the document, what role does the integration of Artificial Intelligence (AI) play in the automation of operations and what would be the human role after its implementation?</t>
+          <t>Theo tác giả, công nghệ nào cần được kết hợp để hoàn toàn tự động hóa công tác vận hành một hệ thống thông tin liên lạc và vai trò của con người trong hệ thống này sẽ là gì?</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>The integration of Artificial Intelligence (AI) plays a significant role in achieving full automation of operations. It is proposed to be used to intelligently and accurately solve decision-making problems in operations. After its implementation, the human role would be limited to supervision, asset protection, maintenance, and handling of any potential issues.</t>
+          <t>Để hoàn toàn tự động hóa công tác vận hành một hệ thống thông tin liên lạc, tác giả đề xuất cần kết hợp công nghệ trí tuệ nhân tạo (AI). Trong hệ thống này, con người sẽ chỉ đóng vai trò giám sát, bảo vệ tài sản, sửa chữa bảo dưỡng và xử lý sự cố (nếu có).</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3193,46 +3165,46 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a comprehensive explanation of the role of AI in automation and the human role post-implementation. However, it could have included more specific examples or details to fully answer the question.</t>
+          <t>The generated answer is relevant to the user query and appears to be correct, providing a specific technology (AI) and outlining the human role in the system. However, without a reference answer, it's not possible to confirm the absolute correctness.</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Based on the data provided in the 'testing.json' file, what was the highest recorded salinity at any location in the Province of Ben Tre on 8/1/2023?</t>
+          <t>Hãy liệt kê các thông số đo lường khí hậu được ghi nhận tại địa điểm "Sông Cổ Chiên - Châu Thành (Cầu Rạch Gốc)" vào ngày "8/1/2023" theo dữ liệu trong tệp testing.json.</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>The highest recorded salinity at any location in the Province of Ben Tre on 8/1/2023 was 13.00.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không chứa bất kỳ dữ liệu nào về các thông số đo lường khí hậu tại địa điểm "Sông Cổ Chiên - Châu Thành (Cầu Rạch Gốc)" vào ngày "8/1/2023" theo dữ liệu trong tệp testing.json.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and appears to be correct, as it provides a specific value for the highest recorded salinity in the Province of Ben Tre on the specified date. Without a reference answer, it's impossible to verify the exact correctness, but the response is in line with the type of answer expected from the question.</t>
+          <t>The generated answer is relevant and correct. It directly addresses the user's query and states that there is no available data for the specified location and date in the testing.json file.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>According to the meteorological readings from the 'testing.json' file, which location in the Province of Ben Tre had a pH level of 8.5 on 8/1/2023?</t>
+          <t>Trong tệp testing.json, địa điểm nào có nồng độ muối (Salinity) cao nhất vào ngày "8/1/2023" và thông số đó là bao nhiêu?</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>The location in the Province of Ben Tre that had a pH level of 8.5 on 8/1/2023 was HTX nghêu Thành Đạt - Hiệp Thạnh - TX. Duyên Hải.</t>
+          <t>Xin lỗi, nhưng thông tin trong ngữ cảnh không cung cấp dữ liệu về nồng độ muối (Salinity) ở bất kỳ địa điểm nào vào ngày "8/1/2023".</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3247,78 +3219,78 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and appears to be correct, providing a specific location in the Province of Ben Tre that had the specified pH level on the given date. Without a reference answer, it's impossible to verify the accuracy, but the response is in line with the question's requirements.</t>
+          <t>The generated answer is relevant to the user query and seems correct, but without a reference answer or the actual data from the 'testing.json' file, it's impossible to confirm its absolute correctness. The bot appropriately communicates that it cannot provide the requested information due to lack of data.</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Based on the data provided in the testing.json file, can you analyze and explain the correlation between the salinity and temperature at different locations in Ben Tre province on the date 8/1/2023?</t>
+          <t>Hãy liệt kê các thông số môi trường được ghi nhận tại địa điểm "Sông Long Toàn - TX. Duyên Hải (Cầu Long Toàn)" vào ngày "8/1/2023".</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>On August 1, 2023, in the Ben Tre province, the salinity and temperature readings varied across different locations. For instance, at "Sông Cổ Chiên - Châu Thành (Cầu Rạch Gốc)", "Bến phà Long Hưng - Hòa Minh - Châu Thành", and "Sông Vinh Kim - Cầu Ngang", the salinity was 0.00 and the temperatures were 28.00, 29.00, and 28.00 respectively. At "Sông Hiệp Mỹ - Cầu Ngang (gần Cầu Hiệp Mỹ)", the salinity increased to 1.00 with a temperature of 27.00. The location "Cống Thâu Râu -Mỹ Long Nam - Cầu Ngang" had a salinity of 4.00 and a temperature of 29.00. The highest salinity of 9.00 was recorded at "HTX nghêu Thành Đạt - Hiệp Thạnh - TX. Duyên Hải" with a temperature of 29.00. At "Cầu Sông Giăng - Hiệp Thạnh - TX. Duyên Hải", the salinity was 5.00 and the temperature was 29.00. Lastly, "Sông Long Toàn - TX. Duyên Hải (Cầu Long Toàn)" had the highest salinity of 10.00 with a pH of 7.50. However, the temperature for this location is not provided. From this data, it's not clear if there's a direct correlation between salinity and temperature as they seem to vary independently across different locations.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không chứa các thông số môi trường tại địa điểm "Sông Long Toàn - TX. Duyên Hải (Cầu Long Toàn)" vào ngày "8/1/2023".</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed analysis of the salinity and temperature at different locations in Ben Tre province on the specified date. It also correctly concludes that it's not clear if there's a direct correlation between salinity and temperature. However, it mentions a pH value at the end which was not asked for in the query, hence the slight deduction.</t>
+          <t>The generated answer is relevant to the user query and it seems correct, but without a reference answer, it's hard to confirm its absolute correctness. The bot appropriately communicates that it doesn't have the specific environmental data for the requested location and date.</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>From the information in the testing.json file, identify the location in Ben Tre province that had the highest alkaline level on 8/4/2023 and discuss the potential environmental factors that could have contributed to this high level.</t>
+          <t>Theo dữ liệu trong tệp, địa điểm nào có nồng độ muối (Salinity) cao nhất vào ngày "8/1/2023"?</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>On 8/4/2023, the locations in Ben Tre province with the highest alkaline level were "Sông Vinh Kim - Cầu Ngang" and "Sông Hiệp Mỹ - Cầu Ngang (gần Cầu Hiệp Mỹ)", both with an alkaline level of 90.00. Environmental factors that could contribute to high alkaline levels include the presence of certain minerals in the soil or water, industrial waste discharge, or agricultural runoff, which can contain fertilizers high in alkaline substances. However, the specific contributing factors for these locations are not provided in the data.</t>
+          <t>Dữ liệu trong tệp không cung cấp thông tin cụ thể về nồng độ muối (Salinity) tại bất kỳ địa điểm nào vào ngày "8/1/2023".</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>The generated answer is highly relevant to the user query and provides a detailed response. It correctly identifies the locations with the highest alkaline level on the specified date and discusses potential environmental factors that could contribute to high alkaline levels. However, it does not provide specific contributing factors for these locations, which is why it doesn't get a perfect score.</t>
+          <t>The generated answer is relevant and correct. It accurately responds to the user's query by stating that the file does not provide specific information about the salinity at any location on the date "8/1/2023".</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Based on the data provided in the 'testing.json' file, what were the recorded pH and temperature values at the location "Sông Hiệp Mỹ - Cầu Ngang (gần Cầu Hiệp Mỹ)" on the date "8/4/2023"?</t>
+          <t>Hãy liệt kê các thông tin về môi trường nước tại "Sông Vinh Kim - Cầu Ngang" vào ngày "8/4/2023" theo dữ liệu trong tệp.</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>The recorded pH and temperature values at the location "Sông Hiệp Mỹ - Cầu Ngang (gần Cầu Hiệp Mỹ)" on the date "8/4/2023" were 8.00 and 27.00 respectively.</t>
+          <t>Xin lỗi, nhưng thông tin trong ngữ cảnh không cung cấp chi tiết về môi trường nước tại "Sông Vinh Kim - Cầu Ngang" vào ngày "8/4/2023".</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3328,19 +3300,19 @@
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and appears to be fully correct, providing specific pH and temperature values for the specified location and date. Without a reference answer, it's impossible to verify the accuracy of these values, but the answer is structured and detailed in a way that suggests correctness.</t>
+          <t>The generated answer is relevant to the user query and it seems correct, but without a reference answer or additional context, it's hard to confirm its absolute correctness.</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Analyze the 'testing.json' file and compare the salinity levels recorded at "Sông Vinh Kim - Cầu Ngang" and "Cầu Sông Giăng - Hiệp Thạnh - TX. Duyên Hải" on the date "8/4/2023". Which location had a higher salinity level?</t>
+          <t>Theo dữ liệu trong tệp, địa điểm nào có nhiệt độ cao nhất vào ngày "8/4/2023" và nhiệt độ đó là bao nhiêu?</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>On the date "8/4/2023", the location "Sông Vinh Kim - Cầu Ngang" had a salinity level of "0.00", while the location "Cầu Sông Giăng - Hiệp Thạnh - TX. Duyên Hải" had a salinity level of "5.00". Therefore, "Cầu Sông Giăng - Hiệp Thạnh - TX. Duyên Hải" had a higher salinity level.</t>
+          <t>Dữ liệu trong tệp không cung cấp thông tin cụ thể về nhiệt độ cao nhất vào ngày "8/4/2023" tại bất kỳ địa điểm nào.</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3350,66 +3322,66 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and provides a clear and correct comparison of the salinity levels at the two specified locations on the given date. It also correctly identifies which location had a higher salinity level.</t>
+          <t>The generated answer is relevant to the user query and seems correct, but without a reference answer or the data file, it's impossible to confirm its accuracy.</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Based on the data provided in the testing.json file, can you identify the location with the highest salinity on the date 8/4/2023? Please provide the salinity value and the corresponding pH level at this location.</t>
+          <t>Hãy liệt kê các thông số môi trường được ghi nhận tại địa điểm "HTX nghêu Thành Đạt - Hiệp Thạnh - TX. Duyên Hải" vào ngày "8/4/2023".</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>The location with the highest salinity on the date 8/4/2023 is "Sông Long Toàn - TX. Duyên Hải (Cầu Long Toàn)" with a salinity value of 6.00. The corresponding pH level at this location is 7.50.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không chứa bất kỳ thông tin nào về các thông số môi trường được ghi nhận tại địa điểm "HTX nghêu Thành Đạt - Hiệp Thạnh - TX. Duyên Hải" vào ngày "8/4/2023".</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>The generated answer is relevant to the user query and provides specific details about the location, salinity value, and pH level, which suggests that it is correct. However, without the actual data or a reference answer, it's impossible to verify the accuracy of these details.</t>
+          <t>The generated answer is relevant to the user query and it is correct in stating that it doesn't have the specific information requested. However, it could have been more helpful by suggesting ways to find the requested information.</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Analyze the data in the testing.json file and determine the average temperature recorded across all locations on 8/4/2023. How does this temperature correlate with the NH4/NH3 values observed?</t>
+          <t>So sánh nồng độ muối (Salinity) và nhiệt độ (Temperature) tại các địa điểm "Cống La Bang - Đôn Châu - Duyên Hải" và "Bến đò Phước Thiện - Đông Hải - Duyên Hải" vào ngày "8/4/2023".</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>The average temperature recorded across all locations on 8/4/2023 is 28.67 degrees. The NH4/NH3 values observed on the same date range from 3.00 to 4.00. However, the context does not provide enough information to determine a correlation between the temperature and NH4/NH3 values.</t>
+          <t>Xin lỗi, nhưng thông tin được cung cấp không chứa dữ liệu về nồng độ muối (Salinity) và nhiệt độ (Temperature) tại các địa điểm "Cống La Bang - Đôn Châu - Duyên Hải" và "Bến đò Phước Thiện - Đông Hải - Duyên Hải" vào ngày "8/4/2023".</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>The generated answer is relevant and seems to be correct. It provides the average temperature and the range of NH4/NH3 values for the specified date. It also correctly states that there isn't enough information to determine a correlation between the two. However, without the actual data or a reference answer, it's impossible to confirm the exact correctness of the provided values.</t>
+          <t>The generated answer is relevant to the user query, but it does not provide the specific information requested. However, it correctly states that the requested data is not available, which is a valid response in the absence of the specific data.</t>
         </is>
       </c>
     </row>

</xml_diff>